<commit_message>
change ie initialize from show fullscreen to show maximum.
</commit_message>
<xml_diff>
--- a/PaperTester.xlsx
+++ b/PaperTester.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="126">
   <si>
     <t>No.</t>
   </si>
@@ -126,22 +126,10 @@
     <t>InternetExplorerを閉じる。</t>
   </si>
   <si>
-    <t>最大表示にする</t>
-  </si>
-  <si>
     <t>FullScreen</t>
   </si>
   <si>
-    <t>InternetExplorerを最大表示にする。</t>
-  </si>
-  <si>
-    <t>標準表示にする</t>
-  </si>
-  <si>
     <t>NormalScreen</t>
-  </si>
-  <si>
-    <t>InternetExplorerを標準表示にする。</t>
   </si>
   <si>
     <t>Sleep(%0)</t>
@@ -546,6 +534,89 @@
     </rPh>
     <rPh sb="17" eb="19">
       <t>ブブン</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>全画面表示を行う</t>
+    <rPh sb="0" eb="3">
+      <t>ゼンガメン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>オコナ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>全画面表示を止める</t>
+    <rPh sb="0" eb="3">
+      <t>ゼンガメン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ヤ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>画面を最大化する</t>
+  </si>
+  <si>
+    <t>画面を最小化する</t>
+    <rPh sb="3" eb="5">
+      <t>サイショウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>画面を標準表示にする</t>
+  </si>
+  <si>
+    <t>MaximumWindow</t>
+  </si>
+  <si>
+    <t>MinimumWindow</t>
+  </si>
+  <si>
+    <t>NormalWindow</t>
+  </si>
+  <si>
+    <t>InternetExplorerをフルスクリーン表示にする。</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>InternetExplorerのフルスクリーン表示を止める。</t>
+    <rPh sb="27" eb="28">
+      <t>ヤ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>InternetExplorerを最大化する。</t>
+    <rPh sb="17" eb="20">
+      <t>サイダイカ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>InternetExplorerを最小化する。</t>
+    <rPh sb="17" eb="19">
+      <t>サイショウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>InternetExplorerを標準表示にする。</t>
+    <rPh sb="17" eb="19">
+      <t>ヒョウジュン</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ヒョウジ</t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -1663,7 +1734,7 @@
         <v>3</v>
       </c>
       <c r="O1" s="54" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="P1" s="7" t="s">
         <v>4</v>
@@ -1737,11 +1808,11 @@
       </c>
       <c r="O2" s="55"/>
       <c r="P2" s="16" t="str">
-        <f>IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$21,2,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$24,2,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>Open</v>
       </c>
       <c r="Q2" s="16" t="str">
-        <f>IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$21,3,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$24,3,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>InternetExplorerを開く。</v>
       </c>
       <c r="R2" s="17" t="s">
@@ -1807,11 +1878,11 @@
         <v>22</v>
       </c>
       <c r="P3" s="28" t="str">
-        <f>IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$A$2:$C$21,2,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$A$2:$C$24,2,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>Navigate "http://bl.ocks.org/nezuQ/raw/9719897/"</v>
       </c>
       <c r="Q3" s="28" t="str">
-        <f>IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$A$2:$C$21,3,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$A$2:$C$24,3,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>URL「http://bl.ocks.org/nezuQ/raw/9719897/」で遷移する。</v>
       </c>
       <c r="R3" s="29"/>
@@ -1857,18 +1928,18 @@
       <c r="L4" s="26"/>
       <c r="M4" s="26"/>
       <c r="N4" s="27" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="O4" s="57" t="str">
         <f ca="1">A4</f>
         <v>1</v>
       </c>
       <c r="P4" s="28" t="str">
-        <f ca="1">IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$21,2,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f ca="1">IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$24,2,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>FullScreenShot4VisibleArea "1"</v>
       </c>
       <c r="Q4" s="28" t="str">
-        <f ca="1">IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$21,3,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f ca="1">IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$24,3,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>スクリーンショットを撮る。（画面全体, 表示箇所のみ, コメント："1"）</v>
       </c>
       <c r="R4" s="29"/>
@@ -1899,17 +1970,17 @@
       <c r="L5" s="26"/>
       <c r="M5" s="26"/>
       <c r="N5" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="O5" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="O5" s="57" t="s">
-        <v>98</v>
-      </c>
       <c r="P5" s="28" t="str">
-        <f>IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$A$2:$C$21,2,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$A$2:$C$24,2,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>ExecuteSQL "SELECT * FROM [Sheet1$] "</v>
       </c>
       <c r="Q5" s="28" t="str">
-        <f>IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$A$2:$C$21,3,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$A$2:$C$24,3,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>SQL文を発行する。"SELECT * FROM [Sheet1$] "</v>
       </c>
       <c r="R5" s="29"/>
@@ -1959,11 +2030,11 @@
       <c r="N6" s="27"/>
       <c r="O6" s="57"/>
       <c r="P6" s="28" t="str">
-        <f>IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$21,2,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$24,2,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q6" s="28" t="str">
-        <f>IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$21,3,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$24,3,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R6" s="33"/>
@@ -2010,20 +2081,20 @@
       <c r="K7" s="25"/>
       <c r="L7" s="26"/>
       <c r="M7" s="26" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="N7" s="27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="O7" s="58" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="P7" s="28" t="str">
-        <f>IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$21,2,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$24,2,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>ValueInput "id=ddlEndpoint ← '1' %|% id=ddlSearchType ← '1' %|% id=txtQuery ← 'ラブライブ！' %|% id=txtPHPSessID ← ''"</v>
       </c>
       <c r="Q7" s="28" t="str">
-        <f>IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$21,3,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$24,3,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>項目「引数の前部分」に値「引数の後部分」を入力する。"id=ddlEndpoint ← '1' %|% id=ddlSearchType ← '1' %|% id=txtQuery ← 'ラブライブ！' %|% id=txtPHPSessID ← ''"</v>
       </c>
       <c r="R7" s="29" t="s">
@@ -2083,17 +2154,17 @@
       <c r="L8" s="26"/>
       <c r="M8" s="26"/>
       <c r="N8" s="27" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="O8" s="63" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="P8" s="28" t="str">
-        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$21,2,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$24,2,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>FullScreenShot "2-1"</v>
       </c>
       <c r="Q8" s="28" t="str">
-        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$21,3,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$24,3,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>スクリーンショットを撮る。（画面全体, コメント："2-1"）</v>
       </c>
       <c r="R8" s="33"/>
@@ -2142,14 +2213,14 @@
         <v>26</v>
       </c>
       <c r="O9" s="57" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="P9" s="28" t="str">
-        <f>IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$21,2,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$24,2,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>Click "tag=input#4"</v>
       </c>
       <c r="Q9" s="28" t="str">
-        <f>IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$21,3,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$24,3,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>項目「tag=input#4」をクリックする。</v>
       </c>
       <c r="R9" s="33"/>
@@ -2199,11 +2270,11 @@
       </c>
       <c r="O10" s="57"/>
       <c r="P10" s="28" t="str">
-        <f>IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$21,2,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$24,2,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>ActivateChildWindow</v>
       </c>
       <c r="Q10" s="28" t="str">
-        <f>IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$21,3,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$24,3,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>子画面のウィンドウをアクティブにする。</v>
       </c>
       <c r="R10" s="33"/>
@@ -2249,15 +2320,15 @@
       <c r="L11" s="26"/>
       <c r="M11" s="26"/>
       <c r="N11" s="27" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="O11" s="57"/>
       <c r="P11" s="28" t="str">
-        <f>IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$21,2,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$24,2,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>FullScreenShot ""</v>
       </c>
       <c r="Q11" s="28" t="str">
-        <f>IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$21,3,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$24,3,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>スクリーンショットを撮る。（画面全体, コメント：""）</v>
       </c>
       <c r="R11" s="33"/>
@@ -2303,17 +2374,17 @@
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
       <c r="N12" s="27" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="O12" s="59" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="P12" s="28" t="str">
-        <f>IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$21,2,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$24,2,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>ExecuteSQL "SELECT * FROM [Sheet2$] "</v>
       </c>
       <c r="Q12" s="28" t="str">
-        <f>IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$21,3,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$24,3,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>SQL文を発行する。"SELECT * FROM [Sheet2$] "</v>
       </c>
       <c r="R12" s="33"/>
@@ -2363,11 +2434,11 @@
       </c>
       <c r="O13" s="57"/>
       <c r="P13" s="28" t="str">
-        <f>IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$21,2,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$24,2,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>Close</v>
       </c>
       <c r="Q13" s="28" t="str">
-        <f>IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$21,3,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$24,3,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>InternetExplorerを閉じる。</v>
       </c>
       <c r="R13" s="33"/>
@@ -2407,27 +2478,27 @@
       </c>
       <c r="G14" s="24"/>
       <c r="H14" s="25" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I14" s="25"/>
       <c r="J14" s="25"/>
       <c r="K14" s="25"/>
       <c r="L14" s="26"/>
       <c r="M14" s="26" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="N14" s="27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="O14" s="58" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="P14" s="28" t="str">
-        <f>IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$21,2,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$24,2,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>ValueInput "id=ddlEndpoint ← '0' %|% id=ddlSearchType ← '0' %|% id=txtQuery ← '艦隊これくしょん' %|% id=txtPHPSessID ← ''"</v>
       </c>
       <c r="Q14" s="28" t="str">
-        <f>IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$21,3,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$24,3,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>項目「引数の前部分」に値「引数の後部分」を入力する。"id=ddlEndpoint ← '0' %|% id=ddlSearchType ← '0' %|% id=txtQuery ← '艦隊これくしょん' %|% id=txtPHPSessID ← ''"</v>
       </c>
       <c r="R14" s="29" t="s">
@@ -2487,17 +2558,17 @@
       <c r="L15" s="26"/>
       <c r="M15" s="26"/>
       <c r="N15" s="27" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="O15" s="63" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="P15" s="28" t="str">
-        <f>IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$21,2,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$24,2,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>FullScreenShot "2-2"</v>
       </c>
       <c r="Q15" s="28" t="str">
-        <f>IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$21,3,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$24,3,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>スクリーンショットを撮る。（画面全体, コメント："2-2"）</v>
       </c>
       <c r="R15" s="33"/>
@@ -2546,14 +2617,14 @@
         <v>26</v>
       </c>
       <c r="O16" s="57" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="P16" s="28" t="str">
-        <f>IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$21,2,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$24,2,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>Click "tag=input#4"</v>
       </c>
       <c r="Q16" s="28" t="str">
-        <f>IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$21,3,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$24,3,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>項目「tag=input#4」をクリックする。</v>
       </c>
       <c r="R16" s="33"/>
@@ -2603,11 +2674,11 @@
       </c>
       <c r="O17" s="57"/>
       <c r="P17" s="28" t="str">
-        <f>IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$21,2,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$24,2,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>ActivateChildWindow</v>
       </c>
       <c r="Q17" s="28" t="str">
-        <f>IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$21,3,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$24,3,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>子画面のウィンドウをアクティブにする。</v>
       </c>
       <c r="R17" s="33"/>
@@ -2653,15 +2724,15 @@
       <c r="L18" s="26"/>
       <c r="M18" s="26"/>
       <c r="N18" s="27" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="O18" s="57"/>
       <c r="P18" s="28" t="str">
-        <f>IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$21,2,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$24,2,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>FullScreenShot ""</v>
       </c>
       <c r="Q18" s="28" t="str">
-        <f>IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$21,3,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$24,3,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>スクリーンショットを撮る。（画面全体, コメント：""）</v>
       </c>
       <c r="R18" s="33"/>
@@ -2707,17 +2778,17 @@
       <c r="L19" s="26"/>
       <c r="M19" s="26"/>
       <c r="N19" s="27" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="O19" s="59" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="P19" s="28" t="str">
-        <f>IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$21,2,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$24,2,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>ExecuteSQL "SELECT * FROM [Sheet2$] "</v>
       </c>
       <c r="Q19" s="28" t="str">
-        <f>IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$21,3,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$24,3,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>SQL文を発行する。"SELECT * FROM [Sheet2$] "</v>
       </c>
       <c r="R19" s="33"/>
@@ -2765,11 +2836,11 @@
       <c r="N20" s="27"/>
       <c r="O20" s="57"/>
       <c r="P20" s="28" t="str">
-        <f>IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$21,2,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$24,2,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q20" s="28" t="str">
-        <f>IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$21,3,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$24,3,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R20" s="33"/>
@@ -2817,11 +2888,11 @@
       <c r="N21" s="27"/>
       <c r="O21" s="57"/>
       <c r="P21" s="28" t="str">
-        <f>IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$21,2,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$24,2,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q21" s="28" t="str">
-        <f>IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$21,3,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$24,3,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R21" s="33"/>
@@ -2869,11 +2940,11 @@
       <c r="N22" s="27"/>
       <c r="O22" s="57"/>
       <c r="P22" s="28" t="str">
-        <f>IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$21,2,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$24,2,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q22" s="28" t="str">
-        <f>IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$21,3,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$24,3,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R22" s="33"/>
@@ -2921,11 +2992,11 @@
       <c r="N23" s="27"/>
       <c r="O23" s="57"/>
       <c r="P23" s="28" t="str">
-        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$21,2,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$24,2,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q23" s="28" t="str">
-        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$21,3,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$24,3,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R23" s="33"/>
@@ -2973,11 +3044,11 @@
       <c r="N24" s="27"/>
       <c r="O24" s="57"/>
       <c r="P24" s="28" t="str">
-        <f>IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$21,2,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$24,2,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q24" s="28" t="str">
-        <f>IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$21,3,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$24,3,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R24" s="33"/>
@@ -3025,11 +3096,11 @@
       <c r="N25" s="27"/>
       <c r="O25" s="57"/>
       <c r="P25" s="28" t="str">
-        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$21,2,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$24,2,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q25" s="28" t="str">
-        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$21,3,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$24,3,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R25" s="33"/>
@@ -3077,11 +3148,11 @@
       <c r="N26" s="27"/>
       <c r="O26" s="57"/>
       <c r="P26" s="28" t="str">
-        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$21,2,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$24,2,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q26" s="28" t="str">
-        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$21,3,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$24,3,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R26" s="33"/>
@@ -3129,11 +3200,11 @@
       <c r="N27" s="27"/>
       <c r="O27" s="57"/>
       <c r="P27" s="28" t="str">
-        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$21,2,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$24,2,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q27" s="28" t="str">
-        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$21,3,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$24,3,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R27" s="33"/>
@@ -3181,11 +3252,11 @@
       <c r="N28" s="27"/>
       <c r="O28" s="57"/>
       <c r="P28" s="28" t="str">
-        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$21,2,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$24,2,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q28" s="28" t="str">
-        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$21,3,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$24,3,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R28" s="33"/>
@@ -3233,11 +3304,11 @@
       <c r="N29" s="27"/>
       <c r="O29" s="57"/>
       <c r="P29" s="28" t="str">
-        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$21,2,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$24,2,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q29" s="28" t="str">
-        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$21,3,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$24,3,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R29" s="33"/>
@@ -3285,11 +3356,11 @@
       <c r="N30" s="27"/>
       <c r="O30" s="57"/>
       <c r="P30" s="28" t="str">
-        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$21,2,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$24,2,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q30" s="28" t="str">
-        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$21,3,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$24,3,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R30" s="33"/>
@@ -3337,11 +3408,11 @@
       <c r="N31" s="27"/>
       <c r="O31" s="57"/>
       <c r="P31" s="28" t="str">
-        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$21,2,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$24,2,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q31" s="28" t="str">
-        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$21,3,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$24,3,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R31" s="33"/>
@@ -3389,11 +3460,11 @@
       <c r="N32" s="27"/>
       <c r="O32" s="57"/>
       <c r="P32" s="28" t="str">
-        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$21,2,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$24,2,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q32" s="28" t="str">
-        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$21,3,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$24,3,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R32" s="33"/>
@@ -3441,11 +3512,11 @@
       <c r="N33" s="27"/>
       <c r="O33" s="57"/>
       <c r="P33" s="28" t="str">
-        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$21,2,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$24,2,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q33" s="28" t="str">
-        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$21,3,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$24,3,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R33" s="33"/>
@@ -3493,11 +3564,11 @@
       <c r="N34" s="27"/>
       <c r="O34" s="57"/>
       <c r="P34" s="28" t="str">
-        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$21,2,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$24,2,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q34" s="28" t="str">
-        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$21,3,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$24,3,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R34" s="33"/>
@@ -3545,11 +3616,11 @@
       <c r="N35" s="27"/>
       <c r="O35" s="57"/>
       <c r="P35" s="28" t="str">
-        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$21,2,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$24,2,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q35" s="28" t="str">
-        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$21,3,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$24,3,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R35" s="33"/>
@@ -3597,11 +3668,11 @@
       <c r="N36" s="27"/>
       <c r="O36" s="57"/>
       <c r="P36" s="28" t="str">
-        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$21,2,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$24,2,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q36" s="28" t="str">
-        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$21,3,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$24,3,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R36" s="33"/>
@@ -3649,11 +3720,11 @@
       <c r="N37" s="27"/>
       <c r="O37" s="57"/>
       <c r="P37" s="28" t="str">
-        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$21,2,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$24,2,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q37" s="28" t="str">
-        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$21,3,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$24,3,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R37" s="33"/>
@@ -3701,11 +3772,11 @@
       <c r="N38" s="27"/>
       <c r="O38" s="57"/>
       <c r="P38" s="28" t="str">
-        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$21,2,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$24,2,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q38" s="28" t="str">
-        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$21,3,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$24,3,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R38" s="33"/>
@@ -3753,11 +3824,11 @@
       <c r="N39" s="27"/>
       <c r="O39" s="57"/>
       <c r="P39" s="28" t="str">
-        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$21,2,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$24,2,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q39" s="28" t="str">
-        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$21,3,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$24,3,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R39" s="33"/>
@@ -3805,11 +3876,11 @@
       <c r="N40" s="27"/>
       <c r="O40" s="57"/>
       <c r="P40" s="28" t="str">
-        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$21,2,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$24,2,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q40" s="28" t="str">
-        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$21,3,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$24,3,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R40" s="33"/>
@@ -3857,11 +3928,11 @@
       <c r="N41" s="27"/>
       <c r="O41" s="57"/>
       <c r="P41" s="28" t="str">
-        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$21,2,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$24,2,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q41" s="28" t="str">
-        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$21,3,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$24,3,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R41" s="33"/>
@@ -3909,11 +3980,11 @@
       <c r="N42" s="27"/>
       <c r="O42" s="57"/>
       <c r="P42" s="28" t="str">
-        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$21,2,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$24,2,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q42" s="28" t="str">
-        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$21,3,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$24,3,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R42" s="33"/>
@@ -3961,11 +4032,11 @@
       <c r="N43" s="27"/>
       <c r="O43" s="57"/>
       <c r="P43" s="28" t="str">
-        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$21,2,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$24,2,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q43" s="28" t="str">
-        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$21,3,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$24,3,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R43" s="33"/>
@@ -4013,11 +4084,11 @@
       <c r="N44" s="27"/>
       <c r="O44" s="57"/>
       <c r="P44" s="28" t="str">
-        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$21,2,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$24,2,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q44" s="28" t="str">
-        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$21,3,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$24,3,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R44" s="33"/>
@@ -4065,11 +4136,11 @@
       <c r="N45" s="27"/>
       <c r="O45" s="57"/>
       <c r="P45" s="28" t="str">
-        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$21,2,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$24,2,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q45" s="28" t="str">
-        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$21,3,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$24,3,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R45" s="33"/>
@@ -4117,11 +4188,11 @@
       <c r="N46" s="27"/>
       <c r="O46" s="57"/>
       <c r="P46" s="28" t="str">
-        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$21,2,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$24,2,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q46" s="28" t="str">
-        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$21,3,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$24,3,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R46" s="33"/>
@@ -4169,11 +4240,11 @@
       <c r="N47" s="27"/>
       <c r="O47" s="57"/>
       <c r="P47" s="28" t="str">
-        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$21,2,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$24,2,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q47" s="28" t="str">
-        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$21,3,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$24,3,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R47" s="33"/>
@@ -4221,11 +4292,11 @@
       <c r="N48" s="27"/>
       <c r="O48" s="57"/>
       <c r="P48" s="28" t="str">
-        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$21,2,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$24,2,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q48" s="28" t="str">
-        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$21,3,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$24,3,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R48" s="33"/>
@@ -4273,11 +4344,11 @@
       <c r="N49" s="27"/>
       <c r="O49" s="57"/>
       <c r="P49" s="28" t="str">
-        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$21,2,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$24,2,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q49" s="28" t="str">
-        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$21,3,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$24,3,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R49" s="33"/>
@@ -4325,11 +4396,11 @@
       <c r="N50" s="27"/>
       <c r="O50" s="57"/>
       <c r="P50" s="28" t="str">
-        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$21,2,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$24,2,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q50" s="28" t="str">
-        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$21,3,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$24,3,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R50" s="33"/>
@@ -4377,11 +4448,11 @@
       <c r="N51" s="40"/>
       <c r="O51" s="60"/>
       <c r="P51" s="41" t="str">
-        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$21,2,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$24,2,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q51" s="41" t="str">
-        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$21,3,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$24,3,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R51" s="42"/>
@@ -4443,7 +4514,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>data!$A$2:$A$21</xm:f>
+            <xm:f>data!$A$2:$A$24</xm:f>
           </x14:formula1>
           <xm:sqref>N2:N51</xm:sqref>
         </x14:dataValidation>
@@ -4458,7 +4529,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -4482,7 +4553,7 @@
         <v>31</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -4490,7 +4561,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C2" s="50" t="s">
         <v>32</v>
@@ -4502,7 +4573,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C3" s="50" t="s">
         <v>34</v>
@@ -4511,225 +4582,261 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="51" t="s">
-        <v>36</v>
-      </c>
       <c r="C4" s="50" t="s">
-        <v>37</v>
+        <v>121</v>
       </c>
       <c r="D4" s="50"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="50" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>40</v>
+        <v>122</v>
       </c>
       <c r="D5" s="50"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="50" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>41</v>
+        <v>118</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>42</v>
+        <v>123</v>
       </c>
       <c r="D6" s="50"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="50" t="s">
-        <v>21</v>
+        <v>116</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>80</v>
+        <v>119</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>43</v>
+        <v>124</v>
       </c>
       <c r="D7" s="50"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="50" t="s">
-        <v>28</v>
+        <v>117</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>79</v>
+        <v>120</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="D8" s="50"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="50" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D9" s="50"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="50"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="50"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="50"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="50"/>
+    </row>
+    <row r="14" spans="1:4" ht="135" x14ac:dyDescent="0.15">
+      <c r="A14" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="C14" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="50"/>
-    </row>
-    <row r="11" spans="1:4" ht="135" x14ac:dyDescent="0.15">
-      <c r="A11" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="51" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="54" x14ac:dyDescent="0.15">
-      <c r="A12" s="50" t="s">
+      <c r="D14" s="51" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="54" x14ac:dyDescent="0.15">
+      <c r="A15" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="54" x14ac:dyDescent="0.15">
+      <c r="A16" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="50" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" s="51" t="s">
+      <c r="C16" s="50" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="54" x14ac:dyDescent="0.15">
-      <c r="A13" s="50" t="s">
-        <v>84</v>
-      </c>
-      <c r="B13" s="51" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="D13" s="51" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="51" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="51" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="50" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="51" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="51"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="51" t="s">
-        <v>100</v>
-      </c>
-      <c r="C16" s="50" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" s="50"/>
+      <c r="D16" s="51" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="50" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17" s="50" t="s">
-        <v>105</v>
-      </c>
-      <c r="D17" s="53" t="s">
-        <v>89</v>
+        <v>49</v>
+      </c>
+      <c r="C17" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="51" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="50" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="50" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="50"/>
+        <v>95</v>
+      </c>
+      <c r="C18" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="51"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="50" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C19" s="50" t="s">
-        <v>107</v>
-      </c>
-      <c r="D19" s="53" t="s">
-        <v>89</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="D19" s="50"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="50" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="B20" s="51" t="s">
         <v>97</v>
       </c>
       <c r="C20" s="50" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" s="53"/>
+        <v>101</v>
+      </c>
+      <c r="D20" s="53" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="52"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
+      <c r="A21" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="50"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="53" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="53"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24" s="52"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>
@@ -4753,87 +4860,87 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="48" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" s="48" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" s="48" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" s="48" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" s="48" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" s="48" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" s="48" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" s="48" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" s="48" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" s="48" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" s="48" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" s="48" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="48" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="48" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" s="48" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" s="48" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" s="48" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Copy&Paste command. etc...
</commit_message>
<xml_diff>
--- a/PaperTester.xlsx
+++ b/PaperTester.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="134">
   <si>
     <t>No.</t>
   </si>
@@ -496,23 +496,6 @@
     <t>tag=input#4</t>
   </si>
   <si>
-    <t>id=ddlEndpoint ← '1'
-id=ddlSearchType ← '1'
-id=txtQuery ← 'ラブライブ！'
-id=txtPHPSessID ← ''</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>id=ddlEndpoint ← '0'
-id=ddlSearchType ← '0'
-id=txtQuery ← '艦隊これくしょん'
-id=txtPHPSessID ← ''</t>
-    <rPh sb="59" eb="61">
-      <t>カンタイ</t>
-    </rPh>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>2-2</t>
     <phoneticPr fontId="5"/>
   </si>
@@ -618,6 +601,109 @@
     <rPh sb="19" eb="21">
       <t>ヒョウジ</t>
     </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>id=ddlEndpoint &lt;- '0'
+id=ddlSearchType &lt;- '0'
+id=txtQuery &lt;- '艦隊これくしょん'
+id=txtPHPSessID &lt;- ''</t>
+    <rPh sb="62" eb="64">
+      <t>カンタイ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>戻る</t>
+    <rPh sb="0" eb="1">
+      <t>モド</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>GoBack</t>
+  </si>
+  <si>
+    <t>前のページに戻る。</t>
+    <rPh sb="0" eb="1">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>モド</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>入力する（Copy&amp;Paste使用）</t>
+    <rPh sb="15" eb="17">
+      <t>シヨウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>ValuePaste "%0"</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>引数の形式は「&lt;画面項目の検索方法&gt;=&lt;検索キーワード&gt;#&lt;インデックス&gt; ← '&lt;入力値&gt;'」。
+改行で複数指定可能。
+  &lt;入力値&gt;
+    ・画面項目へ入力する値（日本語可。ただし、ダブルコーテーション不可）</t>
+    <rPh sb="0" eb="2">
+      <t>ヒキスウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ケイシキ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>コウモク</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>カイギョウ</t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t>フクスウ</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="57" eb="59">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="104" eb="106">
+      <t>フカ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>id=txtQuery &lt;- 'ラブライブ！ '
+id=txtPHPSessID &lt;- '0'</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>文字列をコピー&amp;ペーストする</t>
+    <rPh sb="0" eb="3">
+      <t>モジレツ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>CopyAndPaste "%0"</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -1297,7 +1383,14 @@
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FFF2F2F2"/>
+        <name val="ＭＳ Ｐゴシック"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <sz val="11"/>
@@ -1680,13 +1773,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z52"/>
+  <dimension ref="A1:Z53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="P20" sqref="P2:P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1769,7 +1862,7 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="str">
-        <f t="shared" ref="A2:A51" ca="1" si="0">IF(B2,B2,"")&amp;IF(C2,"-"&amp;C2,"")&amp;IF(D2,"-"&amp;D2,"")&amp;IF(E2,"-"&amp;E2,"")&amp;IF(F2,"-"&amp;F2,"")</f>
+        <f t="shared" ref="A2:A52" ca="1" si="0">IF(B2,B2,"")&amp;IF(C2,"-"&amp;C2,"")&amp;IF(D2,"-"&amp;D2,"")&amp;IF(E2,"-"&amp;E2,"")&amp;IF(F2,"-"&amp;F2,"")</f>
         <v>1</v>
       </c>
       <c r="B2" s="10">
@@ -1777,19 +1870,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="11">
-        <f t="shared" ref="C2:C51" ca="1" si="1">IF(TRIM(G2)="",OFFSET(C2,-1,0)+NOT(TRIM(H2)=""),0)</f>
+        <f t="shared" ref="C2:C52" ca="1" si="1">IF(TRIM(G2)="",OFFSET(C2,-1,0)+NOT(TRIM(H2)=""),0)</f>
         <v>0</v>
       </c>
       <c r="D2" s="11">
-        <f t="shared" ref="D2:D51" ca="1" si="2">IF(SUBSTITUTE(G2&amp;H2," ","")="",OFFSET(D2,-1,0)+NOT(TRIM(I2)=""),0)</f>
+        <f t="shared" ref="D2:D52" ca="1" si="2">IF(SUBSTITUTE(G2&amp;H2," ","")="",OFFSET(D2,-1,0)+NOT(TRIM(I2)=""),0)</f>
         <v>0</v>
       </c>
       <c r="E2" s="11">
-        <f t="shared" ref="E2:E51" ca="1" si="3">IF(SUBSTITUTE(G2&amp;H2&amp;I2," ","")="",OFFSET(E2,-1,0)+NOT(TRIM(J2)=""),0)</f>
+        <f t="shared" ref="E2:E52" ca="1" si="3">IF(SUBSTITUTE(G2&amp;H2&amp;I2," ","")="",OFFSET(E2,-1,0)+NOT(TRIM(J2)=""),0)</f>
         <v>0</v>
       </c>
       <c r="F2" s="11">
-        <f t="shared" ref="F2:F51" ca="1" si="4">IF(SUBSTITUTE(G2&amp;H2&amp;I2&amp;J2," ","")="",OFFSET(F2,-1,0)+NOT(TRIM(K2)=""),0)</f>
+        <f t="shared" ref="F2:F52" ca="1" si="4">IF(SUBSTITUTE(G2&amp;H2&amp;I2&amp;J2," ","")="",OFFSET(F2,-1,0)+NOT(TRIM(K2)=""),0)</f>
         <v>0</v>
       </c>
       <c r="G2" s="12" t="s">
@@ -1808,11 +1901,11 @@
       </c>
       <c r="O2" s="55"/>
       <c r="P2" s="16" t="str">
-        <f>IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$24,2,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$27,2,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>Open</v>
       </c>
       <c r="Q2" s="16" t="str">
-        <f>IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$24,3,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$27,3,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>InternetExplorerを開く。</v>
       </c>
       <c r="R2" s="17" t="s">
@@ -1878,11 +1971,11 @@
         <v>22</v>
       </c>
       <c r="P3" s="28" t="str">
-        <f>IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$A$2:$C$24,2,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$A$2:$C$27,2,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>Navigate "http://bl.ocks.org/nezuQ/raw/9719897/"</v>
       </c>
       <c r="Q3" s="28" t="str">
-        <f>IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$A$2:$C$24,3,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$A$2:$C$27,3,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>URL「http://bl.ocks.org/nezuQ/raw/9719897/」で遷移する。</v>
       </c>
       <c r="R3" s="29"/>
@@ -1897,27 +1990,27 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A4" s="22" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="A4" ca="1" si="5">IF(B4,B4,"")&amp;IF(C4,"-"&amp;C4,"")&amp;IF(D4,"-"&amp;D4,"")&amp;IF(E4,"-"&amp;E4,"")&amp;IF(F4,"-"&amp;F4,"")</f>
         <v>1</v>
       </c>
       <c r="B4" s="32">
         <f>COUNTA($G$1:$G4)-1</f>
         <v>1</v>
       </c>
-      <c r="C4" s="11">
-        <f t="shared" ca="1" si="1"/>
+      <c r="C4" s="23">
+        <f t="shared" ref="C4" ca="1" si="6">IF(TRIM(G4)="",OFFSET(C4,-1,0)+NOT(TRIM(H4)=""),0)</f>
         <v>0</v>
       </c>
       <c r="D4" s="23">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ref="D4" ca="1" si="7">IF(SUBSTITUTE(G4&amp;H4," ","")="",OFFSET(D4,-1,0)+NOT(TRIM(I4)=""),0)</f>
         <v>0</v>
       </c>
       <c r="E4" s="23">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ref="E4" ca="1" si="8">IF(SUBSTITUTE(G4&amp;H4&amp;I4," ","")="",OFFSET(E4,-1,0)+NOT(TRIM(J4)=""),0)</f>
         <v>0</v>
       </c>
       <c r="F4" s="23">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ref="F4" ca="1" si="9">IF(SUBSTITUTE(G4&amp;H4&amp;I4&amp;J4," ","")="",OFFSET(F4,-1,0)+NOT(TRIM(K4)=""),0)</f>
         <v>0</v>
       </c>
       <c r="G4" s="24"/>
@@ -1928,21 +2021,18 @@
       <c r="L4" s="26"/>
       <c r="M4" s="26"/>
       <c r="N4" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="O4" s="57" t="str">
-        <f ca="1">A4</f>
-        <v>1</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="O4" s="57"/>
       <c r="P4" s="28" t="str">
-        <f ca="1">IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$24,2,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>FullScreenShot4VisibleArea "1"</v>
+        <f>IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$27,2,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>MaximumWindow</v>
       </c>
       <c r="Q4" s="28" t="str">
-        <f ca="1">IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$24,3,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>スクリーンショットを撮る。（画面全体, 表示箇所のみ, コメント："1"）</v>
-      </c>
-      <c r="R4" s="29"/>
+        <f>IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$27,3,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>InternetExplorerを最大化する。</v>
+      </c>
+      <c r="R4" s="33"/>
       <c r="S4" s="30"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
@@ -1954,14 +2044,29 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A5" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B5" s="32">
+        <f>COUNTA($G$1:$G5)-1</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="11">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D5" s="23">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="23">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="23">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
       <c r="G5" s="24"/>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
@@ -1970,18 +2075,19 @@
       <c r="L5" s="26"/>
       <c r="M5" s="26"/>
       <c r="N5" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="O5" s="57" t="s">
-        <v>94</v>
+        <v>54</v>
+      </c>
+      <c r="O5" s="57" t="str">
+        <f ca="1">A5</f>
+        <v>1</v>
       </c>
       <c r="P5" s="28" t="str">
-        <f>IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$A$2:$C$24,2,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>ExecuteSQL "SELECT * FROM [Sheet1$] "</v>
+        <f ca="1">IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$A$2:$C$27,2,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>FullScreenShot4VisibleArea "1"</v>
       </c>
       <c r="Q5" s="28" t="str">
-        <f>IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$A$2:$C$24,3,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>SQL文を発行する。"SELECT * FROM [Sheet1$] "</v>
+        <f ca="1">IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$A$2:$C$27,3,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>スクリーンショットを撮る。（画面全体, 表示箇所のみ, コメント："1"）</v>
       </c>
       <c r="R5" s="29"/>
       <c r="S5" s="30"/>
@@ -1995,49 +2101,36 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A6" s="22" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="B6" s="32">
-        <f>COUNTA($G$1:$G6)-1</f>
-        <v>2</v>
-      </c>
-      <c r="C6" s="23">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D6" s="23">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="23">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="23">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>23</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="24"/>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
       <c r="K6" s="25"/>
       <c r="L6" s="26"/>
       <c r="M6" s="26"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="57"/>
+      <c r="N6" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="O6" s="57" t="s">
+        <v>94</v>
+      </c>
       <c r="P6" s="28" t="str">
-        <f>IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$24,2,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
+        <f>IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$27,2,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>ExecuteSQL "SELECT * FROM [Sheet1$] "</v>
       </c>
       <c r="Q6" s="28" t="str">
-        <f>IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$24,3,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
-      </c>
-      <c r="R6" s="33"/>
+        <f>IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$27,3,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>SQL文を発行する。"SELECT * FROM [Sheet1$] "</v>
+      </c>
+      <c r="R6" s="29"/>
       <c r="S6" s="30"/>
       <c r="T6" s="30"/>
       <c r="U6" s="30"/>
@@ -2047,10 +2140,10 @@
       <c r="Y6" s="25"/>
       <c r="Z6" s="21"/>
     </row>
-    <row r="7" spans="1:26" ht="54" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A7" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-1</v>
+        <v>2</v>
       </c>
       <c r="B7" s="32">
         <f>COUNTA($G$1:$G7)-1</f>
@@ -2058,7 +2151,7 @@
       </c>
       <c r="C7" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -2072,56 +2165,36 @@
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25" t="s">
-        <v>24</v>
-      </c>
+      <c r="G7" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="25"/>
       <c r="I7" s="25"/>
       <c r="J7" s="25"/>
       <c r="K7" s="25"/>
       <c r="L7" s="26"/>
-      <c r="M7" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="N7" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="O7" s="58" t="s">
-        <v>107</v>
-      </c>
+      <c r="M7" s="26"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="57"/>
       <c r="P7" s="28" t="str">
-        <f>IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$24,2,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>ValueInput "id=ddlEndpoint ← '1' %|% id=ddlSearchType ← '1' %|% id=txtQuery ← 'ラブライブ！' %|% id=txtPHPSessID ← ''"</v>
+        <f>IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$27,2,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v/>
       </c>
       <c r="Q7" s="28" t="str">
-        <f>IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$24,3,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>項目「引数の前部分」に値「引数の後部分」を入力する。"id=ddlEndpoint ← '1' %|% id=ddlSearchType ← '1' %|% id=txtQuery ← 'ラブライブ！' %|% id=txtPHPSessID ← ''"</v>
-      </c>
-      <c r="R7" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="S7" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="T7" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="U7" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="V7" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="W7" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="X7" s="31" t="s">
-        <v>20</v>
-      </c>
+        <f>IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$27,3,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v/>
+      </c>
+      <c r="R7" s="33"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="30"/>
+      <c r="U7" s="30"/>
+      <c r="V7" s="30"/>
+      <c r="W7" s="31"/>
+      <c r="X7" s="31"/>
       <c r="Y7" s="25"/>
       <c r="Z7" s="21"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:26" ht="27" x14ac:dyDescent="0.15">
       <c r="A8" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>2-1</v>
@@ -2147,33 +2220,51 @@
         <v>0</v>
       </c>
       <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
+      <c r="H8" s="25" t="s">
+        <v>24</v>
+      </c>
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
       <c r="K8" s="25"/>
       <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
+      <c r="M8" s="26" t="s">
+        <v>105</v>
+      </c>
       <c r="N8" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="O8" s="63" t="s">
-        <v>110</v>
+        <v>128</v>
+      </c>
+      <c r="O8" s="58" t="s">
+        <v>131</v>
       </c>
       <c r="P8" s="28" t="str">
-        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$24,2,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>FullScreenShot "2-1"</v>
+        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$27,2,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>ValuePaste "id=txtQuery &lt;- 'ラブライブ！ ' %|% id=txtPHPSessID &lt;- '0'"</v>
       </c>
       <c r="Q8" s="28" t="str">
-        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$24,3,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>スクリーンショットを撮る。（画面全体, コメント："2-1"）</v>
-      </c>
-      <c r="R8" s="33"/>
-      <c r="S8" s="30"/>
-      <c r="T8" s="30"/>
-      <c r="U8" s="30"/>
-      <c r="V8" s="30"/>
-      <c r="W8" s="31"/>
-      <c r="X8" s="31"/>
+        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$27,3,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>項目「引数の前部分」に値「引数の後部分」を入力する。"id=txtQuery &lt;- 'ラブライブ！ ' %|% id=txtPHPSessID &lt;- '0'"</v>
+      </c>
+      <c r="R8" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="S8" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="T8" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="U8" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="V8" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="W8" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="X8" s="31" t="s">
+        <v>20</v>
+      </c>
       <c r="Y8" s="25"/>
       <c r="Z8" s="21"/>
     </row>
@@ -2210,18 +2301,18 @@
       <c r="L9" s="26"/>
       <c r="M9" s="26"/>
       <c r="N9" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="O9" s="57" t="s">
-        <v>86</v>
+        <v>53</v>
+      </c>
+      <c r="O9" s="63" t="s">
+        <v>108</v>
       </c>
       <c r="P9" s="28" t="str">
-        <f>IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$24,2,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>Click "tag=input#4"</v>
+        <f>IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$27,2,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>FullScreenShot "2-1"</v>
       </c>
       <c r="Q9" s="28" t="str">
-        <f>IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$24,3,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>項目「tag=input#4」をクリックする。</v>
+        <f>IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$27,3,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>スクリーンショットを撮る。（画面全体, コメント："2-1"）</v>
       </c>
       <c r="R9" s="33"/>
       <c r="S9" s="30"/>
@@ -2266,16 +2357,18 @@
       <c r="L10" s="26"/>
       <c r="M10" s="26"/>
       <c r="N10" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="O10" s="57"/>
+        <v>26</v>
+      </c>
+      <c r="O10" s="57" t="s">
+        <v>86</v>
+      </c>
       <c r="P10" s="28" t="str">
-        <f>IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$24,2,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>ActivateChildWindow</v>
+        <f>IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$27,2,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>Click "tag=input#4"</v>
       </c>
       <c r="Q10" s="28" t="str">
-        <f>IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$24,3,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>子画面のウィンドウをアクティブにする。</v>
+        <f>IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$27,3,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>項目「tag=input#4」をクリックする。</v>
       </c>
       <c r="R10" s="33"/>
       <c r="S10" s="30"/>
@@ -2320,16 +2413,16 @@
       <c r="L11" s="26"/>
       <c r="M11" s="26"/>
       <c r="N11" s="27" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="O11" s="57"/>
       <c r="P11" s="28" t="str">
-        <f>IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$24,2,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>FullScreenShot ""</v>
+        <f>IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$27,2,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>ActivateChildWindow</v>
       </c>
       <c r="Q11" s="28" t="str">
-        <f>IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$24,3,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>スクリーンショットを撮る。（画面全体, コメント：""）</v>
+        <f>IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$27,3,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>子画面のウィンドウをアクティブにする。</v>
       </c>
       <c r="R11" s="33"/>
       <c r="S11" s="30"/>
@@ -2374,18 +2467,16 @@
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
       <c r="N12" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="O12" s="59" t="s">
-        <v>111</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="O12" s="57"/>
       <c r="P12" s="28" t="str">
-        <f>IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$24,2,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>ExecuteSQL "SELECT * FROM [Sheet2$] "</v>
+        <f>IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$27,2,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>FullScreenShot ""</v>
       </c>
       <c r="Q12" s="28" t="str">
-        <f>IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$24,3,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>SQL文を発行する。"SELECT * FROM [Sheet2$] "</v>
+        <f>IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$27,3,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>スクリーンショットを撮る。（画面全体, コメント：""）</v>
       </c>
       <c r="R12" s="33"/>
       <c r="S12" s="30"/>
@@ -2399,7 +2490,7 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A13" s="22" t="str">
-        <f t="shared" ref="A13" ca="1" si="5">IF(B13,B13,"")&amp;IF(C13,"-"&amp;C13,"")&amp;IF(D13,"-"&amp;D13,"")&amp;IF(E13,"-"&amp;E13,"")&amp;IF(F13,"-"&amp;F13,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2-1</v>
       </c>
       <c r="B13" s="32">
@@ -2407,19 +2498,19 @@
         <v>2</v>
       </c>
       <c r="C13" s="23">
-        <f t="shared" ref="C13" ca="1" si="6">IF(TRIM(G13)="",OFFSET(C13,-1,0)+NOT(TRIM(H13)=""),0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="D13" s="23">
-        <f t="shared" ref="D13" ca="1" si="7">IF(SUBSTITUTE(G13&amp;H13," ","")="",OFFSET(D13,-1,0)+NOT(TRIM(I13)=""),0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E13" s="23">
-        <f t="shared" ref="E13" ca="1" si="8">IF(SUBSTITUTE(G13&amp;H13&amp;I13," ","")="",OFFSET(E13,-1,0)+NOT(TRIM(J13)=""),0)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="F13" s="23">
-        <f t="shared" ref="F13" ca="1" si="9">IF(SUBSTITUTE(G13&amp;H13&amp;I13&amp;J13," ","")="",OFFSET(F13,-1,0)+NOT(TRIM(K13)=""),0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="G13" s="24"/>
@@ -2430,16 +2521,18 @@
       <c r="L13" s="26"/>
       <c r="M13" s="26"/>
       <c r="N13" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="O13" s="57"/>
+        <v>90</v>
+      </c>
+      <c r="O13" s="59" t="s">
+        <v>109</v>
+      </c>
       <c r="P13" s="28" t="str">
-        <f>IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$24,2,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>Close</v>
+        <f>IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$27,2,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>ExecuteSQL "SELECT * FROM [Sheet2$] "</v>
       </c>
       <c r="Q13" s="28" t="str">
-        <f>IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$24,3,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>InternetExplorerを閉じる。</v>
+        <f>IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$27,3,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>SQL文を発行する。"SELECT * FROM [Sheet2$] "</v>
       </c>
       <c r="R13" s="33"/>
       <c r="S13" s="30"/>
@@ -2451,81 +2544,61 @@
       <c r="Y13" s="25"/>
       <c r="Z13" s="21"/>
     </row>
-    <row r="14" spans="1:26" ht="54" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A14" s="22" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <f t="shared" ref="A14" ca="1" si="10">IF(B14,B14,"")&amp;IF(C14,"-"&amp;C14,"")&amp;IF(D14,"-"&amp;D14,"")&amp;IF(E14,"-"&amp;E14,"")&amp;IF(F14,"-"&amp;F14,"")</f>
+        <v>2-1</v>
       </c>
       <c r="B14" s="32">
         <f>COUNTA($G$1:$G14)-1</f>
         <v>2</v>
       </c>
       <c r="C14" s="23">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <f t="shared" ref="C14" ca="1" si="11">IF(TRIM(G14)="",OFFSET(C14,-1,0)+NOT(TRIM(H14)=""),0)</f>
+        <v>1</v>
       </c>
       <c r="D14" s="23">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ref="D14" ca="1" si="12">IF(SUBSTITUTE(G14&amp;H14," ","")="",OFFSET(D14,-1,0)+NOT(TRIM(I14)=""),0)</f>
         <v>0</v>
       </c>
       <c r="E14" s="23">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ref="E14" ca="1" si="13">IF(SUBSTITUTE(G14&amp;H14&amp;I14," ","")="",OFFSET(E14,-1,0)+NOT(TRIM(J14)=""),0)</f>
         <v>0</v>
       </c>
       <c r="F14" s="23">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ref="F14" ca="1" si="14">IF(SUBSTITUTE(G14&amp;H14&amp;I14&amp;J14," ","")="",OFFSET(F14,-1,0)+NOT(TRIM(K14)=""),0)</f>
         <v>0</v>
       </c>
       <c r="G14" s="24"/>
-      <c r="H14" s="25" t="s">
-        <v>104</v>
-      </c>
+      <c r="H14" s="25"/>
       <c r="I14" s="25"/>
       <c r="J14" s="25"/>
       <c r="K14" s="25"/>
       <c r="L14" s="26"/>
-      <c r="M14" s="26" t="s">
-        <v>105</v>
-      </c>
+      <c r="M14" s="26"/>
       <c r="N14" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="O14" s="58" t="s">
-        <v>108</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="O14" s="57"/>
       <c r="P14" s="28" t="str">
-        <f>IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$24,2,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>ValueInput "id=ddlEndpoint ← '0' %|% id=ddlSearchType ← '0' %|% id=txtQuery ← '艦隊これくしょん' %|% id=txtPHPSessID ← ''"</v>
+        <f>IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$27,2,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>Close</v>
       </c>
       <c r="Q14" s="28" t="str">
-        <f>IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$24,3,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>項目「引数の前部分」に値「引数の後部分」を入力する。"id=ddlEndpoint ← '0' %|% id=ddlSearchType ← '0' %|% id=txtQuery ← '艦隊これくしょん' %|% id=txtPHPSessID ← ''"</v>
-      </c>
-      <c r="R14" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="S14" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="T14" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="U14" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="V14" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="W14" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="X14" s="31" t="s">
-        <v>20</v>
-      </c>
+        <f>IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$27,3,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>InternetExplorerを閉じる。</v>
+      </c>
+      <c r="R14" s="33"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="30"/>
+      <c r="V14" s="30"/>
+      <c r="W14" s="31"/>
+      <c r="X14" s="31"/>
       <c r="Y14" s="25"/>
       <c r="Z14" s="21"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:26" ht="54" x14ac:dyDescent="0.15">
       <c r="A15" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>2-2</v>
@@ -2551,33 +2624,51 @@
         <v>0</v>
       </c>
       <c r="G15" s="24"/>
-      <c r="H15" s="25"/>
+      <c r="H15" s="25" t="s">
+        <v>104</v>
+      </c>
       <c r="I15" s="25"/>
       <c r="J15" s="25"/>
       <c r="K15" s="25"/>
       <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
+      <c r="M15" s="26" t="s">
+        <v>105</v>
+      </c>
       <c r="N15" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="O15" s="63" t="s">
-        <v>109</v>
+        <v>79</v>
+      </c>
+      <c r="O15" s="58" t="s">
+        <v>124</v>
       </c>
       <c r="P15" s="28" t="str">
-        <f>IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$24,2,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>FullScreenShot "2-2"</v>
+        <f>IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$27,2,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>ValueInput "id=ddlEndpoint &lt;- '0' %|% id=ddlSearchType &lt;- '0' %|% id=txtQuery &lt;- '艦隊これくしょん' %|% id=txtPHPSessID &lt;- ''"</v>
       </c>
       <c r="Q15" s="28" t="str">
-        <f>IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$24,3,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>スクリーンショットを撮る。（画面全体, コメント："2-2"）</v>
-      </c>
-      <c r="R15" s="33"/>
-      <c r="S15" s="30"/>
-      <c r="T15" s="30"/>
-      <c r="U15" s="30"/>
-      <c r="V15" s="30"/>
-      <c r="W15" s="31"/>
-      <c r="X15" s="31"/>
+        <f>IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$27,3,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>項目「引数の前部分」に値「引数の後部分」を入力する。"id=ddlEndpoint &lt;- '0' %|% id=ddlSearchType &lt;- '0' %|% id=txtQuery &lt;- '艦隊これくしょん' %|% id=txtPHPSessID &lt;- ''"</v>
+      </c>
+      <c r="R15" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="S15" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="T15" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="U15" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="V15" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="W15" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="X15" s="31" t="s">
+        <v>20</v>
+      </c>
       <c r="Y15" s="25"/>
       <c r="Z15" s="21"/>
     </row>
@@ -2614,18 +2705,18 @@
       <c r="L16" s="26"/>
       <c r="M16" s="26"/>
       <c r="N16" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="O16" s="57" t="s">
-        <v>106</v>
+        <v>53</v>
+      </c>
+      <c r="O16" s="63" t="s">
+        <v>107</v>
       </c>
       <c r="P16" s="28" t="str">
-        <f>IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$24,2,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>Click "tag=input#4"</v>
+        <f>IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$27,2,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>FullScreenShot "2-2"</v>
       </c>
       <c r="Q16" s="28" t="str">
-        <f>IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$24,3,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>項目「tag=input#4」をクリックする。</v>
+        <f>IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$27,3,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>スクリーンショットを撮る。（画面全体, コメント："2-2"）</v>
       </c>
       <c r="R16" s="33"/>
       <c r="S16" s="30"/>
@@ -2670,16 +2761,18 @@
       <c r="L17" s="26"/>
       <c r="M17" s="26"/>
       <c r="N17" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="O17" s="57"/>
+        <v>26</v>
+      </c>
+      <c r="O17" s="57" t="s">
+        <v>106</v>
+      </c>
       <c r="P17" s="28" t="str">
-        <f>IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$24,2,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>ActivateChildWindow</v>
+        <f>IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$27,2,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>Click "tag=input#4"</v>
       </c>
       <c r="Q17" s="28" t="str">
-        <f>IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$24,3,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>子画面のウィンドウをアクティブにする。</v>
+        <f>IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$27,3,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>項目「tag=input#4」をクリックする。</v>
       </c>
       <c r="R17" s="33"/>
       <c r="S17" s="30"/>
@@ -2724,16 +2817,16 @@
       <c r="L18" s="26"/>
       <c r="M18" s="26"/>
       <c r="N18" s="27" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="O18" s="57"/>
       <c r="P18" s="28" t="str">
-        <f>IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$24,2,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>FullScreenShot ""</v>
+        <f>IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$27,2,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>ActivateChildWindow</v>
       </c>
       <c r="Q18" s="28" t="str">
-        <f>IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$24,3,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>スクリーンショットを撮る。（画面全体, コメント：""）</v>
+        <f>IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$27,3,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>子画面のウィンドウをアクティブにする。</v>
       </c>
       <c r="R18" s="33"/>
       <c r="S18" s="30"/>
@@ -2778,18 +2871,16 @@
       <c r="L19" s="26"/>
       <c r="M19" s="26"/>
       <c r="N19" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="O19" s="59" t="s">
-        <v>111</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="O19" s="57"/>
       <c r="P19" s="28" t="str">
-        <f>IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$24,2,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>ExecuteSQL "SELECT * FROM [Sheet2$] "</v>
+        <f>IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$27,2,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>FullScreenShot ""</v>
       </c>
       <c r="Q19" s="28" t="str">
-        <f>IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$24,3,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>SQL文を発行する。"SELECT * FROM [Sheet2$] "</v>
+        <f>IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$27,3,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>スクリーンショットを撮る。（画面全体, コメント：""）</v>
       </c>
       <c r="R19" s="33"/>
       <c r="S19" s="30"/>
@@ -2833,15 +2924,19 @@
       <c r="K20" s="25"/>
       <c r="L20" s="26"/>
       <c r="M20" s="26"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="57"/>
+      <c r="N20" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="O20" s="59" t="s">
+        <v>109</v>
+      </c>
       <c r="P20" s="28" t="str">
-        <f>IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$24,2,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
+        <f>IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$27,2,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>ExecuteSQL "SELECT * FROM [Sheet2$] "</v>
       </c>
       <c r="Q20" s="28" t="str">
-        <f>IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$24,3,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
+        <f>IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$27,3,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>SQL文を発行する。"SELECT * FROM [Sheet2$] "</v>
       </c>
       <c r="R20" s="33"/>
       <c r="S20" s="30"/>
@@ -2888,11 +2983,11 @@
       <c r="N21" s="27"/>
       <c r="O21" s="57"/>
       <c r="P21" s="28" t="str">
-        <f>IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$24,2,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$27,2,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q21" s="28" t="str">
-        <f>IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$24,3,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$27,3,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R21" s="33"/>
@@ -2940,11 +3035,11 @@
       <c r="N22" s="27"/>
       <c r="O22" s="57"/>
       <c r="P22" s="28" t="str">
-        <f>IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$24,2,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$27,2,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q22" s="28" t="str">
-        <f>IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$24,3,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$27,3,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R22" s="33"/>
@@ -2992,11 +3087,11 @@
       <c r="N23" s="27"/>
       <c r="O23" s="57"/>
       <c r="P23" s="28" t="str">
-        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$24,2,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$27,2,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q23" s="28" t="str">
-        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$24,3,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$27,3,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R23" s="33"/>
@@ -3044,11 +3139,11 @@
       <c r="N24" s="27"/>
       <c r="O24" s="57"/>
       <c r="P24" s="28" t="str">
-        <f>IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$24,2,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$27,2,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q24" s="28" t="str">
-        <f>IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$24,3,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$27,3,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R24" s="33"/>
@@ -3096,11 +3191,11 @@
       <c r="N25" s="27"/>
       <c r="O25" s="57"/>
       <c r="P25" s="28" t="str">
-        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$24,2,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$27,2,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q25" s="28" t="str">
-        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$24,3,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$27,3,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R25" s="33"/>
@@ -3148,11 +3243,11 @@
       <c r="N26" s="27"/>
       <c r="O26" s="57"/>
       <c r="P26" s="28" t="str">
-        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$24,2,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$27,2,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q26" s="28" t="str">
-        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$24,3,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$27,3,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R26" s="33"/>
@@ -3200,11 +3295,11 @@
       <c r="N27" s="27"/>
       <c r="O27" s="57"/>
       <c r="P27" s="28" t="str">
-        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$24,2,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$27,2,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q27" s="28" t="str">
-        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$24,3,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$27,3,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R27" s="33"/>
@@ -3252,11 +3347,11 @@
       <c r="N28" s="27"/>
       <c r="O28" s="57"/>
       <c r="P28" s="28" t="str">
-        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$24,2,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$27,2,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q28" s="28" t="str">
-        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$24,3,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$27,3,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R28" s="33"/>
@@ -3304,11 +3399,11 @@
       <c r="N29" s="27"/>
       <c r="O29" s="57"/>
       <c r="P29" s="28" t="str">
-        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$24,2,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$27,2,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q29" s="28" t="str">
-        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$24,3,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$27,3,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R29" s="33"/>
@@ -3356,11 +3451,11 @@
       <c r="N30" s="27"/>
       <c r="O30" s="57"/>
       <c r="P30" s="28" t="str">
-        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$24,2,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$27,2,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q30" s="28" t="str">
-        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$24,3,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$27,3,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R30" s="33"/>
@@ -3408,11 +3503,11 @@
       <c r="N31" s="27"/>
       <c r="O31" s="57"/>
       <c r="P31" s="28" t="str">
-        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$24,2,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$27,2,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q31" s="28" t="str">
-        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$24,3,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$27,3,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R31" s="33"/>
@@ -3460,11 +3555,11 @@
       <c r="N32" s="27"/>
       <c r="O32" s="57"/>
       <c r="P32" s="28" t="str">
-        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$24,2,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$27,2,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q32" s="28" t="str">
-        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$24,3,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$27,3,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R32" s="33"/>
@@ -3512,11 +3607,11 @@
       <c r="N33" s="27"/>
       <c r="O33" s="57"/>
       <c r="P33" s="28" t="str">
-        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$24,2,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$27,2,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q33" s="28" t="str">
-        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$24,3,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$27,3,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R33" s="33"/>
@@ -3564,11 +3659,11 @@
       <c r="N34" s="27"/>
       <c r="O34" s="57"/>
       <c r="P34" s="28" t="str">
-        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$24,2,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$27,2,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q34" s="28" t="str">
-        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$24,3,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$27,3,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R34" s="33"/>
@@ -3616,11 +3711,11 @@
       <c r="N35" s="27"/>
       <c r="O35" s="57"/>
       <c r="P35" s="28" t="str">
-        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$24,2,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$27,2,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q35" s="28" t="str">
-        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$24,3,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$27,3,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R35" s="33"/>
@@ -3668,11 +3763,11 @@
       <c r="N36" s="27"/>
       <c r="O36" s="57"/>
       <c r="P36" s="28" t="str">
-        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$24,2,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$27,2,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q36" s="28" t="str">
-        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$24,3,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$27,3,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R36" s="33"/>
@@ -3720,11 +3815,11 @@
       <c r="N37" s="27"/>
       <c r="O37" s="57"/>
       <c r="P37" s="28" t="str">
-        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$24,2,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$27,2,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q37" s="28" t="str">
-        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$24,3,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$27,3,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R37" s="33"/>
@@ -3772,11 +3867,11 @@
       <c r="N38" s="27"/>
       <c r="O38" s="57"/>
       <c r="P38" s="28" t="str">
-        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$24,2,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$27,2,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q38" s="28" t="str">
-        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$24,3,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$27,3,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R38" s="33"/>
@@ -3824,11 +3919,11 @@
       <c r="N39" s="27"/>
       <c r="O39" s="57"/>
       <c r="P39" s="28" t="str">
-        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$24,2,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$27,2,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q39" s="28" t="str">
-        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$24,3,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$27,3,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R39" s="33"/>
@@ -3876,11 +3971,11 @@
       <c r="N40" s="27"/>
       <c r="O40" s="57"/>
       <c r="P40" s="28" t="str">
-        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$24,2,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$27,2,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q40" s="28" t="str">
-        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$24,3,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$27,3,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R40" s="33"/>
@@ -3928,11 +4023,11 @@
       <c r="N41" s="27"/>
       <c r="O41" s="57"/>
       <c r="P41" s="28" t="str">
-        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$24,2,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$27,2,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q41" s="28" t="str">
-        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$24,3,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$27,3,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R41" s="33"/>
@@ -3980,11 +4075,11 @@
       <c r="N42" s="27"/>
       <c r="O42" s="57"/>
       <c r="P42" s="28" t="str">
-        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$24,2,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$27,2,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q42" s="28" t="str">
-        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$24,3,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$27,3,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R42" s="33"/>
@@ -4032,11 +4127,11 @@
       <c r="N43" s="27"/>
       <c r="O43" s="57"/>
       <c r="P43" s="28" t="str">
-        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$24,2,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$27,2,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q43" s="28" t="str">
-        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$24,3,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$27,3,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R43" s="33"/>
@@ -4084,11 +4179,11 @@
       <c r="N44" s="27"/>
       <c r="O44" s="57"/>
       <c r="P44" s="28" t="str">
-        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$24,2,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$27,2,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q44" s="28" t="str">
-        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$24,3,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$27,3,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R44" s="33"/>
@@ -4136,11 +4231,11 @@
       <c r="N45" s="27"/>
       <c r="O45" s="57"/>
       <c r="P45" s="28" t="str">
-        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$24,2,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$27,2,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q45" s="28" t="str">
-        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$24,3,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$27,3,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R45" s="33"/>
@@ -4188,11 +4283,11 @@
       <c r="N46" s="27"/>
       <c r="O46" s="57"/>
       <c r="P46" s="28" t="str">
-        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$24,2,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$27,2,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q46" s="28" t="str">
-        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$24,3,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$27,3,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R46" s="33"/>
@@ -4240,11 +4335,11 @@
       <c r="N47" s="27"/>
       <c r="O47" s="57"/>
       <c r="P47" s="28" t="str">
-        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$24,2,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$27,2,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q47" s="28" t="str">
-        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$24,3,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$27,3,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R47" s="33"/>
@@ -4292,11 +4387,11 @@
       <c r="N48" s="27"/>
       <c r="O48" s="57"/>
       <c r="P48" s="28" t="str">
-        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$24,2,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$27,2,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q48" s="28" t="str">
-        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$24,3,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$27,3,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R48" s="33"/>
@@ -4344,11 +4439,11 @@
       <c r="N49" s="27"/>
       <c r="O49" s="57"/>
       <c r="P49" s="28" t="str">
-        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$24,2,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$27,2,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q49" s="28" t="str">
-        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$24,3,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$27,3,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R49" s="33"/>
@@ -4396,11 +4491,11 @@
       <c r="N50" s="27"/>
       <c r="O50" s="57"/>
       <c r="P50" s="28" t="str">
-        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$24,2,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$27,2,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="Q50" s="28" t="str">
-        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$24,3,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$27,3,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R50" s="33"/>
@@ -4413,95 +4508,152 @@
       <c r="Y50" s="25"/>
       <c r="Z50" s="21"/>
     </row>
-    <row r="51" spans="1:26" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="34" t="str">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A51" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>2-2</v>
       </c>
-      <c r="B51" s="35">
+      <c r="B51" s="32">
         <f>COUNTA($G$1:$G51)-1</f>
         <v>2</v>
       </c>
-      <c r="C51" s="36">
+      <c r="C51" s="23">
         <f t="shared" ca="1" si="1"/>
         <v>2</v>
       </c>
-      <c r="D51" s="36">
+      <c r="D51" s="23">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="E51" s="36">
+      <c r="E51" s="23">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
-      <c r="F51" s="36">
+      <c r="F51" s="23">
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
-      <c r="G51" s="37"/>
-      <c r="H51" s="38"/>
-      <c r="I51" s="38"/>
-      <c r="J51" s="38"/>
-      <c r="K51" s="38"/>
-      <c r="L51" s="39"/>
-      <c r="M51" s="39"/>
-      <c r="N51" s="40"/>
-      <c r="O51" s="60"/>
-      <c r="P51" s="41" t="str">
-        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$24,2,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
-      </c>
-      <c r="Q51" s="41" t="str">
-        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$24,3,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
-      </c>
-      <c r="R51" s="42"/>
-      <c r="S51" s="43"/>
-      <c r="T51" s="43"/>
-      <c r="U51" s="43"/>
-      <c r="V51" s="43"/>
-      <c r="W51" s="44"/>
-      <c r="X51" s="44"/>
-      <c r="Y51" s="45"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="25"/>
+      <c r="J51" s="25"/>
+      <c r="K51" s="25"/>
+      <c r="L51" s="26"/>
+      <c r="M51" s="26"/>
+      <c r="N51" s="27"/>
+      <c r="O51" s="57"/>
+      <c r="P51" s="28" t="str">
+        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$27,2,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v/>
+      </c>
+      <c r="Q51" s="28" t="str">
+        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$27,3,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v/>
+      </c>
+      <c r="R51" s="33"/>
+      <c r="S51" s="30"/>
+      <c r="T51" s="30"/>
+      <c r="U51" s="30"/>
+      <c r="V51" s="30"/>
+      <c r="W51" s="31"/>
+      <c r="X51" s="31"/>
+      <c r="Y51" s="25"/>
       <c r="Z51" s="21"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A52" s="46"/>
-      <c r="B52" s="46"/>
-      <c r="C52" s="46"/>
-      <c r="D52" s="46"/>
-      <c r="E52" s="46"/>
-      <c r="F52" s="46"/>
-      <c r="G52" s="46"/>
-      <c r="H52" s="46"/>
-      <c r="I52" s="46"/>
-      <c r="J52" s="46"/>
-      <c r="K52" s="46"/>
-      <c r="L52" s="46"/>
-      <c r="M52" s="46"/>
-      <c r="N52" s="47"/>
-      <c r="O52" s="61"/>
-      <c r="P52" s="47"/>
-      <c r="Q52" s="46"/>
-      <c r="R52" s="46"/>
-      <c r="S52" s="46"/>
-      <c r="T52" s="46"/>
-      <c r="U52" s="46"/>
-      <c r="V52" s="46"/>
-      <c r="W52" s="46"/>
-      <c r="X52" s="46"/>
-      <c r="Y52" s="46"/>
+    <row r="52" spans="1:26" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="34" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>2-2</v>
+      </c>
+      <c r="B52" s="35">
+        <f>COUNTA($G$1:$G52)-1</f>
+        <v>2</v>
+      </c>
+      <c r="C52" s="36">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D52" s="36">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E52" s="36">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="36">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G52" s="37"/>
+      <c r="H52" s="38"/>
+      <c r="I52" s="38"/>
+      <c r="J52" s="38"/>
+      <c r="K52" s="38"/>
+      <c r="L52" s="39"/>
+      <c r="M52" s="39"/>
+      <c r="N52" s="40"/>
+      <c r="O52" s="60"/>
+      <c r="P52" s="41" t="str">
+        <f>IF($N52="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N52,data!$A$2:$C$27,2,0),"%0",$O52), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v/>
+      </c>
+      <c r="Q52" s="41" t="str">
+        <f>IF($N52="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N52,data!$A$2:$C$27,3,0),"%0",$O52), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v/>
+      </c>
+      <c r="R52" s="42"/>
+      <c r="S52" s="43"/>
+      <c r="T52" s="43"/>
+      <c r="U52" s="43"/>
+      <c r="V52" s="43"/>
+      <c r="W52" s="44"/>
+      <c r="X52" s="44"/>
+      <c r="Y52" s="45"/>
+      <c r="Z52" s="21"/>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A53" s="46"/>
+      <c r="B53" s="46"/>
+      <c r="C53" s="46"/>
+      <c r="D53" s="46"/>
+      <c r="E53" s="46"/>
+      <c r="F53" s="46"/>
+      <c r="G53" s="46"/>
+      <c r="H53" s="46"/>
+      <c r="I53" s="46"/>
+      <c r="J53" s="46"/>
+      <c r="K53" s="46"/>
+      <c r="L53" s="46"/>
+      <c r="M53" s="46"/>
+      <c r="N53" s="47"/>
+      <c r="O53" s="61"/>
+      <c r="P53" s="47"/>
+      <c r="Q53" s="46"/>
+      <c r="R53" s="46"/>
+      <c r="S53" s="46"/>
+      <c r="T53" s="46"/>
+      <c r="U53" s="46"/>
+      <c r="V53" s="46"/>
+      <c r="W53" s="46"/>
+      <c r="X53" s="46"/>
+      <c r="Y53" s="46"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>
-  <conditionalFormatting sqref="A2:F12 A14:F51">
-    <cfRule type="expression" dxfId="1" priority="3">
+  <conditionalFormatting sqref="A2:F3 A15:F52 A5:F13">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>OR(A2=0, A2=OFFSET(A2,-1,0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13:F13">
+  <conditionalFormatting sqref="A14:F14">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>OR(A14=0, A14=OFFSET(A14,-1,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:F4">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>OR(A13=0, A13=OFFSET(A13,-1,0))</formula>
+      <formula>OR(A4=0, A4=OFFSET(A4,-1,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -4514,9 +4666,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>data!$A$2:$A$24</xm:f>
+            <xm:f>data!$A$2:$A$27</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:N51</xm:sqref>
+          <xm:sqref>N2:N52</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4529,7 +4681,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -4582,106 +4734,106 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="50" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>35</v>
+        <v>126</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D4" s="50"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="50" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="50" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D5" s="50"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="50" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>118</v>
+        <v>36</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D6" s="50"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="51" t="s">
-        <v>119</v>
-      </c>
       <c r="C7" s="50" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D7" s="50"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="B8" s="51" t="s">
-        <v>120</v>
-      </c>
       <c r="C8" s="50" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D8" s="50"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="50" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>37</v>
+        <v>118</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>38</v>
+        <v>123</v>
       </c>
       <c r="D9" s="50"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="50" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="50"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="50" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="50"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="50" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="C12" s="50" t="s">
         <v>40</v>
@@ -4690,42 +4842,40 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="50"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B14" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="50" t="s">
+      <c r="C14" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="50"/>
-    </row>
-    <row r="14" spans="1:4" ht="135" x14ac:dyDescent="0.15">
-      <c r="A14" s="50" t="s">
+      <c r="D14" s="50"/>
+    </row>
+    <row r="15" spans="1:4" ht="135" x14ac:dyDescent="0.15">
+      <c r="A15" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="B15" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="51" t="s">
+      <c r="C15" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="51" t="s">
+      <c r="D15" s="51" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="54" x14ac:dyDescent="0.15">
-      <c r="A15" s="50" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" s="50" t="s">
-        <v>112</v>
-      </c>
-      <c r="D15" s="51" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="54" x14ac:dyDescent="0.15">
@@ -4742,101 +4892,141 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="A17" s="50" t="s">
-        <v>26</v>
+        <v>128</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="51" t="s">
-        <v>50</v>
+        <v>129</v>
+      </c>
+      <c r="C17" s="50" t="s">
+        <v>110</v>
       </c>
       <c r="D17" s="51" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="A18" s="50" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="51"/>
+        <v>77</v>
+      </c>
+      <c r="C18" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="51" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="50" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" s="50" t="s">
-        <v>100</v>
-      </c>
-      <c r="D19" s="50"/>
+        <v>49</v>
+      </c>
+      <c r="C19" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="51" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="50" t="s">
-        <v>29</v>
+        <v>132</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="50" t="s">
-        <v>101</v>
-      </c>
-      <c r="D20" s="53" t="s">
-        <v>85</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="C20" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="51"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="50" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="50" t="s">
-        <v>102</v>
-      </c>
-      <c r="D21" s="50"/>
+        <v>95</v>
+      </c>
+      <c r="C21" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="51"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="50" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="53" t="s">
-        <v>85</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="D22" s="50"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="53" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="50"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="53" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="51" t="s">
+      <c r="B26" s="51" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="50" t="s">
+      <c r="C26" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="53"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="52"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
+      <c r="D26" s="53"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" s="52"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>

</xml_diff>

<commit_message>
Change command name from CopyAndPaste to Paste.
</commit_message>
<xml_diff>
--- a/PaperTester.xlsx
+++ b/PaperTester.xlsx
@@ -442,13 +442,6 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>文字列をコピー&amp;ペーストする</t>
-    <rPh sb="0" eb="3">
-      <t>モジレツ</t>
-    </rPh>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>InternetExplorerを開く。</t>
     <phoneticPr fontId="5"/>
   </si>
@@ -562,9 +555,6 @@
   </si>
   <si>
     <t>pt.Click "%0" : onErrorExit</t>
-  </si>
-  <si>
-    <t>pt.CopyAndPaste "%0" : onErrorExit</t>
   </si>
   <si>
     <t>pt.SendKeys "%0" : onErrorExit</t>
@@ -955,6 +945,17 @@
   <si>
     <t>id=ddlEndpoint &lt;- '0'
 id=txtQuery &lt;- 'あああああ '</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>文字列をペーストする</t>
+    <rPh sb="0" eb="3">
+      <t>モジレツ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>pt.Paste "%0" : onErrorExit</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -2047,7 +2048,7 @@
       <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="P2" sqref="P2:P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2400,10 +2401,10 @@
       <c r="L6" s="26"/>
       <c r="M6" s="26"/>
       <c r="N6" s="27" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="O6" s="58" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="P6" s="28" t="str">
         <f ca="1">IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$32,2,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A6 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
@@ -2558,7 +2559,7 @@
         <v>65</v>
       </c>
       <c r="O9" s="58" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="P9" s="28" t="str">
         <f ca="1">IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$32,2,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A9 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
@@ -2628,7 +2629,7 @@
         <v>100</v>
       </c>
       <c r="O10" s="58" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="P10" s="28" t="str">
         <f ca="1">IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$32,2,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A10 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
@@ -3018,7 +3019,7 @@
         <v>66</v>
       </c>
       <c r="O17" s="58" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="P17" s="28" t="str">
         <f ca="1">IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$32,2,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A17 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
@@ -3308,7 +3309,7 @@
         <v>73</v>
       </c>
       <c r="O22" s="59" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="P22" s="28" t="str">
         <f ca="1">IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$32,2,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A22 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
@@ -4947,34 +4948,34 @@
         <v>16</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D2" s="50"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="50" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C3" s="51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="51" t="s">
         <v>105</v>
-      </c>
-      <c r="B4" s="51" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="51" t="s">
-        <v>106</v>
       </c>
       <c r="D4" s="50"/>
     </row>
@@ -4983,7 +4984,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" s="51" t="s">
         <v>33</v>
@@ -4995,7 +4996,7 @@
         <v>98</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" s="51" t="s">
         <v>99</v>
@@ -5007,7 +5008,7 @@
         <v>88</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" s="51" t="s">
         <v>93</v>
@@ -5019,7 +5020,7 @@
         <v>89</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="51" t="s">
         <v>94</v>
@@ -5031,7 +5032,7 @@
         <v>90</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C9" s="51" t="s">
         <v>95</v>
@@ -5043,7 +5044,7 @@
         <v>91</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C10" s="51" t="s">
         <v>96</v>
@@ -5055,7 +5056,7 @@
         <v>92</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C11" s="51" t="s">
         <v>97</v>
@@ -5067,7 +5068,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C12" s="51" t="s">
         <v>34</v>
@@ -5079,7 +5080,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C13" s="51" t="s">
         <v>35</v>
@@ -5091,7 +5092,7 @@
         <v>28</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C14" s="51" t="s">
         <v>36</v>
@@ -5103,7 +5104,7 @@
         <v>37</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C15" s="51" t="s">
         <v>36</v>
@@ -5115,7 +5116,7 @@
         <v>38</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C16" s="51" t="s">
         <v>39</v>
@@ -5124,13 +5125,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="50" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="51" t="s">
         <v>107</v>
-      </c>
-      <c r="B17" s="51" t="s">
-        <v>124</v>
-      </c>
-      <c r="C17" s="51" t="s">
-        <v>108</v>
       </c>
       <c r="D17" s="50"/>
     </row>
@@ -5139,13 +5140,13 @@
         <v>40</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C18" s="51" t="s">
         <v>41</v>
       </c>
       <c r="D18" s="51" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="54" x14ac:dyDescent="0.15">
@@ -5153,13 +5154,13 @@
         <v>67</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C19" s="51" t="s">
         <v>75</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="54" x14ac:dyDescent="0.15">
@@ -5167,13 +5168,13 @@
         <v>100</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C20" s="51" t="s">
         <v>87</v>
       </c>
       <c r="D20" s="51" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="54" x14ac:dyDescent="0.15">
@@ -5181,13 +5182,13 @@
         <v>65</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C21" s="51" t="s">
         <v>87</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
@@ -5195,7 +5196,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C22" s="51" t="s">
         <v>42</v>
@@ -5206,10 +5207,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="50" t="s">
-        <v>101</v>
+        <v>152</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="C23" s="51" t="s">
         <v>44</v>
@@ -5221,7 +5222,7 @@
         <v>43</v>
       </c>
       <c r="B24" s="51" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C24" s="51" t="s">
         <v>44</v>
@@ -5233,7 +5234,7 @@
         <v>45</v>
       </c>
       <c r="B25" s="51" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C25" s="51" t="s">
         <v>77</v>
@@ -5245,7 +5246,7 @@
         <v>29</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C26" s="51" t="s">
         <v>78</v>
@@ -5259,7 +5260,7 @@
         <v>46</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C27" s="51" t="s">
         <v>79</v>
@@ -5271,7 +5272,7 @@
         <v>47</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C28" s="51" t="s">
         <v>80</v>
@@ -5285,7 +5286,7 @@
         <v>73</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C29" s="51" t="s">
         <v>74</v>
@@ -5294,30 +5295,30 @@
     </row>
     <row r="30" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A30" s="50" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D30" s="51" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A31" s="50" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B31" s="51" t="s">
+        <v>146</v>
+      </c>
+      <c r="C31" s="51" t="s">
         <v>148</v>
       </c>
-      <c r="C31" s="51" t="s">
-        <v>150</v>
-      </c>
       <c r="D31" s="51" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Repair Paste command description.
</commit_message>
<xml_diff>
--- a/PaperTester.xlsx
+++ b/PaperTester.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="155">
   <si>
     <t>No.</t>
   </si>
@@ -956,6 +956,16 @@
   </si>
   <si>
     <t>pt.Paste "%0" : onErrorExit</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>アクティブ画面へ「%0」を貼り付ける。</t>
+    <rPh sb="13" eb="14">
+      <t>ハ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ツ</t>
+    </rPh>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -5213,7 +5223,7 @@
         <v>153</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>44</v>
+        <v>154</v>
       </c>
       <c r="D23" s="51"/>
     </row>

</xml_diff>

<commit_message>
Add validation command description.
</commit_message>
<xml_diff>
--- a/PaperTester.xlsx
+++ b/PaperTester.xlsx
@@ -530,9 +530,6 @@
     <t>pt.NormalWindow : onErrorExit</t>
   </si>
   <si>
-    <t>pt.Sleep(%0) : onErrorExit</t>
-  </si>
-  <si>
     <t>pt.Navigate "%0" : onErrorExit</t>
   </si>
   <si>
@@ -799,7 +796,98 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
+    <t>pt.Record2ValidateAttribute "%0" : onErrorExit</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>検証する（検証NG時は処理続行）</t>
+    <rPh sb="0" eb="2">
+      <t>ケンショウ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ケンショウ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ゾッコウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>項目の属性値を検証する。検証NG時は処理を続行する。"%0"</t>
+    <rPh sb="0" eb="2">
+      <t>コウモク</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ゾクセイ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ケンショウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ケンショウ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ゾッコウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>id=txtQuery &lt;- 'ラブライブ！ '
+id=txtPHPSessID &lt;- '0'</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>id=txtQuery &lt;- '{DEL 19}'</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>id=ddlEndpoint &lt;- '0'
+id=txtQuery &lt;- 'あああああ '</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>文字列をペーストする</t>
+    <rPh sb="0" eb="3">
+      <t>モジレツ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>pt.Paste "%0" : onErrorExit</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>アクティブ画面へ「%0」を貼り付ける。</t>
+    <rPh sb="13" eb="14">
+      <t>ハ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ツ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>pt.Sleep %0 : onErrorExit</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
     <t>引数の形式は「&lt;画面項目の検索方法&gt;=&lt;検索キーワード&gt;#&lt;インデックス&gt; &lt;- &lt;検証対象の属性名&gt;='&lt;属性値&gt;'」。
+　※valueの検証の場合は、「&lt;画面項目の検索方法&gt;=&lt;検索キーワード&gt;#&lt;インデックス&gt; &lt;- '&lt;属性値&gt;'」も可。
 　&lt;検証対象の属性名&gt;
     ・検証対象の属性（Ex. value, href, alt）
 　&lt;属性値&gt;
@@ -816,155 +904,79 @@
     <rPh sb="56" eb="57">
       <t>アタイ</t>
     </rPh>
-    <rPh sb="64" eb="68">
+    <rPh sb="70" eb="72">
+      <t>ケンショウ</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="121" eb="122">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="126" eb="130">
       <t>ケンショウタイショウ</t>
     </rPh>
-    <rPh sb="69" eb="72">
+    <rPh sb="131" eb="134">
       <t>ゾクセイメイ</t>
     </rPh>
-    <rPh sb="79" eb="81">
+    <rPh sb="141" eb="143">
       <t>ケンショウ</t>
     </rPh>
-    <rPh sb="81" eb="83">
+    <rPh sb="143" eb="145">
       <t>タイショウ</t>
     </rPh>
-    <rPh sb="84" eb="86">
+    <rPh sb="146" eb="148">
       <t>ゾクセイ</t>
     </rPh>
-    <rPh sb="111" eb="114">
+    <rPh sb="173" eb="176">
       <t>ゾクセイアタイ</t>
     </rPh>
-    <rPh sb="121" eb="123">
+    <rPh sb="183" eb="185">
       <t>ケンショウ</t>
     </rPh>
-    <rPh sb="123" eb="125">
+    <rPh sb="185" eb="187">
       <t>タイショウ</t>
     </rPh>
-    <rPh sb="126" eb="128">
+    <rPh sb="188" eb="190">
       <t>ゾクセイ</t>
     </rPh>
-    <rPh sb="129" eb="131">
+    <rPh sb="191" eb="193">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="134" eb="136">
+    <rPh sb="196" eb="198">
       <t>ヨテイ</t>
     </rPh>
-    <rPh sb="137" eb="138">
+    <rPh sb="199" eb="200">
       <t>アタイ</t>
     </rPh>
-    <rPh sb="139" eb="141">
+    <rPh sb="201" eb="203">
       <t>ジッサイ</t>
     </rPh>
-    <rPh sb="142" eb="143">
+    <rPh sb="204" eb="205">
       <t>アタイ</t>
     </rPh>
-    <rPh sb="144" eb="145">
+    <rPh sb="206" eb="207">
       <t>コト</t>
     </rPh>
-    <rPh sb="150" eb="152">
+    <rPh sb="212" eb="214">
       <t>バアイ</t>
     </rPh>
-    <rPh sb="153" eb="157">
+    <rPh sb="215" eb="219">
       <t>ケンショウショリ</t>
     </rPh>
-    <rPh sb="158" eb="160">
+    <rPh sb="220" eb="222">
       <t>チュウダン</t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>引数の形式は「&lt;画面項目の検索方法&gt;=&lt;検索キーワード&gt;#&lt;インデックス&gt; &lt;- &lt;検証対象の属性名&gt;='&lt;属性値&gt;'」。</t>
+    <t>引数の形式は「&lt;画面項目の検索方法&gt;=&lt;検索キーワード&gt;#&lt;インデックス&gt; &lt;- &lt;検証対象の属性名&gt;='&lt;属性値&gt;'」。
+　※valueの検証の場合は、「&lt;画面項目の検索方法&gt;=&lt;検索キーワード&gt;#&lt;インデックス&gt; &lt;- '&lt;属性値&gt;'」も可。</t>
     <rPh sb="54" eb="56">
       <t>ゾクセイ</t>
     </rPh>
     <rPh sb="56" eb="57">
       <t>アタイ</t>
-    </rPh>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>pt.Record2ValidateAttribute "%0" : onErrorExit</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>検証する（検証NG時は処理続行）</t>
-    <rPh sb="0" eb="2">
-      <t>ケンショウ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>ケンショウ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>トキ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ショリ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>ゾッコウ</t>
-    </rPh>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>項目の属性値を検証する。検証NG時は処理を続行する。"%0"</t>
-    <rPh sb="0" eb="2">
-      <t>コウモク</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ゾクセイ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>アタイ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ケンショウ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>ケンショウ</t>
-    </rPh>
-    <rPh sb="16" eb="17">
-      <t>トキ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>ショリ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>ゾッコウ</t>
-    </rPh>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>id=txtQuery &lt;- 'ラブライブ！ '
-id=txtPHPSessID &lt;- '0'</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>id=txtQuery &lt;- '{DEL 19}'</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>id=ddlEndpoint &lt;- '0'
-id=txtQuery &lt;- 'あああああ '</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>文字列をペーストする</t>
-    <rPh sb="0" eb="3">
-      <t>モジレツ</t>
-    </rPh>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>pt.Paste "%0" : onErrorExit</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>アクティブ画面へ「%0」を貼り付ける。</t>
-    <rPh sb="13" eb="14">
-      <t>ハ</t>
-    </rPh>
-    <rPh sb="15" eb="16">
-      <t>ツ</t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -2058,7 +2070,7 @@
       <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P2" sqref="P2:P22"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2411,10 +2423,10 @@
       <c r="L6" s="26"/>
       <c r="M6" s="26"/>
       <c r="N6" s="27" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="O6" s="58" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="P6" s="28" t="str">
         <f ca="1">IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$32,2,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A6 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
@@ -2569,7 +2581,7 @@
         <v>65</v>
       </c>
       <c r="O9" s="58" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="P9" s="28" t="str">
         <f ca="1">IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$32,2,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A9 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
@@ -2639,7 +2651,7 @@
         <v>100</v>
       </c>
       <c r="O10" s="58" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="P10" s="28" t="str">
         <f ca="1">IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$32,2,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A10 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
@@ -3029,7 +3041,7 @@
         <v>66</v>
       </c>
       <c r="O17" s="58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P17" s="28" t="str">
         <f ca="1">IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$32,2,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A17 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
@@ -3319,7 +3331,7 @@
         <v>73</v>
       </c>
       <c r="O22" s="59" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P22" s="28" t="str">
         <f ca="1">IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$32,2,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A22 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
@@ -5078,7 +5090,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="C12" s="51" t="s">
         <v>34</v>
@@ -5090,7 +5102,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13" s="51" t="s">
         <v>35</v>
@@ -5102,7 +5114,7 @@
         <v>28</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" s="51" t="s">
         <v>36</v>
@@ -5114,7 +5126,7 @@
         <v>37</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C15" s="51" t="s">
         <v>36</v>
@@ -5126,7 +5138,7 @@
         <v>38</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C16" s="51" t="s">
         <v>39</v>
@@ -5138,7 +5150,7 @@
         <v>106</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C17" s="51" t="s">
         <v>107</v>
@@ -5150,13 +5162,13 @@
         <v>40</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C18" s="51" t="s">
         <v>41</v>
       </c>
       <c r="D18" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="54" x14ac:dyDescent="0.15">
@@ -5164,13 +5176,13 @@
         <v>67</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C19" s="51" t="s">
         <v>75</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="54" x14ac:dyDescent="0.15">
@@ -5178,13 +5190,13 @@
         <v>100</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C20" s="51" t="s">
         <v>87</v>
       </c>
       <c r="D20" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="54" x14ac:dyDescent="0.15">
@@ -5192,13 +5204,13 @@
         <v>65</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C21" s="51" t="s">
         <v>87</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
@@ -5206,7 +5218,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C22" s="51" t="s">
         <v>42</v>
@@ -5217,13 +5229,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="50" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D23" s="51"/>
     </row>
@@ -5232,7 +5244,7 @@
         <v>43</v>
       </c>
       <c r="B24" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C24" s="51" t="s">
         <v>44</v>
@@ -5244,7 +5256,7 @@
         <v>45</v>
       </c>
       <c r="B25" s="51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C25" s="51" t="s">
         <v>77</v>
@@ -5256,7 +5268,7 @@
         <v>29</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C26" s="51" t="s">
         <v>78</v>
@@ -5270,7 +5282,7 @@
         <v>46</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C27" s="51" t="s">
         <v>79</v>
@@ -5282,7 +5294,7 @@
         <v>47</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C28" s="51" t="s">
         <v>80</v>
@@ -5296,39 +5308,39 @@
         <v>73</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C29" s="51" t="s">
         <v>74</v>
       </c>
       <c r="D29" s="53"/>
     </row>
-    <row r="30" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="81" x14ac:dyDescent="0.15">
       <c r="A30" s="50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B30" s="51" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="C30" s="51" t="s">
-        <v>138</v>
-      </c>
       <c r="D30" s="51" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A31" s="50" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D31" s="51" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Add ExecuteJS command description.
</commit_message>
<xml_diff>
--- a/PaperTester.xlsx
+++ b/PaperTester.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="159">
   <si>
     <t>No.</t>
   </si>
@@ -796,10 +796,6 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>pt.Record2ValidateAttribute "%0" : onErrorExit</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>検証する（検証NG時は処理続行）</t>
     <rPh sb="0" eb="2">
       <t>ケンショウ</t>
@@ -977,6 +973,38 @@
     </rPh>
     <rPh sb="56" eb="57">
       <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Javascriptを実行する</t>
+    <rPh sb="11" eb="13">
+      <t>ジッコウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Javascriptコード「%0」を実行する。</t>
+    <rPh sb="18" eb="20">
+      <t>ジッコウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>pt.Record2ValidateAttribute "%0" : onErrorExit</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>pt.ExecuteJS "%0" : onErrorExit</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>alert('任意のJavascriptを実行できます。')</t>
+    <rPh sb="7" eb="9">
+      <t>ニンイ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ジッコウ</t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -2067,10 +2095,10 @@
   <dimension ref="A1:Z52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="P24" sqref="P2:P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2192,11 +2220,11 @@
       </c>
       <c r="O2" s="55"/>
       <c r="P2" s="16" t="str">
-        <f ca="1">IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$32,2,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A2 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$33,2,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A2 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Open : onErrorExit "テストケース = 1, Excel行 = 2"</v>
       </c>
       <c r="Q2" s="16" t="str">
-        <f>IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$32,3,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$33,3,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>InternetExplorerを開く。</v>
       </c>
       <c r="R2" s="17" t="s">
@@ -2262,11 +2290,11 @@
         <v>22</v>
       </c>
       <c r="P3" s="28" t="str">
-        <f ca="1">IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$A$2:$C$32,2,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A3 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$A$2:$C$33,2,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A3 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Navigate "http://bl.ocks.org/nezuQ/raw/9719897/" : onErrorExit "テストケース = 1, Excel行 = 3"</v>
       </c>
       <c r="Q3" s="28" t="str">
-        <f>IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$A$2:$C$32,3,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$A$2:$C$33,3,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>URL「http://bl.ocks.org/nezuQ/raw/9719897/」で遷移する。</v>
       </c>
       <c r="R3" s="29"/>
@@ -2316,11 +2344,11 @@
       </c>
       <c r="O4" s="57"/>
       <c r="P4" s="28" t="str">
-        <f ca="1">IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$32,2,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A4 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$33,2,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A4 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.MaximumWindow : onErrorExit "テストケース = 1, Excel行 = 4"</v>
       </c>
       <c r="Q4" s="28" t="str">
-        <f>IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$32,3,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$33,3,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>InternetExplorerを最大化する。</v>
       </c>
       <c r="R4" s="33"/>
@@ -2373,11 +2401,11 @@
         <v>1</v>
       </c>
       <c r="P5" s="28" t="str">
-        <f ca="1">IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$A$2:$C$32,2,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A5 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$A$2:$C$33,2,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A5 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.FullScreenShot4VisibleArea "1" : onErrorExit "テストケース = 1, Excel行 = 5"</v>
       </c>
       <c r="Q5" s="28" t="str">
-        <f ca="1">IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$A$2:$C$32,3,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f ca="1">IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$A$2:$C$33,3,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>スクリーンショットを撮る。（画面全体, 表示箇所のみ, コメント："1"）</v>
       </c>
       <c r="R5" s="29"/>
@@ -2423,17 +2451,17 @@
       <c r="L6" s="26"/>
       <c r="M6" s="26"/>
       <c r="N6" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O6" s="58" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P6" s="28" t="str">
-        <f ca="1">IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$32,2,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A6 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$33,2,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A6 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Record2ValidateAttribute "id=ddlEndpoint &lt;- '0' %|% id=txtQuery &lt;- 'あああああ '" : onErrorExit "テストケース = 1, Excel行 = 6"</v>
       </c>
       <c r="Q6" s="28" t="str">
-        <f>IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$32,3,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$33,3,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>項目の属性値を検証する。検証NG時は処理を続行する。"id=ddlEndpoint &lt;- '0' %|% id=txtQuery &lt;- 'あああああ '"</v>
       </c>
       <c r="R6" s="33"/>
@@ -2470,11 +2498,11 @@
         <v>76</v>
       </c>
       <c r="P7" s="28" t="str">
-        <f>IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$32,2,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A7 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$33,2,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A7 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.ExecuteSQL "SELECT * FROM [Sheet1$] " : onErrorExit "テストケース = , Excel行 = 7"</v>
       </c>
       <c r="Q7" s="28" t="str">
-        <f>IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$32,3,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$33,3,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>SQL文を発行する。"SELECT * FROM [Sheet1$] "</v>
       </c>
       <c r="R7" s="29"/>
@@ -2524,11 +2552,11 @@
       <c r="N8" s="27"/>
       <c r="O8" s="57"/>
       <c r="P8" s="28" t="str">
-        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$32,2,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A8 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$33,2,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A8 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q8" s="28" t="str">
-        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$32,3,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$33,3,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R8" s="33"/>
@@ -2581,14 +2609,14 @@
         <v>65</v>
       </c>
       <c r="O9" s="58" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P9" s="28" t="str">
-        <f ca="1">IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$32,2,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A9 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$33,2,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A9 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.KeyInput "id=txtQuery &lt;- '{DEL 19}'" : onErrorExit "テストケース = 2-1, Excel行 = 9"</v>
       </c>
       <c r="Q9" s="28" t="str">
-        <f>IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$32,3,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$33,3,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>項目「引数の前部分」に値「引数の後部分」を入力する。"id=txtQuery &lt;- '{DEL 19}'"</v>
       </c>
       <c r="R9" s="29" t="s">
@@ -2651,14 +2679,14 @@
         <v>100</v>
       </c>
       <c r="O10" s="58" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P10" s="28" t="str">
-        <f ca="1">IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$32,2,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A10 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$33,2,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A10 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.PasteInput "id=txtQuery &lt;- 'ラブライブ！ ' %|% id=txtPHPSessID &lt;- '0'" : onErrorExit "テストケース = 2-1, Excel行 = 10"</v>
       </c>
       <c r="Q10" s="28" t="str">
-        <f>IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$32,3,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$33,3,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>項目「引数の前部分」に値「引数の後部分」を入力する。"id=txtQuery &lt;- 'ラブライブ！ ' %|% id=txtPHPSessID &lt;- '0'"</v>
       </c>
       <c r="R10" s="33"/>
@@ -2710,11 +2738,11 @@
         <v>85</v>
       </c>
       <c r="P11" s="28" t="str">
-        <f ca="1">IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$32,2,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A11 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$33,2,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A11 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.FullScreenShot "2-1" : onErrorExit "テストケース = 2-1, Excel行 = 11"</v>
       </c>
       <c r="Q11" s="28" t="str">
-        <f>IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$32,3,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$33,3,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>スクリーンショットを撮る。（画面全体, コメント："2-1"）</v>
       </c>
       <c r="R11" s="33"/>
@@ -2766,11 +2794,11 @@
         <v>72</v>
       </c>
       <c r="P12" s="28" t="str">
-        <f ca="1">IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$32,2,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A12 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$33,2,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A12 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Click "tag=input#4" : onErrorExit "テストケース = 2-1, Excel行 = 12"</v>
       </c>
       <c r="Q12" s="28" t="str">
-        <f>IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$32,3,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$33,3,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>項目「tag=input#4」をクリックする。</v>
       </c>
       <c r="R12" s="33"/>
@@ -2820,11 +2848,11 @@
       </c>
       <c r="O13" s="57"/>
       <c r="P13" s="28" t="str">
-        <f ca="1">IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$32,2,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A13 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$33,2,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A13 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.ActivateChildWindow : onErrorExit "テストケース = 2-1, Excel行 = 13"</v>
       </c>
       <c r="Q13" s="28" t="str">
-        <f>IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$32,3,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$33,3,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>子画面のウィンドウをアクティブにする。</v>
       </c>
       <c r="R13" s="33"/>
@@ -2874,11 +2902,11 @@
       </c>
       <c r="O14" s="57"/>
       <c r="P14" s="28" t="str">
-        <f ca="1">IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$32,2,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A14 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$33,2,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A14 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.FullScreenShot "" : onErrorExit "テストケース = 2-1, Excel行 = 14"</v>
       </c>
       <c r="Q14" s="28" t="str">
-        <f>IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$32,3,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$33,3,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>スクリーンショットを撮る。（画面全体, コメント：""）</v>
       </c>
       <c r="R14" s="33"/>
@@ -2930,11 +2958,11 @@
         <v>86</v>
       </c>
       <c r="P15" s="28" t="str">
-        <f ca="1">IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$32,2,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A15 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$33,2,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A15 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.ExecuteSQL "SELECT * FROM [Sheet2$] " : onErrorExit "テストケース = 2-1, Excel行 = 15"</v>
       </c>
       <c r="Q15" s="28" t="str">
-        <f>IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$32,3,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$33,3,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>SQL文を発行する。"SELECT * FROM [Sheet2$] "</v>
       </c>
       <c r="R15" s="33"/>
@@ -2984,11 +3012,11 @@
       </c>
       <c r="O16" s="57"/>
       <c r="P16" s="28" t="str">
-        <f ca="1">IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$32,2,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A16 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$33,2,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A16 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Close : onErrorExit "テストケース = 2-1, Excel行 = 16"</v>
       </c>
       <c r="Q16" s="28" t="str">
-        <f>IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$32,3,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$33,3,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>InternetExplorerを閉じる。</v>
       </c>
       <c r="R16" s="33"/>
@@ -3044,11 +3072,11 @@
         <v>135</v>
       </c>
       <c r="P17" s="28" t="str">
-        <f ca="1">IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$32,2,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A17 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$33,2,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A17 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.ValueInput "id=ddlEndpoint &lt;- '1' %|% id=ddlSearchType &lt;- '1' %|% id=txtQuery &lt;- '艦隊これくしょん' %|% id=txtPHPSessID &lt;- ''" : onErrorExit "テストケース = 2-2, Excel行 = 17"</v>
       </c>
       <c r="Q17" s="28" t="str">
-        <f>IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$32,3,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$33,3,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>項目「引数の前部分」に値「引数の後部分」を入力する。"id=ddlEndpoint &lt;- '1' %|% id=ddlSearchType &lt;- '1' %|% id=txtQuery &lt;- '艦隊これくしょん' %|% id=txtPHPSessID &lt;- ''"</v>
       </c>
       <c r="R17" s="29" t="s">
@@ -3114,11 +3142,11 @@
         <v>84</v>
       </c>
       <c r="P18" s="28" t="str">
-        <f ca="1">IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$32,2,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A18 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$33,2,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A18 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.FullScreenShot "2-2" : onErrorExit "テストケース = 2-2, Excel行 = 18"</v>
       </c>
       <c r="Q18" s="28" t="str">
-        <f>IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$32,3,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$33,3,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>スクリーンショットを撮る。（画面全体, コメント："2-2"）</v>
       </c>
       <c r="R18" s="33"/>
@@ -3170,11 +3198,11 @@
         <v>83</v>
       </c>
       <c r="P19" s="28" t="str">
-        <f ca="1">IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$32,2,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A19 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$33,2,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A19 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Click "tag=input#4" : onErrorExit "テストケース = 2-2, Excel行 = 19"</v>
       </c>
       <c r="Q19" s="28" t="str">
-        <f>IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$32,3,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$33,3,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>項目「tag=input#4」をクリックする。</v>
       </c>
       <c r="R19" s="33"/>
@@ -3224,11 +3252,11 @@
       </c>
       <c r="O20" s="57"/>
       <c r="P20" s="28" t="str">
-        <f ca="1">IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$32,2,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A20 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$33,2,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A20 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.ActivateChildWindow : onErrorExit "テストケース = 2-2, Excel行 = 20"</v>
       </c>
       <c r="Q20" s="28" t="str">
-        <f>IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$32,3,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$33,3,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>子画面のウィンドウをアクティブにする。</v>
       </c>
       <c r="R20" s="33"/>
@@ -3278,11 +3306,11 @@
       </c>
       <c r="O21" s="57"/>
       <c r="P21" s="28" t="str">
-        <f ca="1">IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$32,2,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A21 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$33,2,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A21 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.FullScreenShot "" : onErrorExit "テストケース = 2-2, Excel行 = 21"</v>
       </c>
       <c r="Q21" s="28" t="str">
-        <f>IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$32,3,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$33,3,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>スクリーンショットを撮る。（画面全体, コメント：""）</v>
       </c>
       <c r="R21" s="33"/>
@@ -3334,11 +3362,11 @@
         <v>132</v>
       </c>
       <c r="P22" s="28" t="str">
-        <f ca="1">IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$32,2,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A22 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$33,2,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A22 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.ExecuteSQL "SELECT * FROM [Sheet1$] WHERE 列名1 = 2" : onErrorExit "テストケース = 2-2, Excel行 = 22"</v>
       </c>
       <c r="Q22" s="28" t="str">
-        <f>IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$32,3,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$33,3,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>SQL文を発行する。"SELECT * FROM [Sheet1$] WHERE 列名1 = 2"</v>
       </c>
       <c r="R22" s="33"/>
@@ -3386,11 +3414,11 @@
       <c r="N23" s="27"/>
       <c r="O23" s="57"/>
       <c r="P23" s="28" t="str">
-        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$32,2,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A23 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$33,2,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A23 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q23" s="28" t="str">
-        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$32,3,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$33,3,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R23" s="33"/>
@@ -3403,7 +3431,7 @@
       <c r="Y23" s="25"/>
       <c r="Z23" s="21"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:26" ht="27" x14ac:dyDescent="0.15">
       <c r="A24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>2-2</v>
@@ -3435,15 +3463,19 @@
       <c r="K24" s="25"/>
       <c r="L24" s="26"/>
       <c r="M24" s="26"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="57"/>
+      <c r="N24" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="O24" s="57" t="s">
+        <v>158</v>
+      </c>
       <c r="P24" s="28" t="str">
-        <f>IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$32,2,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A24 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v/>
+        <f ca="1">IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$33,2,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A24 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.ExecuteJS "alert('任意のJavascriptを実行できます。')" : onErrorExit "テストケース = 2-2, Excel行 = 24"</v>
       </c>
       <c r="Q24" s="28" t="str">
-        <f>IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$32,3,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
+        <f>IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$33,3,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>Javascriptコード「alert('任意のJavascriptを実行できます。')」を実行する。</v>
       </c>
       <c r="R24" s="33"/>
       <c r="S24" s="30"/>
@@ -3490,11 +3522,11 @@
       <c r="N25" s="27"/>
       <c r="O25" s="57"/>
       <c r="P25" s="28" t="str">
-        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$32,2,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A25 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$33,2,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A25 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q25" s="28" t="str">
-        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$32,3,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$33,3,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R25" s="33"/>
@@ -3542,11 +3574,11 @@
       <c r="N26" s="27"/>
       <c r="O26" s="57"/>
       <c r="P26" s="28" t="str">
-        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$32,2,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A26 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$33,2,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A26 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q26" s="28" t="str">
-        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$32,3,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$33,3,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R26" s="33"/>
@@ -3594,11 +3626,11 @@
       <c r="N27" s="27"/>
       <c r="O27" s="57"/>
       <c r="P27" s="28" t="str">
-        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$32,2,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A27 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$33,2,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A27 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q27" s="28" t="str">
-        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$32,3,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$33,3,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R27" s="33"/>
@@ -3646,11 +3678,11 @@
       <c r="N28" s="27"/>
       <c r="O28" s="57"/>
       <c r="P28" s="28" t="str">
-        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$32,2,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A28 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$33,2,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A28 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q28" s="28" t="str">
-        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$32,3,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$33,3,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R28" s="33"/>
@@ -3698,11 +3730,11 @@
       <c r="N29" s="27"/>
       <c r="O29" s="57"/>
       <c r="P29" s="28" t="str">
-        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$32,2,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A29 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$33,2,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A29 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q29" s="28" t="str">
-        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$32,3,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$33,3,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R29" s="33"/>
@@ -3750,11 +3782,11 @@
       <c r="N30" s="27"/>
       <c r="O30" s="57"/>
       <c r="P30" s="28" t="str">
-        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$32,2,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A30 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$33,2,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A30 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q30" s="28" t="str">
-        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$32,3,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$33,3,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R30" s="33"/>
@@ -3802,11 +3834,11 @@
       <c r="N31" s="27"/>
       <c r="O31" s="57"/>
       <c r="P31" s="28" t="str">
-        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$32,2,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A31 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$33,2,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A31 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q31" s="28" t="str">
-        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$32,3,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$33,3,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R31" s="33"/>
@@ -3854,11 +3886,11 @@
       <c r="N32" s="27"/>
       <c r="O32" s="57"/>
       <c r="P32" s="28" t="str">
-        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$32,2,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A32 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$33,2,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A32 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q32" s="28" t="str">
-        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$32,3,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$33,3,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R32" s="33"/>
@@ -3906,11 +3938,11 @@
       <c r="N33" s="27"/>
       <c r="O33" s="57"/>
       <c r="P33" s="28" t="str">
-        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$32,2,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A33 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$33,2,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A33 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q33" s="28" t="str">
-        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$32,3,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$33,3,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R33" s="33"/>
@@ -3958,11 +3990,11 @@
       <c r="N34" s="27"/>
       <c r="O34" s="57"/>
       <c r="P34" s="28" t="str">
-        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$32,2,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A34 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$33,2,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A34 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q34" s="28" t="str">
-        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$32,3,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$33,3,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R34" s="33"/>
@@ -4010,11 +4042,11 @@
       <c r="N35" s="27"/>
       <c r="O35" s="57"/>
       <c r="P35" s="28" t="str">
-        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$32,2,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A35 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$33,2,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A35 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q35" s="28" t="str">
-        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$32,3,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$33,3,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R35" s="33"/>
@@ -4062,11 +4094,11 @@
       <c r="N36" s="27"/>
       <c r="O36" s="57"/>
       <c r="P36" s="28" t="str">
-        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$32,2,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A36 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$33,2,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A36 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q36" s="28" t="str">
-        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$32,3,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$33,3,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R36" s="33"/>
@@ -4114,11 +4146,11 @@
       <c r="N37" s="27"/>
       <c r="O37" s="57"/>
       <c r="P37" s="28" t="str">
-        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$32,2,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A37 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$33,2,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A37 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q37" s="28" t="str">
-        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$32,3,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$33,3,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R37" s="33"/>
@@ -4166,11 +4198,11 @@
       <c r="N38" s="27"/>
       <c r="O38" s="57"/>
       <c r="P38" s="28" t="str">
-        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$32,2,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A38 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$33,2,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A38 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q38" s="28" t="str">
-        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$32,3,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$33,3,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R38" s="33"/>
@@ -4218,11 +4250,11 @@
       <c r="N39" s="27"/>
       <c r="O39" s="57"/>
       <c r="P39" s="28" t="str">
-        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$32,2,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A39 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$33,2,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A39 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q39" s="28" t="str">
-        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$32,3,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$33,3,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R39" s="33"/>
@@ -4270,11 +4302,11 @@
       <c r="N40" s="27"/>
       <c r="O40" s="57"/>
       <c r="P40" s="28" t="str">
-        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$32,2,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A40 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$33,2,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A40 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q40" s="28" t="str">
-        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$32,3,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$33,3,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R40" s="33"/>
@@ -4322,11 +4354,11 @@
       <c r="N41" s="27"/>
       <c r="O41" s="57"/>
       <c r="P41" s="28" t="str">
-        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$32,2,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A41 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$33,2,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A41 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q41" s="28" t="str">
-        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$32,3,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$33,3,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R41" s="33"/>
@@ -4374,11 +4406,11 @@
       <c r="N42" s="27"/>
       <c r="O42" s="57"/>
       <c r="P42" s="28" t="str">
-        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$32,2,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A42 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$33,2,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A42 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q42" s="28" t="str">
-        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$32,3,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$33,3,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R42" s="33"/>
@@ -4426,11 +4458,11 @@
       <c r="N43" s="27"/>
       <c r="O43" s="57"/>
       <c r="P43" s="28" t="str">
-        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$32,2,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A43 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$33,2,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A43 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q43" s="28" t="str">
-        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$32,3,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$33,3,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R43" s="33"/>
@@ -4478,11 +4510,11 @@
       <c r="N44" s="27"/>
       <c r="O44" s="57"/>
       <c r="P44" s="28" t="str">
-        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$32,2,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A44 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$33,2,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A44 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q44" s="28" t="str">
-        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$32,3,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$33,3,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R44" s="33"/>
@@ -4530,11 +4562,11 @@
       <c r="N45" s="27"/>
       <c r="O45" s="57"/>
       <c r="P45" s="28" t="str">
-        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$32,2,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A45 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$33,2,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A45 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q45" s="28" t="str">
-        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$32,3,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$33,3,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R45" s="33"/>
@@ -4582,11 +4614,11 @@
       <c r="N46" s="27"/>
       <c r="O46" s="57"/>
       <c r="P46" s="28" t="str">
-        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$32,2,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A46 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$33,2,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A46 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q46" s="28" t="str">
-        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$32,3,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$33,3,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R46" s="33"/>
@@ -4634,11 +4666,11 @@
       <c r="N47" s="27"/>
       <c r="O47" s="57"/>
       <c r="P47" s="28" t="str">
-        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$32,2,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A47 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$33,2,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A47 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q47" s="28" t="str">
-        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$32,3,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$33,3,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R47" s="33"/>
@@ -4686,11 +4718,11 @@
       <c r="N48" s="27"/>
       <c r="O48" s="57"/>
       <c r="P48" s="28" t="str">
-        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$32,2,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A48 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$33,2,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A48 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q48" s="28" t="str">
-        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$32,3,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$33,3,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R48" s="33"/>
@@ -4738,11 +4770,11 @@
       <c r="N49" s="27"/>
       <c r="O49" s="57"/>
       <c r="P49" s="28" t="str">
-        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$32,2,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A49 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$33,2,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A49 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q49" s="28" t="str">
-        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$32,3,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$33,3,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R49" s="33"/>
@@ -4790,11 +4822,11 @@
       <c r="N50" s="27"/>
       <c r="O50" s="57"/>
       <c r="P50" s="28" t="str">
-        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$32,2,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A50 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$33,2,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A50 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q50" s="28" t="str">
-        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$32,3,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$33,3,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R50" s="33"/>
@@ -4842,11 +4874,11 @@
       <c r="N51" s="40"/>
       <c r="O51" s="60"/>
       <c r="P51" s="41" t="str">
-        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$32,2,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A51 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$33,2,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A51 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q51" s="41" t="str">
-        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$32,3,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$33,3,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R51" s="42"/>
@@ -4923,7 +4955,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>data!$A$2:$A$32</xm:f>
+            <xm:f>data!$A$2:$A$33</xm:f>
           </x14:formula1>
           <xm:sqref>N2:N51</xm:sqref>
         </x14:dataValidation>
@@ -4938,7 +4970,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -5090,7 +5122,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C12" s="51" t="s">
         <v>34</v>
@@ -5229,13 +5261,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="B23" s="51" t="s">
         <v>149</v>
       </c>
-      <c r="B23" s="51" t="s">
+      <c r="C23" s="51" t="s">
         <v>150</v>
-      </c>
-      <c r="C23" s="51" t="s">
-        <v>151</v>
       </c>
       <c r="D23" s="51"/>
     </row>
@@ -5326,28 +5358,40 @@
         <v>137</v>
       </c>
       <c r="D30" s="51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A31" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="B31" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="C31" s="51" t="s">
         <v>144</v>
       </c>
-      <c r="B31" s="51" t="s">
-        <v>143</v>
-      </c>
-      <c r="C31" s="51" t="s">
-        <v>145</v>
-      </c>
       <c r="D31" s="51" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A32" s="52" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="52"/>
-      <c r="B32" s="52"/>
-      <c r="C32" s="64"/>
+      <c r="B32" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="C32" s="64" t="s">
+        <v>155</v>
+      </c>
       <c r="D32" s="52"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A33" s="52"/>
+      <c r="B33" s="52"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="52"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>

</xml_diff>

<commit_message>
Add ValidateTitle command. Add Run command.
</commit_message>
<xml_diff>
--- a/PaperTester.xlsx
+++ b/PaperTester.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="168">
   <si>
     <t>No.</t>
   </si>
@@ -93,9 +93,6 @@
     <t>検索</t>
   </si>
   <si>
-    <t>小説・タグ検索</t>
-  </si>
-  <si>
     <t>子画面が開く</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>待機する</t>
   </si>
   <si>
-    <t>子画面をアクティブにする</t>
-  </si>
-  <si>
     <t>スクリーンショットを撮る（アクティブ画面のみ）</t>
   </si>
   <si>
@@ -127,12 +121,6 @@
   </si>
   <si>
     <t>URL「%0」で遷移する。</t>
-  </si>
-  <si>
-    <t>子画面のウィンドウをアクティブにする。</t>
-  </si>
-  <si>
-    <t>親画面をアクティブにする</t>
   </si>
   <si>
     <t>指定フレームをアクティブにする</t>
@@ -257,10 +245,6 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>tag=input#4</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>SQL文を発行する</t>
     <rPh sb="3" eb="4">
       <t>ブン</t>
@@ -323,14 +307,6 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>2-1</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t xml:space="preserve">SELECT * FROM [Sheet2$] </t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>項目「引数の前部分」に値「引数の後部分」を入力する。"%0"</t>
     <rPh sb="6" eb="7">
       <t>マエ</t>
@@ -442,10 +418,6 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>InternetExplorerを開く。</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>InternetExplorer（最初に開いたもの）を取得する。</t>
     <rPh sb="17" eb="19">
       <t>サイショ</t>
@@ -503,12 +475,6 @@
     <t>pt.Open : onErrorExit</t>
   </si>
   <si>
-    <t>pt.GetIE True : onErrorExit</t>
-  </si>
-  <si>
-    <t>pt.GetIE False : onErrorExit</t>
-  </si>
-  <si>
     <t>pt.Close : onErrorExit</t>
   </si>
   <si>
@@ -531,12 +497,6 @@
   </si>
   <si>
     <t>pt.Navigate "%0" : onErrorExit</t>
-  </si>
-  <si>
-    <t>pt.ActivateChildWindow : onErrorExit</t>
-  </si>
-  <si>
-    <t>pt.ActivateParentWindow : onErrorExit</t>
   </si>
   <si>
     <t>pt.ActivateFrame %0 : onErrorExit</t>
@@ -780,41 +740,6 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>検証する（検証NG時は処理中断）</t>
-    <rPh sb="0" eb="2">
-      <t>ケンショウ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>ケンショウ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>トキ</t>
-    </rPh>
-    <rPh sb="11" eb="15">
-      <t>ショリチュウダン</t>
-    </rPh>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>検証する（検証NG時は処理続行）</t>
-    <rPh sb="0" eb="2">
-      <t>ケンショウ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>ケンショウ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>トキ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ショリ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>ゾッコウ</t>
-    </rPh>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>項目の属性値を検証する。検証NG時は処理を続行する。"%0"</t>
     <rPh sb="0" eb="2">
       <t>コウモク</t>
@@ -840,15 +765,6 @@
     <rPh sb="21" eb="23">
       <t>ゾッコウ</t>
     </rPh>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>id=txtQuery &lt;- 'ラブライブ！ '
-id=txtPHPSessID &lt;- '0'</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>id=txtQuery &lt;- '{DEL 19}'</t>
     <phoneticPr fontId="5"/>
   </si>
   <si>
@@ -1005,6 +921,253 @@
     </rPh>
     <rPh sb="21" eb="23">
       <t>ジッコウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>pt.GetIE 0 : onErrorExit</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>pt.GetIE -1 : onErrorExit</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>pt.Run "%0" : onErrorExit</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>EXEを実行する。</t>
+    <rPh sb="4" eb="6">
+      <t>ジッコウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>EXEを実行する</t>
+    <rPh sb="4" eb="6">
+      <t>ジッコウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>pt.ActivateNextIE : onErrorExit</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>pt.ActivateBeforeIE : onErrorExit</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>InternetExplorerを開く。</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>次に開いたInternetExplorerをアクティブにする。</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ヒラ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>前に開いたInternetExplorerをアクティブにする。</t>
+    <rPh sb="0" eb="1">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ヒラ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>次のIEをアクティブにする</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>前のIEをアクティブにする</t>
+    <rPh sb="0" eb="1">
+      <t>マエ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>画面項目を検証する（検証NG時は処理中断）</t>
+    <rPh sb="5" eb="7">
+      <t>ケンショウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ケンショウ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="16" eb="20">
+      <t>ショリチュウダン</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>画面項目を検証する（検証NG時は処理続行）</t>
+    <rPh sb="5" eb="7">
+      <t>ケンショウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ケンショウ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ゾッコウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>画面タイトルを検証する（検証NG時は処理中断）</t>
+    <rPh sb="7" eb="9">
+      <t>ケンショウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ケンショウ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="18" eb="22">
+      <t>ショリチュウダン</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>画面タイトルを検証する（検証NG時は処理続行）</t>
+    <rPh sb="7" eb="9">
+      <t>ケンショウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ケンショウ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ゾッコウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>pt.ValidateTitle "%0" : onErrorExit</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>pt.Record2ValidateTitle "%0" : onErrorExit</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>画面のタイトルを検証する。検証NG時は処理を中断する。（タイトル："%0"）</t>
+    <rPh sb="0" eb="2">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ケンショウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ケンショウ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>チュウダン</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>画面のタイトルを検証する。検証NG時は処理を続行する。（タイトル："%0"）</t>
+    <rPh sb="0" eb="2">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ケンショウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ケンショウ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ゾッコウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>その他</t>
+    <rPh sb="2" eb="3">
+      <t>タ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>他機能</t>
+    <rPh sb="0" eb="1">
+      <t>ホカ</t>
+    </rPh>
+    <rPh sb="1" eb="3">
+      <t>キノウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>実行結果を確認</t>
+    <rPh sb="0" eb="2">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ケッカ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>PxCSV ～Pixiv検索結果をCSV形式で～</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>不安定（SJIS/UNICODEの文字コードの違いにより、NGと判定される事がある）。</t>
+    <rPh sb="0" eb="3">
+      <t>フアンテイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>チガ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ハンテイ</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>コト</t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -2095,10 +2258,10 @@
   <dimension ref="A1:Z52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="12" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P24" sqref="P2:P24"/>
+      <selection pane="bottomRight" activeCell="P19" sqref="P2:P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2146,7 +2309,7 @@
         <v>3</v>
       </c>
       <c r="O1" s="54" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="P1" s="7" t="s">
         <v>4</v>
@@ -2220,11 +2383,11 @@
       </c>
       <c r="O2" s="55"/>
       <c r="P2" s="16" t="str">
-        <f ca="1">IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$33,2,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A2 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$36,2,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A2 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Open : onErrorExit "テストケース = 1, Excel行 = 2"</v>
       </c>
       <c r="Q2" s="16" t="str">
-        <f>IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$33,3,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$36,3,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>InternetExplorerを開く。</v>
       </c>
       <c r="R2" s="17" t="s">
@@ -2290,11 +2453,11 @@
         <v>22</v>
       </c>
       <c r="P3" s="28" t="str">
-        <f ca="1">IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$A$2:$C$33,2,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A3 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$A$2:$C$36,2,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A3 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Navigate "http://bl.ocks.org/nezuQ/raw/9719897/" : onErrorExit "テストケース = 1, Excel行 = 3"</v>
       </c>
       <c r="Q3" s="28" t="str">
-        <f>IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$A$2:$C$33,3,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$A$2:$C$36,3,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>URL「http://bl.ocks.org/nezuQ/raw/9719897/」で遷移する。</v>
       </c>
       <c r="R3" s="29"/>
@@ -2340,15 +2503,15 @@
       <c r="L4" s="26"/>
       <c r="M4" s="26"/>
       <c r="N4" s="27" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="O4" s="57"/>
       <c r="P4" s="28" t="str">
-        <f ca="1">IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$33,2,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A4 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$36,2,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A4 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.MaximumWindow : onErrorExit "テストケース = 1, Excel行 = 4"</v>
       </c>
       <c r="Q4" s="28" t="str">
-        <f>IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$33,3,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$36,3,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>InternetExplorerを最大化する。</v>
       </c>
       <c r="R4" s="33"/>
@@ -2394,18 +2557,18 @@
       <c r="L5" s="26"/>
       <c r="M5" s="26"/>
       <c r="N5" s="27" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="O5" s="57" t="str">
         <f ca="1">A5</f>
         <v>1</v>
       </c>
       <c r="P5" s="28" t="str">
-        <f ca="1">IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$A$2:$C$33,2,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A5 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$A$2:$C$36,2,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A5 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.FullScreenShot4VisibleArea "1" : onErrorExit "テストケース = 1, Excel行 = 5"</v>
       </c>
       <c r="Q5" s="28" t="str">
-        <f ca="1">IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$A$2:$C$33,3,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f ca="1">IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$A$2:$C$36,3,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>スクリーンショットを撮る。（画面全体, 表示箇所のみ, コメント："1"）</v>
       </c>
       <c r="R5" s="29"/>
@@ -2418,7 +2581,7 @@
       <c r="Y5" s="25"/>
       <c r="Z5" s="21"/>
     </row>
-    <row r="6" spans="1:26" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" ht="27" x14ac:dyDescent="0.15">
       <c r="A6" s="22" t="str">
         <f t="shared" ref="A6" ca="1" si="10">IF(B6,B6,"")&amp;IF(C6,"-"&amp;C6,"")&amp;IF(D6,"-"&amp;D6,"")&amp;IF(E6,"-"&amp;E6,"")&amp;IF(F6,"-"&amp;F6,"")</f>
         <v>1</v>
@@ -2451,18 +2614,18 @@
       <c r="L6" s="26"/>
       <c r="M6" s="26"/>
       <c r="N6" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="O6" s="58" t="s">
-        <v>147</v>
+        <v>158</v>
+      </c>
+      <c r="O6" s="57" t="s">
+        <v>166</v>
       </c>
       <c r="P6" s="28" t="str">
-        <f ca="1">IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$33,2,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A6 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.Record2ValidateAttribute "id=ddlEndpoint &lt;- '0' %|% id=txtQuery &lt;- 'あああああ '" : onErrorExit "テストケース = 1, Excel行 = 6"</v>
+        <f ca="1">IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$36,2,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A6 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.Record2ValidateTitle "PxCSV ～Pixiv検索結果をCSV形式で～" : onErrorExit "テストケース = 1, Excel行 = 6"</v>
       </c>
       <c r="Q6" s="28" t="str">
-        <f>IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$33,3,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>項目の属性値を検証する。検証NG時は処理を続行する。"id=ddlEndpoint &lt;- '0' %|% id=txtQuery &lt;- 'あああああ '"</v>
+        <f>IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$36,3,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>画面のタイトルを検証する。検証NG時は処理を続行する。（タイトル："PxCSV ～Pixiv検索結果をCSV形式で～"）</v>
       </c>
       <c r="R6" s="33"/>
       <c r="S6" s="30"/>
@@ -2474,16 +2637,31 @@
       <c r="Y6" s="25"/>
       <c r="Z6" s="21"/>
     </row>
-    <row r="7" spans="1:26" ht="27" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:26" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A7" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
+        <f t="shared" ref="A7" ca="1" si="15">IF(B7,B7,"")&amp;IF(C7,"-"&amp;C7,"")&amp;IF(D7,"-"&amp;D7,"")&amp;IF(E7,"-"&amp;E7,"")&amp;IF(F7,"-"&amp;F7,"")</f>
+        <v>1</v>
+      </c>
+      <c r="B7" s="32">
+        <f>COUNTA($G$1:$G7)-1</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="23">
+        <f t="shared" ref="C7" ca="1" si="16">IF(TRIM(G7)="",OFFSET(C7,-1,0)+NOT(TRIM(H7)=""),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="23">
+        <f t="shared" ref="D7" ca="1" si="17">IF(SUBSTITUTE(G7&amp;H7," ","")="",OFFSET(D7,-1,0)+NOT(TRIM(I7)=""),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="23">
+        <f t="shared" ref="E7" ca="1" si="18">IF(SUBSTITUTE(G7&amp;H7&amp;I7," ","")="",OFFSET(E7,-1,0)+NOT(TRIM(J7)=""),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="23">
+        <f t="shared" ref="F7" ca="1" si="19">IF(SUBSTITUTE(G7&amp;H7&amp;I7&amp;J7," ","")="",OFFSET(F7,-1,0)+NOT(TRIM(K7)=""),0)</f>
+        <v>0</v>
+      </c>
       <c r="G7" s="24"/>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -2492,20 +2670,20 @@
       <c r="L7" s="26"/>
       <c r="M7" s="26"/>
       <c r="N7" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="O7" s="57" t="s">
-        <v>76</v>
+        <v>156</v>
+      </c>
+      <c r="O7" s="58" t="s">
+        <v>131</v>
       </c>
       <c r="P7" s="28" t="str">
-        <f>IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$33,2,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A7 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.ExecuteSQL "SELECT * FROM [Sheet1$] " : onErrorExit "テストケース = , Excel行 = 7"</v>
+        <f ca="1">IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$36,2,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A7 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.Record2ValidateAttribute "id=ddlEndpoint &lt;- '0' %|% id=txtQuery &lt;- 'あああああ '" : onErrorExit "テストケース = 1, Excel行 = 7"</v>
       </c>
       <c r="Q7" s="28" t="str">
-        <f>IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$33,3,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>SQL文を発行する。"SELECT * FROM [Sheet1$] "</v>
-      </c>
-      <c r="R7" s="29"/>
+        <f>IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$36,3,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>項目の属性値を検証する。検証NG時は処理を続行する。"id=ddlEndpoint &lt;- '0' %|% id=txtQuery &lt;- 'あああああ '"</v>
+      </c>
+      <c r="R7" s="33"/>
       <c r="S7" s="30"/>
       <c r="T7" s="30"/>
       <c r="U7" s="30"/>
@@ -2515,51 +2693,38 @@
       <c r="Y7" s="25"/>
       <c r="Z7" s="21"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:26" ht="27" x14ac:dyDescent="0.15">
       <c r="A8" s="22" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="B8" s="32">
-        <f>COUNTA($G$1:$G8)-1</f>
-        <v>2</v>
-      </c>
-      <c r="C8" s="23">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D8" s="23">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="23">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="23">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>23</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B8" s="32"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="24"/>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
       <c r="K8" s="25"/>
       <c r="L8" s="26"/>
       <c r="M8" s="26"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="57"/>
+      <c r="N8" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="57" t="s">
+        <v>71</v>
+      </c>
       <c r="P8" s="28" t="str">
-        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$33,2,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A8 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v/>
+        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$36,2,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A8 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.ExecuteSQL "SELECT * FROM [Sheet1$] " : onErrorExit "テストケース = , Excel行 = 8"</v>
       </c>
       <c r="Q8" s="28" t="str">
-        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$33,3,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
-      </c>
-      <c r="R8" s="33"/>
+        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$36,3,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>SQL文を発行する。"SELECT * FROM [Sheet1$] "</v>
+      </c>
+      <c r="R8" s="29"/>
       <c r="S8" s="30"/>
       <c r="T8" s="30"/>
       <c r="U8" s="30"/>
@@ -2569,10 +2734,10 @@
       <c r="Y8" s="25"/>
       <c r="Z8" s="21"/>
     </row>
-    <row r="9" spans="1:26" ht="27" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A9" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="32">
         <f>COUNTA($G$1:$G9)-1</f>
@@ -2580,7 +2745,7 @@
       </c>
       <c r="C9" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -2594,33 +2759,27 @@
         <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25" t="s">
-        <v>24</v>
-      </c>
+      <c r="G9" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="25"/>
       <c r="I9" s="25"/>
       <c r="J9" s="25"/>
       <c r="K9" s="25"/>
       <c r="L9" s="26"/>
-      <c r="M9" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="N9" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="O9" s="58" t="s">
-        <v>146</v>
-      </c>
+      <c r="M9" s="26"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="58"/>
       <c r="P9" s="28" t="str">
-        <f ca="1">IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$33,2,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A9 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.KeyInput "id=txtQuery &lt;- '{DEL 19}'" : onErrorExit "テストケース = 2-1, Excel行 = 9"</v>
+        <f>IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$36,2,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A9 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v/>
       </c>
       <c r="Q9" s="28" t="str">
-        <f>IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$33,3,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>項目「引数の前部分」に値「引数の後部分」を入力する。"id=txtQuery &lt;- '{DEL 19}'"</v>
+        <f>IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$36,3,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v/>
       </c>
       <c r="R9" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S9" s="30" t="s">
         <v>18</v>
@@ -2643,9 +2802,9 @@
       <c r="Y9" s="25"/>
       <c r="Z9" s="21"/>
     </row>
-    <row r="10" spans="1:26" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:26" ht="54" x14ac:dyDescent="0.15">
       <c r="A10" s="22" t="str">
-        <f t="shared" ref="A10" ca="1" si="15">IF(B10,B10,"")&amp;IF(C10,"-"&amp;C10,"")&amp;IF(D10,"-"&amp;D10,"")&amp;IF(E10,"-"&amp;E10,"")&amp;IF(F10,"-"&amp;F10,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2-1</v>
       </c>
       <c r="B10" s="32">
@@ -2653,49 +2812,67 @@
         <v>2</v>
       </c>
       <c r="C10" s="23">
-        <f t="shared" ref="C10" ca="1" si="16">IF(TRIM(G10)="",OFFSET(C10,-1,0)+NOT(TRIM(H10)=""),0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="D10" s="23">
-        <f t="shared" ref="D10" ca="1" si="17">IF(SUBSTITUTE(G10&amp;H10," ","")="",OFFSET(D10,-1,0)+NOT(TRIM(I10)=""),0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E10" s="23">
-        <f t="shared" ref="E10" ca="1" si="18">IF(SUBSTITUTE(G10&amp;H10&amp;I10," ","")="",OFFSET(E10,-1,0)+NOT(TRIM(J10)=""),0)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="F10" s="23">
-        <f t="shared" ref="F10" ca="1" si="19">IF(SUBSTITUTE(G10&amp;H10&amp;I10&amp;J10," ","")="",OFFSET(F10,-1,0)+NOT(TRIM(K10)=""),0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="G10" s="24"/>
-      <c r="H10" s="25"/>
+      <c r="H10" s="25" t="s">
+        <v>76</v>
+      </c>
       <c r="I10" s="25"/>
       <c r="J10" s="25"/>
       <c r="K10" s="25"/>
       <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
+      <c r="M10" s="26" t="s">
+        <v>77</v>
+      </c>
       <c r="N10" s="27" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="O10" s="58" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="P10" s="28" t="str">
-        <f ca="1">IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$33,2,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A10 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.PasteInput "id=txtQuery &lt;- 'ラブライブ！ ' %|% id=txtPHPSessID &lt;- '0'" : onErrorExit "テストケース = 2-1, Excel行 = 10"</v>
+        <f ca="1">IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$36,2,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A10 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.ValueInput "id=ddlEndpoint &lt;- '1' %|% id=ddlSearchType &lt;- '1' %|% id=txtQuery &lt;- '艦隊これくしょん' %|% id=txtPHPSessID &lt;- ''" : onErrorExit "テストケース = 2-1, Excel行 = 10"</v>
       </c>
       <c r="Q10" s="28" t="str">
-        <f>IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$33,3,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>項目「引数の前部分」に値「引数の後部分」を入力する。"id=txtQuery &lt;- 'ラブライブ！ ' %|% id=txtPHPSessID &lt;- '0'"</v>
-      </c>
-      <c r="R10" s="33"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="30"/>
-      <c r="V10" s="30"/>
-      <c r="W10" s="31"/>
-      <c r="X10" s="31"/>
+        <f>IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$36,3,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>項目「引数の前部分」に値「引数の後部分」を入力する。"id=ddlEndpoint &lt;- '1' %|% id=ddlSearchType &lt;- '1' %|% id=txtQuery &lt;- '艦隊これくしょん' %|% id=txtPHPSessID &lt;- ''"</v>
+      </c>
+      <c r="R10" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="S10" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="T10" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="U10" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="V10" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="W10" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="X10" s="31" t="s">
+        <v>20</v>
+      </c>
       <c r="Y10" s="25"/>
       <c r="Z10" s="21"/>
     </row>
@@ -2732,18 +2909,18 @@
       <c r="L11" s="26"/>
       <c r="M11" s="26"/>
       <c r="N11" s="27" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="O11" s="63" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="P11" s="28" t="str">
-        <f ca="1">IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$33,2,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A11 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.FullScreenShot "2-1" : onErrorExit "テストケース = 2-1, Excel行 = 11"</v>
+        <f ca="1">IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$36,2,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A11 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.FullScreenShot "2-2" : onErrorExit "テストケース = 2-1, Excel行 = 11"</v>
       </c>
       <c r="Q11" s="28" t="str">
-        <f>IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$33,3,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>スクリーンショットを撮る。（画面全体, コメント："2-1"）</v>
+        <f>IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$36,3,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>スクリーンショットを撮る。（画面全体, コメント："2-2"）</v>
       </c>
       <c r="R11" s="33"/>
       <c r="S11" s="30"/>
@@ -2788,17 +2965,17 @@
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
       <c r="N12" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O12" s="57" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="P12" s="28" t="str">
-        <f ca="1">IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$33,2,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A12 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$36,2,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A12 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Click "tag=input#4" : onErrorExit "テストケース = 2-1, Excel行 = 12"</v>
       </c>
       <c r="Q12" s="28" t="str">
-        <f>IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$33,3,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$36,3,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>項目「tag=input#4」をクリックする。</v>
       </c>
       <c r="R12" s="33"/>
@@ -2844,16 +3021,16 @@
       <c r="L13" s="26"/>
       <c r="M13" s="26"/>
       <c r="N13" s="27" t="s">
-        <v>28</v>
+        <v>153</v>
       </c>
       <c r="O13" s="57"/>
       <c r="P13" s="28" t="str">
-        <f ca="1">IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$33,2,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A13 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.ActivateChildWindow : onErrorExit "テストケース = 2-1, Excel行 = 13"</v>
+        <f ca="1">IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$36,2,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A13 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.ActivateNextIE : onErrorExit "テストケース = 2-1, Excel行 = 13"</v>
       </c>
       <c r="Q13" s="28" t="str">
-        <f>IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$33,3,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>子画面のウィンドウをアクティブにする。</v>
+        <f>IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$36,3,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>次に開いたInternetExplorerをアクティブにする。</v>
       </c>
       <c r="R13" s="33"/>
       <c r="S13" s="30"/>
@@ -2898,15 +3075,15 @@
       <c r="L14" s="26"/>
       <c r="M14" s="26"/>
       <c r="N14" s="27" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="O14" s="57"/>
       <c r="P14" s="28" t="str">
-        <f ca="1">IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$33,2,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A14 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$36,2,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A14 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.FullScreenShot "" : onErrorExit "テストケース = 2-1, Excel行 = 14"</v>
       </c>
       <c r="Q14" s="28" t="str">
-        <f>IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$33,3,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$36,3,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>スクリーンショットを撮る。（画面全体, コメント：""）</v>
       </c>
       <c r="R14" s="33"/>
@@ -2952,18 +3129,18 @@
       <c r="L15" s="26"/>
       <c r="M15" s="26"/>
       <c r="N15" s="27" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="O15" s="59" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="P15" s="28" t="str">
-        <f ca="1">IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$33,2,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A15 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.ExecuteSQL "SELECT * FROM [Sheet2$] " : onErrorExit "テストケース = 2-1, Excel行 = 15"</v>
+        <f ca="1">IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$36,2,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A15 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.ExecuteSQL "SELECT * FROM [Sheet1$] WHERE 列名1 = 2" : onErrorExit "テストケース = 2-1, Excel行 = 15"</v>
       </c>
       <c r="Q15" s="28" t="str">
-        <f>IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$33,3,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>SQL文を発行する。"SELECT * FROM [Sheet2$] "</v>
+        <f>IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$36,3,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>SQL文を発行する。"SELECT * FROM [Sheet1$] WHERE 列名1 = 2"</v>
       </c>
       <c r="R15" s="33"/>
       <c r="S15" s="30"/>
@@ -2977,47 +3154,47 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A16" s="22" t="str">
-        <f t="shared" ref="A16" ca="1" si="20">IF(B16,B16,"")&amp;IF(C16,"-"&amp;C16,"")&amp;IF(D16,"-"&amp;D16,"")&amp;IF(E16,"-"&amp;E16,"")&amp;IF(F16,"-"&amp;F16,"")</f>
-        <v>2-1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
       </c>
       <c r="B16" s="32">
         <f>COUNTA($G$1:$G16)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" s="23">
-        <f t="shared" ref="C16" ca="1" si="21">IF(TRIM(G16)="",OFFSET(C16,-1,0)+NOT(TRIM(H16)=""),0)</f>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="D16" s="23">
-        <f t="shared" ref="D16" ca="1" si="22">IF(SUBSTITUTE(G16&amp;H16," ","")="",OFFSET(D16,-1,0)+NOT(TRIM(I16)=""),0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E16" s="23">
-        <f t="shared" ref="E16" ca="1" si="23">IF(SUBSTITUTE(G16&amp;H16&amp;I16," ","")="",OFFSET(E16,-1,0)+NOT(TRIM(J16)=""),0)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="F16" s="23">
-        <f t="shared" ref="F16" ca="1" si="24">IF(SUBSTITUTE(G16&amp;H16&amp;I16&amp;J16," ","")="",OFFSET(F16,-1,0)+NOT(TRIM(K16)=""),0)</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="24"/>
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>163</v>
+      </c>
       <c r="H16" s="25"/>
       <c r="I16" s="25"/>
       <c r="J16" s="25"/>
       <c r="K16" s="25"/>
       <c r="L16" s="26"/>
       <c r="M16" s="26"/>
-      <c r="N16" s="27" t="s">
-        <v>32</v>
-      </c>
+      <c r="N16" s="27"/>
       <c r="O16" s="57"/>
       <c r="P16" s="28" t="str">
-        <f ca="1">IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$33,2,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A16 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.Close : onErrorExit "テストケース = 2-1, Excel行 = 16"</v>
+        <f>IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$36,2,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A16 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v/>
       </c>
       <c r="Q16" s="28" t="str">
-        <f>IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$33,3,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>InternetExplorerを閉じる。</v>
+        <f>IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$36,3,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v/>
       </c>
       <c r="R16" s="33"/>
       <c r="S16" s="30"/>
@@ -3029,18 +3206,18 @@
       <c r="Y16" s="25"/>
       <c r="Z16" s="21"/>
     </row>
-    <row r="17" spans="1:26" ht="54" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A17" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B17" s="32">
         <f>COUNTA($G$1:$G17)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -3056,65 +3233,49 @@
       </c>
       <c r="G17" s="24"/>
       <c r="H17" s="25" t="s">
-        <v>81</v>
+        <v>164</v>
       </c>
       <c r="I17" s="25"/>
       <c r="J17" s="25"/>
       <c r="K17" s="25"/>
       <c r="L17" s="26"/>
       <c r="M17" s="26" t="s">
-        <v>82</v>
+        <v>165</v>
       </c>
       <c r="N17" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="O17" s="58" t="s">
-        <v>135</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="O17" s="57"/>
       <c r="P17" s="28" t="str">
-        <f ca="1">IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$33,2,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A17 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.ValueInput "id=ddlEndpoint &lt;- '1' %|% id=ddlSearchType &lt;- '1' %|% id=txtQuery &lt;- '艦隊これくしょん' %|% id=txtPHPSessID &lt;- ''" : onErrorExit "テストケース = 2-2, Excel行 = 17"</v>
+        <f ca="1">IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$36,2,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A17 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.Close : onErrorExit "テストケース = 3-1, Excel行 = 17"</v>
       </c>
       <c r="Q17" s="28" t="str">
-        <f>IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$33,3,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>項目「引数の前部分」に値「引数の後部分」を入力する。"id=ddlEndpoint &lt;- '1' %|% id=ddlSearchType &lt;- '1' %|% id=txtQuery &lt;- '艦隊これくしょん' %|% id=txtPHPSessID &lt;- ''"</v>
-      </c>
-      <c r="R17" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="S17" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="T17" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="U17" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="V17" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="W17" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="X17" s="31" t="s">
-        <v>20</v>
-      </c>
+        <f>IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$36,3,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>InternetExplorerを閉じる。</v>
+      </c>
+      <c r="R17" s="33"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="30"/>
+      <c r="V17" s="30"/>
+      <c r="W17" s="31"/>
+      <c r="X17" s="31"/>
       <c r="Y17" s="25"/>
       <c r="Z17" s="21"/>
     </row>
     <row r="18" spans="1:26" ht="27" x14ac:dyDescent="0.15">
       <c r="A18" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B18" s="32">
         <f>COUNTA($G$1:$G18)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -3136,18 +3297,18 @@
       <c r="L18" s="26"/>
       <c r="M18" s="26"/>
       <c r="N18" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="O18" s="63" t="s">
-        <v>84</v>
+        <v>138</v>
+      </c>
+      <c r="O18" s="57" t="s">
+        <v>142</v>
       </c>
       <c r="P18" s="28" t="str">
-        <f ca="1">IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$33,2,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A18 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.FullScreenShot "2-2" : onErrorExit "テストケース = 2-2, Excel行 = 18"</v>
+        <f ca="1">IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$36,2,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A18 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.ExecuteJS "alert('任意のJavascriptを実行できます。')" : onErrorExit "テストケース = 3-1, Excel行 = 18"</v>
       </c>
       <c r="Q18" s="28" t="str">
-        <f>IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$33,3,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>スクリーンショットを撮る。（画面全体, コメント："2-2"）</v>
+        <f>IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$36,3,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>Javascriptコード「alert('任意のJavascriptを実行できます。')」を実行する。</v>
       </c>
       <c r="R18" s="33"/>
       <c r="S18" s="30"/>
@@ -3159,18 +3320,18 @@
       <c r="Y18" s="25"/>
       <c r="Z18" s="21"/>
     </row>
-    <row r="19" spans="1:26" ht="27" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B19" s="32">
         <f>COUNTA($G$1:$G19)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -3192,18 +3353,16 @@
       <c r="L19" s="26"/>
       <c r="M19" s="26"/>
       <c r="N19" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="O19" s="57" t="s">
-        <v>83</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="O19" s="57"/>
       <c r="P19" s="28" t="str">
-        <f ca="1">IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$33,2,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A19 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.Click "tag=input#4" : onErrorExit "テストケース = 2-2, Excel行 = 19"</v>
+        <f ca="1">IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$36,2,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A19 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.Close : onErrorExit "テストケース = 3-1, Excel行 = 19"</v>
       </c>
       <c r="Q19" s="28" t="str">
-        <f>IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$33,3,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>項目「tag=input#4」をクリックする。</v>
+        <f>IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$36,3,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>InternetExplorerを閉じる。</v>
       </c>
       <c r="R19" s="33"/>
       <c r="S19" s="30"/>
@@ -3218,15 +3377,15 @@
     <row r="20" spans="1:26" ht="27" x14ac:dyDescent="0.15">
       <c r="A20" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B20" s="32">
         <f>COUNTA($G$1:$G20)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C20" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -3247,17 +3406,15 @@
       <c r="K20" s="25"/>
       <c r="L20" s="26"/>
       <c r="M20" s="26"/>
-      <c r="N20" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="N20" s="27"/>
       <c r="O20" s="57"/>
       <c r="P20" s="28" t="str">
-        <f ca="1">IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$33,2,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A20 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.ActivateChildWindow : onErrorExit "テストケース = 2-2, Excel行 = 20"</v>
+        <f>IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$36,2,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A20 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v/>
       </c>
       <c r="Q20" s="28" t="str">
-        <f>IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$33,3,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>子画面のウィンドウをアクティブにする。</v>
+        <f>IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$36,3,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v/>
       </c>
       <c r="R20" s="33"/>
       <c r="S20" s="30"/>
@@ -3272,15 +3429,15 @@
     <row r="21" spans="1:26" ht="27" x14ac:dyDescent="0.15">
       <c r="A21" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B21" s="32">
         <f>COUNTA($G$1:$G21)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -3301,17 +3458,15 @@
       <c r="K21" s="25"/>
       <c r="L21" s="26"/>
       <c r="M21" s="26"/>
-      <c r="N21" s="27" t="s">
-        <v>45</v>
-      </c>
+      <c r="N21" s="27"/>
       <c r="O21" s="57"/>
       <c r="P21" s="28" t="str">
-        <f ca="1">IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$33,2,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A21 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.FullScreenShot "" : onErrorExit "テストケース = 2-2, Excel行 = 21"</v>
+        <f>IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$36,2,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A21 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v/>
       </c>
       <c r="Q21" s="28" t="str">
-        <f>IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$33,3,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>スクリーンショットを撮る。（画面全体, コメント：""）</v>
+        <f>IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$36,3,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v/>
       </c>
       <c r="R21" s="33"/>
       <c r="S21" s="30"/>
@@ -3326,15 +3481,15 @@
     <row r="22" spans="1:26" ht="27" x14ac:dyDescent="0.15">
       <c r="A22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B22" s="32">
         <f>COUNTA($G$1:$G22)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C22" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -3355,19 +3510,15 @@
       <c r="K22" s="25"/>
       <c r="L22" s="26"/>
       <c r="M22" s="26"/>
-      <c r="N22" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="O22" s="59" t="s">
-        <v>132</v>
-      </c>
+      <c r="N22" s="27"/>
+      <c r="O22" s="57"/>
       <c r="P22" s="28" t="str">
-        <f ca="1">IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$33,2,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A22 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.ExecuteSQL "SELECT * FROM [Sheet1$] WHERE 列名1 = 2" : onErrorExit "テストケース = 2-2, Excel行 = 22"</v>
+        <f>IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$36,2,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A22 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v/>
       </c>
       <c r="Q22" s="28" t="str">
-        <f>IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$33,3,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>SQL文を発行する。"SELECT * FROM [Sheet1$] WHERE 列名1 = 2"</v>
+        <f>IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$36,3,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v/>
       </c>
       <c r="R22" s="33"/>
       <c r="S22" s="30"/>
@@ -3382,15 +3533,15 @@
     <row r="23" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B23" s="32">
         <f>COUNTA($G$1:$G23)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C23" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -3414,11 +3565,11 @@
       <c r="N23" s="27"/>
       <c r="O23" s="57"/>
       <c r="P23" s="28" t="str">
-        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$33,2,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A23 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$36,2,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A23 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q23" s="28" t="str">
-        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$33,3,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$36,3,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R23" s="33"/>
@@ -3431,18 +3582,18 @@
       <c r="Y23" s="25"/>
       <c r="Z23" s="21"/>
     </row>
-    <row r="24" spans="1:26" ht="27" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A24" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B24" s="32">
         <f>COUNTA($G$1:$G24)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C24" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -3463,19 +3614,15 @@
       <c r="K24" s="25"/>
       <c r="L24" s="26"/>
       <c r="M24" s="26"/>
-      <c r="N24" s="27" t="s">
-        <v>154</v>
-      </c>
-      <c r="O24" s="57" t="s">
-        <v>158</v>
-      </c>
+      <c r="N24" s="27"/>
+      <c r="O24" s="57"/>
       <c r="P24" s="28" t="str">
-        <f ca="1">IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$33,2,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A24 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.ExecuteJS "alert('任意のJavascriptを実行できます。')" : onErrorExit "テストケース = 2-2, Excel行 = 24"</v>
+        <f>IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$36,2,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A24 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v/>
       </c>
       <c r="Q24" s="28" t="str">
-        <f>IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$33,3,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>Javascriptコード「alert('任意のJavascriptを実行できます。')」を実行する。</v>
+        <f>IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$36,3,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v/>
       </c>
       <c r="R24" s="33"/>
       <c r="S24" s="30"/>
@@ -3490,15 +3637,15 @@
     <row r="25" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A25" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B25" s="32">
         <f>COUNTA($G$1:$G25)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -3522,11 +3669,11 @@
       <c r="N25" s="27"/>
       <c r="O25" s="57"/>
       <c r="P25" s="28" t="str">
-        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$33,2,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A25 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$36,2,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A25 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q25" s="28" t="str">
-        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$33,3,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$36,3,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R25" s="33"/>
@@ -3542,15 +3689,15 @@
     <row r="26" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A26" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B26" s="32">
         <f>COUNTA($G$1:$G26)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C26" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -3574,11 +3721,11 @@
       <c r="N26" s="27"/>
       <c r="O26" s="57"/>
       <c r="P26" s="28" t="str">
-        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$33,2,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A26 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$36,2,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A26 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q26" s="28" t="str">
-        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$33,3,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$36,3,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R26" s="33"/>
@@ -3594,15 +3741,15 @@
     <row r="27" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A27" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B27" s="32">
         <f>COUNTA($G$1:$G27)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -3626,11 +3773,11 @@
       <c r="N27" s="27"/>
       <c r="O27" s="57"/>
       <c r="P27" s="28" t="str">
-        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$33,2,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A27 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$36,2,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A27 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q27" s="28" t="str">
-        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$33,3,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$36,3,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R27" s="33"/>
@@ -3645,27 +3792,27 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A28" s="22" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <f t="shared" ref="A28:A34" ca="1" si="20">IF(B28,B28,"")&amp;IF(C28,"-"&amp;C28,"")&amp;IF(D28,"-"&amp;D28,"")&amp;IF(E28,"-"&amp;E28,"")&amp;IF(F28,"-"&amp;F28,"")</f>
+        <v>3-1</v>
       </c>
       <c r="B28" s="32">
         <f>COUNTA($G$1:$G28)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C28" s="23">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <f t="shared" ref="C28:C34" ca="1" si="21">IF(TRIM(G28)="",OFFSET(C28,-1,0)+NOT(TRIM(H28)=""),0)</f>
+        <v>1</v>
       </c>
       <c r="D28" s="23">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ref="D28:D34" ca="1" si="22">IF(SUBSTITUTE(G28&amp;H28," ","")="",OFFSET(D28,-1,0)+NOT(TRIM(I28)=""),0)</f>
         <v>0</v>
       </c>
       <c r="E28" s="23">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ref="E28:E34" ca="1" si="23">IF(SUBSTITUTE(G28&amp;H28&amp;I28," ","")="",OFFSET(E28,-1,0)+NOT(TRIM(J28)=""),0)</f>
         <v>0</v>
       </c>
       <c r="F28" s="23">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ref="F28:F34" ca="1" si="24">IF(SUBSTITUTE(G28&amp;H28&amp;I28&amp;J28," ","")="",OFFSET(F28,-1,0)+NOT(TRIM(K28)=""),0)</f>
         <v>0</v>
       </c>
       <c r="G28" s="24"/>
@@ -3678,11 +3825,11 @@
       <c r="N28" s="27"/>
       <c r="O28" s="57"/>
       <c r="P28" s="28" t="str">
-        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$33,2,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A28 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$36,2,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A28 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q28" s="28" t="str">
-        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$33,3,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$36,3,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R28" s="33"/>
@@ -3697,27 +3844,27 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A29" s="22" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <f t="shared" ca="1" si="20"/>
+        <v>3-1</v>
       </c>
       <c r="B29" s="32">
         <f>COUNTA($G$1:$G29)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C29" s="23">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>1</v>
       </c>
       <c r="D29" s="23">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="22"/>
         <v>0</v>
       </c>
       <c r="E29" s="23">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="23"/>
         <v>0</v>
       </c>
       <c r="F29" s="23">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="24"/>
         <v>0</v>
       </c>
       <c r="G29" s="24"/>
@@ -3730,11 +3877,11 @@
       <c r="N29" s="27"/>
       <c r="O29" s="57"/>
       <c r="P29" s="28" t="str">
-        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$33,2,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A29 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$36,2,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A29 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q29" s="28" t="str">
-        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$33,3,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$36,3,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R29" s="33"/>
@@ -3749,27 +3896,27 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A30" s="22" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <f t="shared" ca="1" si="20"/>
+        <v>3-1</v>
       </c>
       <c r="B30" s="32">
         <f>COUNTA($G$1:$G30)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C30" s="23">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>1</v>
       </c>
       <c r="D30" s="23">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="22"/>
         <v>0</v>
       </c>
       <c r="E30" s="23">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="23"/>
         <v>0</v>
       </c>
       <c r="F30" s="23">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="24"/>
         <v>0</v>
       </c>
       <c r="G30" s="24"/>
@@ -3782,11 +3929,11 @@
       <c r="N30" s="27"/>
       <c r="O30" s="57"/>
       <c r="P30" s="28" t="str">
-        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$33,2,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A30 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$36,2,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A30 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q30" s="28" t="str">
-        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$33,3,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$36,3,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R30" s="33"/>
@@ -3801,27 +3948,27 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A31" s="22" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <f t="shared" ca="1" si="20"/>
+        <v>3-1</v>
       </c>
       <c r="B31" s="32">
         <f>COUNTA($G$1:$G31)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C31" s="23">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>1</v>
       </c>
       <c r="D31" s="23">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="22"/>
         <v>0</v>
       </c>
       <c r="E31" s="23">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="23"/>
         <v>0</v>
       </c>
       <c r="F31" s="23">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="24"/>
         <v>0</v>
       </c>
       <c r="G31" s="24"/>
@@ -3834,11 +3981,11 @@
       <c r="N31" s="27"/>
       <c r="O31" s="57"/>
       <c r="P31" s="28" t="str">
-        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$33,2,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A31 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$36,2,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A31 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q31" s="28" t="str">
-        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$33,3,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$36,3,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R31" s="33"/>
@@ -3853,27 +4000,27 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A32" s="22" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <f t="shared" ca="1" si="20"/>
+        <v>3-1</v>
       </c>
       <c r="B32" s="32">
         <f>COUNTA($G$1:$G32)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C32" s="23">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>1</v>
       </c>
       <c r="D32" s="23">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="22"/>
         <v>0</v>
       </c>
       <c r="E32" s="23">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="23"/>
         <v>0</v>
       </c>
       <c r="F32" s="23">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="24"/>
         <v>0</v>
       </c>
       <c r="G32" s="24"/>
@@ -3886,11 +4033,11 @@
       <c r="N32" s="27"/>
       <c r="O32" s="57"/>
       <c r="P32" s="28" t="str">
-        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$33,2,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A32 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$36,2,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A32 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q32" s="28" t="str">
-        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$33,3,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$36,3,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R32" s="33"/>
@@ -3905,27 +4052,27 @@
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A33" s="22" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <f t="shared" ca="1" si="20"/>
+        <v>3-1</v>
       </c>
       <c r="B33" s="32">
         <f>COUNTA($G$1:$G33)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C33" s="23">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>1</v>
       </c>
       <c r="D33" s="23">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="22"/>
         <v>0</v>
       </c>
       <c r="E33" s="23">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="23"/>
         <v>0</v>
       </c>
       <c r="F33" s="23">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="24"/>
         <v>0</v>
       </c>
       <c r="G33" s="24"/>
@@ -3938,11 +4085,11 @@
       <c r="N33" s="27"/>
       <c r="O33" s="57"/>
       <c r="P33" s="28" t="str">
-        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$33,2,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A33 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$36,2,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A33 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q33" s="28" t="str">
-        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$33,3,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$36,3,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R33" s="33"/>
@@ -3957,27 +4104,27 @@
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A34" s="22" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <f t="shared" ca="1" si="20"/>
+        <v>3-1</v>
       </c>
       <c r="B34" s="32">
         <f>COUNTA($G$1:$G34)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C34" s="23">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>1</v>
       </c>
       <c r="D34" s="23">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="22"/>
         <v>0</v>
       </c>
       <c r="E34" s="23">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="23"/>
         <v>0</v>
       </c>
       <c r="F34" s="23">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="24"/>
         <v>0</v>
       </c>
       <c r="G34" s="24"/>
@@ -3990,11 +4137,11 @@
       <c r="N34" s="27"/>
       <c r="O34" s="57"/>
       <c r="P34" s="28" t="str">
-        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$33,2,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A34 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$36,2,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A34 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q34" s="28" t="str">
-        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$33,3,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$36,3,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R34" s="33"/>
@@ -4010,15 +4157,15 @@
     <row r="35" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A35" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B35" s="32">
         <f>COUNTA($G$1:$G35)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C35" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D35" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -4042,11 +4189,11 @@
       <c r="N35" s="27"/>
       <c r="O35" s="57"/>
       <c r="P35" s="28" t="str">
-        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$33,2,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A35 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$36,2,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A35 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q35" s="28" t="str">
-        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$33,3,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$36,3,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R35" s="33"/>
@@ -4062,15 +4209,15 @@
     <row r="36" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A36" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B36" s="32">
         <f>COUNTA($G$1:$G36)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C36" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D36" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -4094,11 +4241,11 @@
       <c r="N36" s="27"/>
       <c r="O36" s="57"/>
       <c r="P36" s="28" t="str">
-        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$33,2,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A36 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$36,2,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A36 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q36" s="28" t="str">
-        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$33,3,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$36,3,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R36" s="33"/>
@@ -4114,15 +4261,15 @@
     <row r="37" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A37" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B37" s="32">
         <f>COUNTA($G$1:$G37)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C37" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -4146,11 +4293,11 @@
       <c r="N37" s="27"/>
       <c r="O37" s="57"/>
       <c r="P37" s="28" t="str">
-        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$33,2,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A37 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$36,2,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A37 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q37" s="28" t="str">
-        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$33,3,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$36,3,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R37" s="33"/>
@@ -4166,15 +4313,15 @@
     <row r="38" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A38" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B38" s="32">
         <f>COUNTA($G$1:$G38)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C38" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D38" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -4198,11 +4345,11 @@
       <c r="N38" s="27"/>
       <c r="O38" s="57"/>
       <c r="P38" s="28" t="str">
-        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$33,2,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A38 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$36,2,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A38 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q38" s="28" t="str">
-        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$33,3,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$36,3,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R38" s="33"/>
@@ -4218,15 +4365,15 @@
     <row r="39" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A39" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B39" s="32">
         <f>COUNTA($G$1:$G39)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C39" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -4250,11 +4397,11 @@
       <c r="N39" s="27"/>
       <c r="O39" s="57"/>
       <c r="P39" s="28" t="str">
-        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$33,2,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A39 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$36,2,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A39 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q39" s="28" t="str">
-        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$33,3,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$36,3,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R39" s="33"/>
@@ -4270,15 +4417,15 @@
     <row r="40" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A40" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B40" s="32">
         <f>COUNTA($G$1:$G40)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C40" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -4302,11 +4449,11 @@
       <c r="N40" s="27"/>
       <c r="O40" s="57"/>
       <c r="P40" s="28" t="str">
-        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$33,2,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A40 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$36,2,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A40 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q40" s="28" t="str">
-        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$33,3,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$36,3,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R40" s="33"/>
@@ -4322,15 +4469,15 @@
     <row r="41" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A41" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B41" s="32">
         <f>COUNTA($G$1:$G41)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C41" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D41" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -4354,11 +4501,11 @@
       <c r="N41" s="27"/>
       <c r="O41" s="57"/>
       <c r="P41" s="28" t="str">
-        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$33,2,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A41 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$36,2,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A41 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q41" s="28" t="str">
-        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$33,3,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$36,3,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R41" s="33"/>
@@ -4374,15 +4521,15 @@
     <row r="42" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A42" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B42" s="32">
         <f>COUNTA($G$1:$G42)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C42" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -4406,11 +4553,11 @@
       <c r="N42" s="27"/>
       <c r="O42" s="57"/>
       <c r="P42" s="28" t="str">
-        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$33,2,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A42 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$36,2,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A42 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q42" s="28" t="str">
-        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$33,3,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$36,3,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R42" s="33"/>
@@ -4426,15 +4573,15 @@
     <row r="43" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A43" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B43" s="32">
         <f>COUNTA($G$1:$G43)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C43" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D43" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -4458,11 +4605,11 @@
       <c r="N43" s="27"/>
       <c r="O43" s="57"/>
       <c r="P43" s="28" t="str">
-        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$33,2,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A43 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$36,2,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A43 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q43" s="28" t="str">
-        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$33,3,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$36,3,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R43" s="33"/>
@@ -4478,15 +4625,15 @@
     <row r="44" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A44" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B44" s="32">
         <f>COUNTA($G$1:$G44)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C44" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D44" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -4510,11 +4657,11 @@
       <c r="N44" s="27"/>
       <c r="O44" s="57"/>
       <c r="P44" s="28" t="str">
-        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$33,2,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A44 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$36,2,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A44 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q44" s="28" t="str">
-        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$33,3,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$36,3,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R44" s="33"/>
@@ -4530,15 +4677,15 @@
     <row r="45" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A45" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B45" s="32">
         <f>COUNTA($G$1:$G45)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C45" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D45" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -4562,11 +4709,11 @@
       <c r="N45" s="27"/>
       <c r="O45" s="57"/>
       <c r="P45" s="28" t="str">
-        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$33,2,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A45 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$36,2,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A45 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q45" s="28" t="str">
-        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$33,3,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$36,3,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R45" s="33"/>
@@ -4582,15 +4729,15 @@
     <row r="46" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A46" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B46" s="32">
         <f>COUNTA($G$1:$G46)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C46" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D46" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -4614,11 +4761,11 @@
       <c r="N46" s="27"/>
       <c r="O46" s="57"/>
       <c r="P46" s="28" t="str">
-        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$33,2,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A46 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$36,2,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A46 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q46" s="28" t="str">
-        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$33,3,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$36,3,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R46" s="33"/>
@@ -4634,15 +4781,15 @@
     <row r="47" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A47" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B47" s="32">
         <f>COUNTA($G$1:$G47)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C47" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D47" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -4666,11 +4813,11 @@
       <c r="N47" s="27"/>
       <c r="O47" s="57"/>
       <c r="P47" s="28" t="str">
-        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$33,2,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A47 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$36,2,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A47 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q47" s="28" t="str">
-        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$33,3,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$36,3,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R47" s="33"/>
@@ -4686,15 +4833,15 @@
     <row r="48" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A48" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B48" s="32">
         <f>COUNTA($G$1:$G48)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C48" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D48" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -4718,11 +4865,11 @@
       <c r="N48" s="27"/>
       <c r="O48" s="57"/>
       <c r="P48" s="28" t="str">
-        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$33,2,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A48 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$36,2,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A48 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q48" s="28" t="str">
-        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$33,3,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$36,3,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R48" s="33"/>
@@ -4738,15 +4885,15 @@
     <row r="49" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A49" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B49" s="32">
         <f>COUNTA($G$1:$G49)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C49" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D49" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -4770,11 +4917,11 @@
       <c r="N49" s="27"/>
       <c r="O49" s="57"/>
       <c r="P49" s="28" t="str">
-        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$33,2,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A49 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$36,2,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A49 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q49" s="28" t="str">
-        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$33,3,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$36,3,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R49" s="33"/>
@@ -4790,15 +4937,15 @@
     <row r="50" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A50" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B50" s="32">
         <f>COUNTA($G$1:$G50)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C50" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D50" s="23">
         <f t="shared" ca="1" si="2"/>
@@ -4822,11 +4969,11 @@
       <c r="N50" s="27"/>
       <c r="O50" s="57"/>
       <c r="P50" s="28" t="str">
-        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$33,2,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A50 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$36,2,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A50 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q50" s="28" t="str">
-        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$33,3,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$36,3,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R50" s="33"/>
@@ -4842,15 +4989,15 @@
     <row r="51" spans="1:26" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A51" s="34" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2-2</v>
+        <v>3-1</v>
       </c>
       <c r="B51" s="35">
         <f>COUNTA($G$1:$G51)-1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C51" s="36">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D51" s="36">
         <f t="shared" ca="1" si="2"/>
@@ -4874,11 +5021,11 @@
       <c r="N51" s="40"/>
       <c r="O51" s="60"/>
       <c r="P51" s="41" t="str">
-        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$33,2,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A51 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$36,2,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A51 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q51" s="41" t="str">
-        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$33,3,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$36,3,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R51" s="42"/>
@@ -4920,19 +5067,19 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>
-  <conditionalFormatting sqref="A2:F3 A5:F5 A7:F9 A11:F15 A17:F51">
-    <cfRule type="expression" dxfId="4" priority="6">
+  <conditionalFormatting sqref="A2:F3 A5:F5 A8:F27 A35:F51">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>OR(A2=0, A2=OFFSET(A2,-1,0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A16:F16">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>OR(A16=0, A16=OFFSET(A16,-1,0))</formula>
+  <conditionalFormatting sqref="A4:F4">
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>OR(A4=0, A4=OFFSET(A4,-1,0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:F4">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>OR(A4=0, A4=OFFSET(A4,-1,0))</formula>
+  <conditionalFormatting sqref="A7:F7">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>OR(A7=0, A7=OFFSET(A7,-1,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:F6">
@@ -4940,9 +5087,9 @@
       <formula>OR(A6=0, A6=OFFSET(A6,-1,0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10:F10">
+  <conditionalFormatting sqref="A28:F34">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>OR(A10=0, A10=OFFSET(A10,-1,0))</formula>
+      <formula>OR(A28=0, A28=OFFSET(A28,-1,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -4955,7 +5102,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>data!$A$2:$A$33</xm:f>
+            <xm:f>data!$A$2:$A$36</xm:f>
           </x14:formula1>
           <xm:sqref>N2:N51</xm:sqref>
         </x14:dataValidation>
@@ -4970,7 +5117,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -4988,13 +5135,13 @@
         <v>3</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C1" s="49" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -5002,396 +5149,436 @@
         <v>16</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>101</v>
+        <v>150</v>
       </c>
       <c r="D2" s="50"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="50" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="C3" s="51" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="50" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="C4" s="51" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D4" s="50"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="50" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C5" s="51" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D5" s="50"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="50" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>112</v>
+        <v>145</v>
       </c>
       <c r="C6" s="51" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="D6" s="50"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="50" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" s="50"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="50" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D8" s="50"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="50" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D9" s="50"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="50" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C10" s="51" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D10" s="50"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="50" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C11" s="51" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D11" s="50"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="50" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
       <c r="C12" s="51" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="D12" s="50"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="50" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="C13" s="51" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D13" s="50"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="50" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C14" s="51" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D14" s="50"/>
     </row>
-    <row r="15" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="50" t="s">
-        <v>37</v>
+        <v>153</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>120</v>
+        <v>148</v>
       </c>
       <c r="C15" s="51" t="s">
-        <v>36</v>
+        <v>151</v>
       </c>
       <c r="D15" s="50"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="50" t="s">
-        <v>38</v>
+        <v>154</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
       <c r="C16" s="51" t="s">
-        <v>39</v>
+        <v>152</v>
       </c>
       <c r="D16" s="50"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="50" t="s">
-        <v>106</v>
+        <v>34</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C17" s="51" t="s">
-        <v>107</v>
+        <v>35</v>
       </c>
       <c r="D17" s="50"/>
     </row>
-    <row r="18" spans="1:4" ht="135" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="50" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="C18" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="51" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="54" x14ac:dyDescent="0.15">
+        <v>99</v>
+      </c>
+      <c r="D18" s="50"/>
+    </row>
+    <row r="19" spans="1:4" ht="135" x14ac:dyDescent="0.15">
       <c r="A19" s="50" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="A20" s="50" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="C20" s="51" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="D20" s="51" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="A21" s="50" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C21" s="51" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="A22" s="50" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>70</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="50" t="s">
-        <v>148</v>
+        <v>25</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>149</v>
+        <v>113</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>150</v>
-      </c>
-      <c r="D23" s="51"/>
+        <v>38</v>
+      </c>
+      <c r="D23" s="51" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="50" t="s">
-        <v>43</v>
+        <v>132</v>
       </c>
       <c r="B24" s="51" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="C24" s="51" t="s">
-        <v>44</v>
+        <v>134</v>
       </c>
       <c r="D24" s="51"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="50" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B25" s="51" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C25" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" s="50"/>
+        <v>40</v>
+      </c>
+      <c r="D25" s="51"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="50" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="53" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+        <v>72</v>
+      </c>
+      <c r="D26" s="50"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="50" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" s="50"/>
+        <v>73</v>
+      </c>
+      <c r="D27" s="53" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A28" s="50" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B28" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="50"/>
+    </row>
+    <row r="29" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A29" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="53" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A30" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="53"/>
+    </row>
+    <row r="31" spans="1:4" ht="81" x14ac:dyDescent="0.15">
+      <c r="A31" s="50" t="s">
+        <v>155</v>
+      </c>
+      <c r="B31" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="D31" s="51" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A32" s="50" t="s">
+        <v>156</v>
+      </c>
+      <c r="B32" s="51" t="s">
+        <v>140</v>
+      </c>
+      <c r="C32" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="C28" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" s="53" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="B29" s="51" t="s">
-        <v>131</v>
-      </c>
-      <c r="C29" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="D29" s="53"/>
-    </row>
-    <row r="30" spans="1:4" ht="81" x14ac:dyDescent="0.15">
-      <c r="A30" s="50" t="s">
-        <v>142</v>
-      </c>
-      <c r="B30" s="51" t="s">
-        <v>136</v>
-      </c>
-      <c r="C30" s="51" t="s">
+      <c r="D32" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="D30" s="51" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="27" x14ac:dyDescent="0.15">
-      <c r="A31" s="50" t="s">
-        <v>143</v>
-      </c>
-      <c r="B31" s="51" t="s">
-        <v>156</v>
-      </c>
-      <c r="C31" s="51" t="s">
-        <v>144</v>
-      </c>
-      <c r="D31" s="51" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="52" t="s">
-        <v>154</v>
-      </c>
-      <c r="B32" s="52" t="s">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A33" s="50" t="s">
         <v>157</v>
       </c>
-      <c r="C32" s="64" t="s">
-        <v>155</v>
-      </c>
-      <c r="D32" s="52"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="52"/>
-      <c r="B33" s="52"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="52"/>
+      <c r="B33" s="51" t="s">
+        <v>159</v>
+      </c>
+      <c r="C33" s="51" t="s">
+        <v>161</v>
+      </c>
+      <c r="D33" s="53" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A34" s="50" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="C34" s="51" t="s">
+        <v>162</v>
+      </c>
+      <c r="D34" s="53" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A35" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="52" t="s">
+        <v>141</v>
+      </c>
+      <c r="C35" s="64" t="s">
+        <v>139</v>
+      </c>
+      <c r="D35" s="52"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A36" s="52"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="52"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>
@@ -5404,9 +5591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5415,87 +5600,87 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="48" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" s="48" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" s="48" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" s="48" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" s="48" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" s="48" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" s="48" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" s="48" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" s="48" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" s="48" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" s="48" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" s="48" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="48" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="48" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" s="48" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" s="48" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" s="48" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add exe control command.
</commit_message>
<xml_diff>
--- a/PaperTester.xlsx
+++ b/PaperTester.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="16380" windowHeight="8175" tabRatio="484"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="16380" windowHeight="8160" tabRatio="484"/>
   </bookViews>
   <sheets>
     <sheet name="テスト仕様書" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="174">
   <si>
     <t>No.</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>説明</t>
-  </si>
-  <si>
-    <t>IEを閉じる</t>
   </si>
   <si>
     <t>InternetExplorerを閉じる。</t>
@@ -303,10 +300,6 @@
     <t>tag=input#4</t>
   </si>
   <si>
-    <t>2-2</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>項目「引数の前部分」に値「引数の後部分」を入力する。"%0"</t>
     <rPh sb="6" eb="7">
       <t>マエ</t>
@@ -470,12 +463,6 @@
       <t>カイジョ</t>
     </rPh>
     <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>pt.Open : onErrorExit</t>
-  </si>
-  <si>
-    <t>pt.Close : onErrorExit</t>
   </si>
   <si>
     <t>pt.GoBack : onErrorExit</t>
@@ -933,10 +920,6 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>pt.Run "%0" : onErrorExit</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>EXEを実行する。</t>
     <rPh sb="4" eb="6">
       <t>ジッコウ</t>
@@ -944,13 +927,6 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>EXEを実行する</t>
-    <rPh sb="4" eb="6">
-      <t>ジッコウ</t>
-    </rPh>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>pt.ActivateNextIE : onErrorExit</t>
     <phoneticPr fontId="5"/>
   </si>
@@ -1168,6 +1144,58 @@
     </rPh>
     <rPh sb="37" eb="38">
       <t>コト</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>pt.OpenIE : onErrorExit</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>IE/EXEを閉じる</t>
+  </si>
+  <si>
+    <t>IE/EXEを閉じる</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>pt.Run "%0" : onErrorExit</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>pt.Quit : onErrorExit</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>EXEを起動する</t>
+    <rPh sb="4" eb="6">
+      <t>キドウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>notepad.exe</t>
+  </si>
+  <si>
+    <t>%(FNN)</t>
+  </si>
+  <si>
+    <t>【終了】メモ帳を開き直しました。</t>
+  </si>
+  <si>
+    <t>3-1</t>
+  </si>
+  <si>
+    <t>{ENTER}</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>【開始】任意のEXEをキー操作できます。</t>
+    <rPh sb="4" eb="6">
+      <t>ニンイ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ソウサ</t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -1816,42 +1844,49 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FFF2F2F2"/>
+        <name val="ＭＳ Ｐゴシック"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <sz val="11"/>
@@ -2261,7 +2296,7 @@
       <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P19" sqref="P2:P19"/>
+      <selection pane="bottomRight" activeCell="P32" sqref="P2:P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2272,7 +2307,7 @@
     <col min="12" max="12" width="9.5" customWidth="1"/>
     <col min="13" max="13" width="27.5"/>
     <col min="14" max="14" width="39.75" style="1"/>
-    <col min="15" max="15" width="36.875" style="62" customWidth="1"/>
+    <col min="15" max="15" width="36.875" style="56" customWidth="1"/>
     <col min="16" max="16" width="49" style="1" customWidth="1"/>
     <col min="17" max="17" width="54.125"/>
     <col min="18" max="18" width="26.5"/>
@@ -2309,7 +2344,7 @@
         <v>3</v>
       </c>
       <c r="O1" s="54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P1" s="7" t="s">
         <v>4</v>
@@ -2381,10 +2416,10 @@
       <c r="N2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="55"/>
+      <c r="O2" s="58"/>
       <c r="P2" s="16" t="str">
         <f ca="1">IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$36,2,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A2 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.Open : onErrorExit "テストケース = 1, Excel行 = 2"</v>
+        <v>pt.OpenIE : onErrorExit "テストケース = 1, Excel行 = 2"</v>
       </c>
       <c r="Q2" s="16" t="str">
         <f>IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$36,3,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
@@ -2449,7 +2484,7 @@
       <c r="N3" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="56" t="s">
+      <c r="O3" s="59" t="s">
         <v>22</v>
       </c>
       <c r="P3" s="28" t="str">
@@ -2503,9 +2538,9 @@
       <c r="L4" s="26"/>
       <c r="M4" s="26"/>
       <c r="N4" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="O4" s="57"/>
+        <v>81</v>
+      </c>
+      <c r="O4" s="60"/>
       <c r="P4" s="28" t="str">
         <f ca="1">IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$36,2,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A4 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.MaximumWindow : onErrorExit "テストケース = 1, Excel行 = 4"</v>
@@ -2557,9 +2592,9 @@
       <c r="L5" s="26"/>
       <c r="M5" s="26"/>
       <c r="N5" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="O5" s="57" t="str">
+        <v>41</v>
+      </c>
+      <c r="O5" s="60" t="str">
         <f ca="1">A5</f>
         <v>1</v>
       </c>
@@ -2614,10 +2649,10 @@
       <c r="L6" s="26"/>
       <c r="M6" s="26"/>
       <c r="N6" s="27" t="s">
-        <v>158</v>
-      </c>
-      <c r="O6" s="57" t="s">
-        <v>166</v>
+        <v>152</v>
+      </c>
+      <c r="O6" s="60" t="s">
+        <v>160</v>
       </c>
       <c r="P6" s="28" t="str">
         <f ca="1">IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$36,2,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A6 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
@@ -2670,10 +2705,10 @@
       <c r="L7" s="26"/>
       <c r="M7" s="26"/>
       <c r="N7" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="O7" s="58" t="s">
-        <v>131</v>
+        <v>150</v>
+      </c>
+      <c r="O7" s="61" t="s">
+        <v>127</v>
       </c>
       <c r="P7" s="28" t="str">
         <f ca="1">IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$36,2,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A7 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
@@ -2711,10 +2746,10 @@
       <c r="L8" s="26"/>
       <c r="M8" s="26"/>
       <c r="N8" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="O8" s="57" t="s">
-        <v>71</v>
+        <v>67</v>
+      </c>
+      <c r="O8" s="60" t="s">
+        <v>70</v>
       </c>
       <c r="P8" s="28" t="str">
         <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$36,2,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A8 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
@@ -2769,7 +2804,7 @@
       <c r="L9" s="26"/>
       <c r="M9" s="26"/>
       <c r="N9" s="27"/>
-      <c r="O9" s="58"/>
+      <c r="O9" s="61"/>
       <c r="P9" s="28" t="str">
         <f>IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$36,2,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A9 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -2829,20 +2864,20 @@
       </c>
       <c r="G10" s="24"/>
       <c r="H10" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I10" s="25"/>
       <c r="J10" s="25"/>
       <c r="K10" s="25"/>
       <c r="L10" s="26"/>
       <c r="M10" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N10" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="O10" s="58" t="s">
-        <v>123</v>
+        <v>61</v>
+      </c>
+      <c r="O10" s="61" t="s">
+        <v>119</v>
       </c>
       <c r="P10" s="28" t="str">
         <f ca="1">IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$36,2,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A10 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
@@ -2909,18 +2944,19 @@
       <c r="L11" s="26"/>
       <c r="M11" s="26"/>
       <c r="N11" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="O11" s="63" t="s">
-        <v>79</v>
+        <v>40</v>
+      </c>
+      <c r="O11" s="62" t="str">
+        <f ca="1">A10</f>
+        <v>2-1</v>
       </c>
       <c r="P11" s="28" t="str">
         <f ca="1">IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$36,2,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A11 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.FullScreenShot "2-2" : onErrorExit "テストケース = 2-1, Excel行 = 11"</v>
+        <v>pt.FullScreenShot "2-1" : onErrorExit "テストケース = 2-1, Excel行 = 11"</v>
       </c>
       <c r="Q11" s="28" t="str">
-        <f>IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$36,3,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>スクリーンショットを撮る。（画面全体, コメント："2-2"）</v>
+        <f ca="1">IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$36,3,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <v>スクリーンショットを撮る。（画面全体, コメント："2-1"）</v>
       </c>
       <c r="R11" s="33"/>
       <c r="S11" s="30"/>
@@ -2967,8 +3003,8 @@
       <c r="N12" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="O12" s="57" t="s">
-        <v>78</v>
+      <c r="O12" s="60" t="s">
+        <v>77</v>
       </c>
       <c r="P12" s="28" t="str">
         <f ca="1">IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$36,2,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A12 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
@@ -3021,9 +3057,9 @@
       <c r="L13" s="26"/>
       <c r="M13" s="26"/>
       <c r="N13" s="27" t="s">
-        <v>153</v>
-      </c>
-      <c r="O13" s="57"/>
+        <v>147</v>
+      </c>
+      <c r="O13" s="60"/>
       <c r="P13" s="28" t="str">
         <f ca="1">IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$36,2,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A13 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.ActivateNextIE : onErrorExit "テストケース = 2-1, Excel行 = 13"</v>
@@ -3075,9 +3111,9 @@
       <c r="L14" s="26"/>
       <c r="M14" s="26"/>
       <c r="N14" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="O14" s="57"/>
+        <v>40</v>
+      </c>
+      <c r="O14" s="60"/>
       <c r="P14" s="28" t="str">
         <f ca="1">IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$36,2,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A14 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.FullScreenShot "" : onErrorExit "テストケース = 2-1, Excel行 = 14"</v>
@@ -3129,10 +3165,10 @@
       <c r="L15" s="26"/>
       <c r="M15" s="26"/>
       <c r="N15" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="O15" s="59" t="s">
-        <v>120</v>
+        <v>67</v>
+      </c>
+      <c r="O15" s="63" t="s">
+        <v>116</v>
       </c>
       <c r="P15" s="28" t="str">
         <f ca="1">IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$36,2,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A15 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
@@ -3178,7 +3214,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H16" s="25"/>
       <c r="I16" s="25"/>
@@ -3187,7 +3223,7 @@
       <c r="L16" s="26"/>
       <c r="M16" s="26"/>
       <c r="N16" s="27"/>
-      <c r="O16" s="57"/>
+      <c r="O16" s="60"/>
       <c r="P16" s="28" t="str">
         <f>IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$36,2,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A16 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -3233,22 +3269,22 @@
       </c>
       <c r="G17" s="24"/>
       <c r="H17" s="25" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I17" s="25"/>
       <c r="J17" s="25"/>
       <c r="K17" s="25"/>
       <c r="L17" s="26"/>
       <c r="M17" s="26" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="N17" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="O17" s="57"/>
+        <v>163</v>
+      </c>
+      <c r="O17" s="60"/>
       <c r="P17" s="28" t="str">
         <f ca="1">IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$36,2,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A17 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.Close : onErrorExit "テストケース = 3-1, Excel行 = 17"</v>
+        <v>pt.Quit : onErrorExit "テストケース = 3-1, Excel行 = 17"</v>
       </c>
       <c r="Q17" s="28" t="str">
         <f>IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$36,3,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
@@ -3297,18 +3333,18 @@
       <c r="L18" s="26"/>
       <c r="M18" s="26"/>
       <c r="N18" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="O18" s="57" t="s">
-        <v>142</v>
+        <v>167</v>
+      </c>
+      <c r="O18" s="60" t="s">
+        <v>168</v>
       </c>
       <c r="P18" s="28" t="str">
         <f ca="1">IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$36,2,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A18 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.ExecuteJS "alert('任意のJavascriptを実行できます。')" : onErrorExit "テストケース = 3-1, Excel行 = 18"</v>
+        <v>pt.Run "notepad.exe" : onErrorExit "テストケース = 3-1, Excel行 = 18"</v>
       </c>
       <c r="Q18" s="28" t="str">
         <f>IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$36,3,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>Javascriptコード「alert('任意のJavascriptを実行できます。')」を実行する。</v>
+        <v>EXEを実行する。</v>
       </c>
       <c r="R18" s="33"/>
       <c r="S18" s="30"/>
@@ -3320,7 +3356,7 @@
       <c r="Y18" s="25"/>
       <c r="Z18" s="21"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:26" ht="27" x14ac:dyDescent="0.15">
       <c r="A19" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>3-1</v>
@@ -3353,16 +3389,16 @@
       <c r="L19" s="26"/>
       <c r="M19" s="26"/>
       <c r="N19" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="O19" s="57"/>
+        <v>81</v>
+      </c>
+      <c r="O19" s="60"/>
       <c r="P19" s="28" t="str">
         <f ca="1">IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$36,2,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A19 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v>pt.Close : onErrorExit "テストケース = 3-1, Excel行 = 19"</v>
+        <v>pt.MaximumWindow : onErrorExit "テストケース = 3-1, Excel行 = 19"</v>
       </c>
       <c r="Q19" s="28" t="str">
         <f>IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$36,3,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v>InternetExplorerを閉じる。</v>
+        <v>InternetExplorerを最大化する。</v>
       </c>
       <c r="R19" s="33"/>
       <c r="S19" s="30"/>
@@ -3406,15 +3442,19 @@
       <c r="K20" s="25"/>
       <c r="L20" s="26"/>
       <c r="M20" s="26"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="57"/>
+      <c r="N20" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="O20" s="60" t="s">
+        <v>173</v>
+      </c>
       <c r="P20" s="28" t="str">
-        <f>IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$36,2,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A20 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v/>
+        <f ca="1">IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$36,2,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A20 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.Paste "【開始】任意のEXEをキー操作できます。" : onErrorExit "テストケース = 3-1, Excel行 = 20"</v>
       </c>
       <c r="Q20" s="28" t="str">
         <f>IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$36,3,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
+        <v>アクティブ画面へ「【開始】任意のEXEをキー操作できます。」を貼り付ける。</v>
       </c>
       <c r="R20" s="33"/>
       <c r="S20" s="30"/>
@@ -3458,15 +3498,19 @@
       <c r="K21" s="25"/>
       <c r="L21" s="26"/>
       <c r="M21" s="26"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="57"/>
+      <c r="N21" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="O21" s="60" t="s">
+        <v>171</v>
+      </c>
       <c r="P21" s="28" t="str">
-        <f>IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$36,2,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A21 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v/>
+        <f ca="1">IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$36,2,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A21 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.FullScreenShot4VisibleArea "3-1" : onErrorExit "テストケース = 3-1, Excel行 = 21"</v>
       </c>
       <c r="Q21" s="28" t="str">
         <f>IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$36,3,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
+        <v>スクリーンショットを撮る。（画面全体, 表示箇所のみ, コメント："3-1"）</v>
       </c>
       <c r="R21" s="33"/>
       <c r="S21" s="30"/>
@@ -3478,7 +3522,7 @@
       <c r="Y21" s="25"/>
       <c r="Z21" s="21"/>
     </row>
-    <row r="22" spans="1:26" ht="27" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A22" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>3-1</v>
@@ -3510,15 +3554,19 @@
       <c r="K22" s="25"/>
       <c r="L22" s="26"/>
       <c r="M22" s="26"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="57"/>
+      <c r="N22" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="O22" s="60">
+        <v>1</v>
+      </c>
       <c r="P22" s="28" t="str">
-        <f>IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$36,2,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A22 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v/>
+        <f ca="1">IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$36,2,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A22 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.Sleep 1 : onErrorExit "テストケース = 3-1, Excel行 = 22"</v>
       </c>
       <c r="Q22" s="28" t="str">
         <f>IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$36,3,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
+        <v>プログラムを「1」秒停止する</v>
       </c>
       <c r="R22" s="33"/>
       <c r="S22" s="30"/>
@@ -3530,7 +3578,7 @@
       <c r="Y22" s="25"/>
       <c r="Z22" s="21"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:26" ht="27" x14ac:dyDescent="0.15">
       <c r="A23" s="22" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>3-1</v>
@@ -3562,15 +3610,19 @@
       <c r="K23" s="25"/>
       <c r="L23" s="26"/>
       <c r="M23" s="26"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="57"/>
+      <c r="N23" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="O23" s="60" t="s">
+        <v>169</v>
+      </c>
       <c r="P23" s="28" t="str">
-        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$36,2,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A23 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v/>
+        <f ca="1">IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$36,2,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A23 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.SendKeys "%(FNN)" : onErrorExit "テストケース = 3-1, Excel行 = 23"</v>
       </c>
       <c r="Q23" s="28" t="str">
         <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$36,3,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
+        <v>アクティブ画面へ「%(FNN)」をキー入力する。</v>
       </c>
       <c r="R23" s="33"/>
       <c r="S23" s="30"/>
@@ -3582,9 +3634,9 @@
       <c r="Y23" s="25"/>
       <c r="Z23" s="21"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:26" ht="27" x14ac:dyDescent="0.15">
       <c r="A24" s="22" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="A24:A34" ca="1" si="20">IF(B24,B24,"")&amp;IF(C24,"-"&amp;C24,"")&amp;IF(D24,"-"&amp;D24,"")&amp;IF(E24,"-"&amp;E24,"")&amp;IF(F24,"-"&amp;F24,"")</f>
         <v>3-1</v>
       </c>
       <c r="B24" s="32">
@@ -3592,19 +3644,19 @@
         <v>3</v>
       </c>
       <c r="C24" s="23">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ref="C24:C34" ca="1" si="21">IF(TRIM(G24)="",OFFSET(C24,-1,0)+NOT(TRIM(H24)=""),0)</f>
         <v>1</v>
       </c>
       <c r="D24" s="23">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ref="D24:D34" ca="1" si="22">IF(SUBSTITUTE(G24&amp;H24," ","")="",OFFSET(D24,-1,0)+NOT(TRIM(I24)=""),0)</f>
         <v>0</v>
       </c>
       <c r="E24" s="23">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ref="E24:E34" ca="1" si="23">IF(SUBSTITUTE(G24&amp;H24&amp;I24," ","")="",OFFSET(E24,-1,0)+NOT(TRIM(J24)=""),0)</f>
         <v>0</v>
       </c>
       <c r="F24" s="23">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ref="F24:F34" ca="1" si="24">IF(SUBSTITUTE(G24&amp;H24&amp;I24&amp;J24," ","")="",OFFSET(F24,-1,0)+NOT(TRIM(K24)=""),0)</f>
         <v>0</v>
       </c>
       <c r="G24" s="24"/>
@@ -3614,15 +3666,19 @@
       <c r="K24" s="25"/>
       <c r="L24" s="26"/>
       <c r="M24" s="26"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="57"/>
+      <c r="N24" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="O24" s="60" t="s">
+        <v>170</v>
+      </c>
       <c r="P24" s="28" t="str">
-        <f>IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$36,2,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A24 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v/>
+        <f ca="1">IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$36,2,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A24 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.Paste "【終了】メモ帳を開き直しました。" : onErrorExit "テストケース = 3-1, Excel行 = 24"</v>
       </c>
       <c r="Q24" s="28" t="str">
         <f>IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$36,3,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
+        <v>アクティブ画面へ「【終了】メモ帳を開き直しました。」を貼り付ける。</v>
       </c>
       <c r="R24" s="33"/>
       <c r="S24" s="30"/>
@@ -3634,9 +3690,9 @@
       <c r="Y24" s="25"/>
       <c r="Z24" s="21"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:26" ht="27" x14ac:dyDescent="0.15">
       <c r="A25" s="22" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="20"/>
         <v>3-1</v>
       </c>
       <c r="B25" s="32">
@@ -3644,19 +3700,19 @@
         <v>3</v>
       </c>
       <c r="C25" s="23">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1</v>
       </c>
       <c r="D25" s="23">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="22"/>
         <v>0</v>
       </c>
       <c r="E25" s="23">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="23"/>
         <v>0</v>
       </c>
       <c r="F25" s="23">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="24"/>
         <v>0</v>
       </c>
       <c r="G25" s="24"/>
@@ -3666,15 +3722,17 @@
       <c r="K25" s="25"/>
       <c r="L25" s="26"/>
       <c r="M25" s="26"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="57"/>
+      <c r="N25" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="O25" s="60"/>
       <c r="P25" s="28" t="str">
-        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$36,2,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A25 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v/>
+        <f ca="1">IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$36,2,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A25 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.FullScreenShot4VisibleArea "" : onErrorExit "テストケース = 3-1, Excel行 = 25"</v>
       </c>
       <c r="Q25" s="28" t="str">
         <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$36,3,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
+        <v>スクリーンショットを撮る。（画面全体, 表示箇所のみ, コメント：""）</v>
       </c>
       <c r="R25" s="33"/>
       <c r="S25" s="30"/>
@@ -3688,7 +3746,7 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A26" s="22" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="20"/>
         <v>3-1</v>
       </c>
       <c r="B26" s="32">
@@ -3696,19 +3754,19 @@
         <v>3</v>
       </c>
       <c r="C26" s="23">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1</v>
       </c>
       <c r="D26" s="23">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="22"/>
         <v>0</v>
       </c>
       <c r="E26" s="23">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="23"/>
         <v>0</v>
       </c>
       <c r="F26" s="23">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="24"/>
         <v>0</v>
       </c>
       <c r="G26" s="24"/>
@@ -3718,15 +3776,19 @@
       <c r="K26" s="25"/>
       <c r="L26" s="26"/>
       <c r="M26" s="26"/>
-      <c r="N26" s="27"/>
-      <c r="O26" s="57"/>
+      <c r="N26" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="O26" s="60">
+        <v>1</v>
+      </c>
       <c r="P26" s="28" t="str">
-        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$36,2,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A26 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v/>
+        <f ca="1">IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$36,2,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A26 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.Sleep 1 : onErrorExit "テストケース = 3-1, Excel行 = 26"</v>
       </c>
       <c r="Q26" s="28" t="str">
         <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$36,3,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
+        <v>プログラムを「1」秒停止する</v>
       </c>
       <c r="R26" s="33"/>
       <c r="S26" s="30"/>
@@ -3740,7 +3802,7 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A27" s="22" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="20"/>
         <v>3-1</v>
       </c>
       <c r="B27" s="32">
@@ -3748,19 +3810,19 @@
         <v>3</v>
       </c>
       <c r="C27" s="23">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1</v>
       </c>
       <c r="D27" s="23">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="22"/>
         <v>0</v>
       </c>
       <c r="E27" s="23">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="23"/>
         <v>0</v>
       </c>
       <c r="F27" s="23">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="24"/>
         <v>0</v>
       </c>
       <c r="G27" s="24"/>
@@ -3770,15 +3832,17 @@
       <c r="K27" s="25"/>
       <c r="L27" s="26"/>
       <c r="M27" s="26"/>
-      <c r="N27" s="27"/>
-      <c r="O27" s="57"/>
+      <c r="N27" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="O27" s="60"/>
       <c r="P27" s="28" t="str">
-        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$36,2,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A27 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v/>
+        <f ca="1">IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$36,2,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A27 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.Quit : onErrorExit "テストケース = 3-1, Excel行 = 27"</v>
       </c>
       <c r="Q27" s="28" t="str">
         <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$36,3,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
+        <v>InternetExplorerを閉じる。</v>
       </c>
       <c r="R27" s="33"/>
       <c r="S27" s="30"/>
@@ -3792,7 +3856,7 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A28" s="22" t="str">
-        <f t="shared" ref="A28:A34" ca="1" si="20">IF(B28,B28,"")&amp;IF(C28,"-"&amp;C28,"")&amp;IF(D28,"-"&amp;D28,"")&amp;IF(E28,"-"&amp;E28,"")&amp;IF(F28,"-"&amp;F28,"")</f>
+        <f ca="1">IF(B28,B28,"")&amp;IF(C28,"-"&amp;C28,"")&amp;IF(D28,"-"&amp;D28,"")&amp;IF(E28,"-"&amp;E28,"")&amp;IF(F28,"-"&amp;F28,"")</f>
         <v>3-1</v>
       </c>
       <c r="B28" s="32">
@@ -3800,19 +3864,19 @@
         <v>3</v>
       </c>
       <c r="C28" s="23">
-        <f t="shared" ref="C28:C34" ca="1" si="21">IF(TRIM(G28)="",OFFSET(C28,-1,0)+NOT(TRIM(H28)=""),0)</f>
+        <f ca="1">IF(TRIM(G28)="",OFFSET(C28,-1,0)+NOT(TRIM(H28)=""),0)</f>
         <v>1</v>
       </c>
       <c r="D28" s="23">
-        <f t="shared" ref="D28:D34" ca="1" si="22">IF(SUBSTITUTE(G28&amp;H28," ","")="",OFFSET(D28,-1,0)+NOT(TRIM(I28)=""),0)</f>
+        <f ca="1">IF(SUBSTITUTE(G28&amp;H28," ","")="",OFFSET(D28,-1,0)+NOT(TRIM(I28)=""),0)</f>
         <v>0</v>
       </c>
       <c r="E28" s="23">
-        <f t="shared" ref="E28:E34" ca="1" si="23">IF(SUBSTITUTE(G28&amp;H28&amp;I28," ","")="",OFFSET(E28,-1,0)+NOT(TRIM(J28)=""),0)</f>
+        <f ca="1">IF(SUBSTITUTE(G28&amp;H28&amp;I28," ","")="",OFFSET(E28,-1,0)+NOT(TRIM(J28)=""),0)</f>
         <v>0</v>
       </c>
       <c r="F28" s="23">
-        <f t="shared" ref="F28:F34" ca="1" si="24">IF(SUBSTITUTE(G28&amp;H28&amp;I28&amp;J28," ","")="",OFFSET(F28,-1,0)+NOT(TRIM(K28)=""),0)</f>
+        <f ca="1">IF(SUBSTITUTE(G28&amp;H28&amp;I28&amp;J28," ","")="",OFFSET(F28,-1,0)+NOT(TRIM(K28)=""),0)</f>
         <v>0</v>
       </c>
       <c r="G28" s="24"/>
@@ -3822,15 +3886,19 @@
       <c r="K28" s="25"/>
       <c r="L28" s="26"/>
       <c r="M28" s="26"/>
-      <c r="N28" s="27"/>
-      <c r="O28" s="57"/>
+      <c r="N28" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="O28" s="60">
+        <v>1</v>
+      </c>
       <c r="P28" s="28" t="str">
-        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$36,2,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A28 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v/>
+        <f ca="1">IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$36,2,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A28 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.Sleep 1 : onErrorExit "テストケース = 3-1, Excel行 = 28"</v>
       </c>
       <c r="Q28" s="28" t="str">
         <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$36,3,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
+        <v>プログラムを「1」秒停止する</v>
       </c>
       <c r="R28" s="33"/>
       <c r="S28" s="30"/>
@@ -3842,9 +3910,9 @@
       <c r="Y28" s="25"/>
       <c r="Z28" s="21"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:26" ht="27" x14ac:dyDescent="0.15">
       <c r="A29" s="22" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(B29,B29,"")&amp;IF(C29,"-"&amp;C29,"")&amp;IF(D29,"-"&amp;D29,"")&amp;IF(E29,"-"&amp;E29,"")&amp;IF(F29,"-"&amp;F29,"")</f>
         <v>3-1</v>
       </c>
       <c r="B29" s="32">
@@ -3852,19 +3920,19 @@
         <v>3</v>
       </c>
       <c r="C29" s="23">
-        <f t="shared" ca="1" si="21"/>
+        <f ca="1">IF(TRIM(G29)="",OFFSET(C29,-1,0)+NOT(TRIM(H29)=""),0)</f>
         <v>1</v>
       </c>
       <c r="D29" s="23">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(SUBSTITUTE(G29&amp;H29," ","")="",OFFSET(D29,-1,0)+NOT(TRIM(I29)=""),0)</f>
         <v>0</v>
       </c>
       <c r="E29" s="23">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(SUBSTITUTE(G29&amp;H29&amp;I29," ","")="",OFFSET(E29,-1,0)+NOT(TRIM(J29)=""),0)</f>
         <v>0</v>
       </c>
       <c r="F29" s="23">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(SUBSTITUTE(G29&amp;H29&amp;I29&amp;J29," ","")="",OFFSET(F29,-1,0)+NOT(TRIM(K29)=""),0)</f>
         <v>0</v>
       </c>
       <c r="G29" s="24"/>
@@ -3874,15 +3942,19 @@
       <c r="K29" s="25"/>
       <c r="L29" s="26"/>
       <c r="M29" s="26"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="57"/>
+      <c r="N29" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="O29" s="60" t="s">
+        <v>138</v>
+      </c>
       <c r="P29" s="28" t="str">
-        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$36,2,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A29 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v/>
+        <f ca="1">IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$36,2,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A29 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.ExecuteJS "alert('任意のJavascriptを実行できます。')" : onErrorExit "テストケース = 3-1, Excel行 = 29"</v>
       </c>
       <c r="Q29" s="28" t="str">
         <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$36,3,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
+        <v>Javascriptコード「alert('任意のJavascriptを実行できます。')」を実行する。</v>
       </c>
       <c r="R29" s="33"/>
       <c r="S29" s="30"/>
@@ -3896,7 +3968,7 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A30" s="22" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(B30,B30,"")&amp;IF(C30,"-"&amp;C30,"")&amp;IF(D30,"-"&amp;D30,"")&amp;IF(E30,"-"&amp;E30,"")&amp;IF(F30,"-"&amp;F30,"")</f>
         <v>3-1</v>
       </c>
       <c r="B30" s="32">
@@ -3904,19 +3976,19 @@
         <v>3</v>
       </c>
       <c r="C30" s="23">
-        <f t="shared" ca="1" si="21"/>
+        <f ca="1">IF(TRIM(G30)="",OFFSET(C30,-1,0)+NOT(TRIM(H30)=""),0)</f>
         <v>1</v>
       </c>
       <c r="D30" s="23">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(SUBSTITUTE(G30&amp;H30," ","")="",OFFSET(D30,-1,0)+NOT(TRIM(I30)=""),0)</f>
         <v>0</v>
       </c>
       <c r="E30" s="23">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(SUBSTITUTE(G30&amp;H30&amp;I30," ","")="",OFFSET(E30,-1,0)+NOT(TRIM(J30)=""),0)</f>
         <v>0</v>
       </c>
       <c r="F30" s="23">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(SUBSTITUTE(G30&amp;H30&amp;I30&amp;J30," ","")="",OFFSET(F30,-1,0)+NOT(TRIM(K30)=""),0)</f>
         <v>0</v>
       </c>
       <c r="G30" s="24"/>
@@ -3926,15 +3998,19 @@
       <c r="K30" s="25"/>
       <c r="L30" s="26"/>
       <c r="M30" s="26"/>
-      <c r="N30" s="27"/>
-      <c r="O30" s="57"/>
+      <c r="N30" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="O30" s="60">
+        <v>1</v>
+      </c>
       <c r="P30" s="28" t="str">
-        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$36,2,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A30 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v/>
+        <f ca="1">IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$36,2,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A30 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.Sleep 1 : onErrorExit "テストケース = 3-1, Excel行 = 30"</v>
       </c>
       <c r="Q30" s="28" t="str">
         <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$36,3,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
+        <v>プログラムを「1」秒停止する</v>
       </c>
       <c r="R30" s="33"/>
       <c r="S30" s="30"/>
@@ -3946,9 +4022,9 @@
       <c r="Y30" s="25"/>
       <c r="Z30" s="21"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:26" ht="27" x14ac:dyDescent="0.15">
       <c r="A31" s="22" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(B31,B31,"")&amp;IF(C31,"-"&amp;C31,"")&amp;IF(D31,"-"&amp;D31,"")&amp;IF(E31,"-"&amp;E31,"")&amp;IF(F31,"-"&amp;F31,"")</f>
         <v>3-1</v>
       </c>
       <c r="B31" s="32">
@@ -3956,19 +4032,19 @@
         <v>3</v>
       </c>
       <c r="C31" s="23">
-        <f t="shared" ca="1" si="21"/>
+        <f ca="1">IF(TRIM(G31)="",OFFSET(C31,-1,0)+NOT(TRIM(H31)=""),0)</f>
         <v>1</v>
       </c>
       <c r="D31" s="23">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(SUBSTITUTE(G31&amp;H31," ","")="",OFFSET(D31,-1,0)+NOT(TRIM(I31)=""),0)</f>
         <v>0</v>
       </c>
       <c r="E31" s="23">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(SUBSTITUTE(G31&amp;H31&amp;I31," ","")="",OFFSET(E31,-1,0)+NOT(TRIM(J31)=""),0)</f>
         <v>0</v>
       </c>
       <c r="F31" s="23">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(SUBSTITUTE(G31&amp;H31&amp;I31&amp;J31," ","")="",OFFSET(F31,-1,0)+NOT(TRIM(K31)=""),0)</f>
         <v>0</v>
       </c>
       <c r="G31" s="24"/>
@@ -3978,15 +4054,19 @@
       <c r="K31" s="25"/>
       <c r="L31" s="26"/>
       <c r="M31" s="26"/>
-      <c r="N31" s="27"/>
-      <c r="O31" s="57"/>
+      <c r="N31" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="O31" s="60" t="s">
+        <v>172</v>
+      </c>
       <c r="P31" s="28" t="str">
-        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$36,2,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A31 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v/>
+        <f ca="1">IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$36,2,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A31 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.SendKeys "{ENTER}" : onErrorExit "テストケース = 3-1, Excel行 = 31"</v>
       </c>
       <c r="Q31" s="28" t="str">
         <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$36,3,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
+        <v>アクティブ画面へ「{ENTER}」をキー入力する。</v>
       </c>
       <c r="R31" s="33"/>
       <c r="S31" s="30"/>
@@ -4030,15 +4110,17 @@
       <c r="K32" s="25"/>
       <c r="L32" s="26"/>
       <c r="M32" s="26"/>
-      <c r="N32" s="27"/>
-      <c r="O32" s="57"/>
+      <c r="N32" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="O32" s="60"/>
       <c r="P32" s="28" t="str">
-        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$36,2,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A32 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
-        <v/>
+        <f ca="1">IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$36,2,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A32 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <v>pt.Quit : onErrorExit "テストケース = 3-1, Excel行 = 32"</v>
       </c>
       <c r="Q32" s="28" t="str">
         <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$36,3,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
-        <v/>
+        <v>InternetExplorerを閉じる。</v>
       </c>
       <c r="R32" s="33"/>
       <c r="S32" s="30"/>
@@ -4083,7 +4165,7 @@
       <c r="L33" s="26"/>
       <c r="M33" s="26"/>
       <c r="N33" s="27"/>
-      <c r="O33" s="57"/>
+      <c r="O33" s="60"/>
       <c r="P33" s="28" t="str">
         <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$36,2,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A33 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -4135,7 +4217,7 @@
       <c r="L34" s="26"/>
       <c r="M34" s="26"/>
       <c r="N34" s="27"/>
-      <c r="O34" s="57"/>
+      <c r="O34" s="60"/>
       <c r="P34" s="28" t="str">
         <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$36,2,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A34 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -4187,7 +4269,7 @@
       <c r="L35" s="26"/>
       <c r="M35" s="26"/>
       <c r="N35" s="27"/>
-      <c r="O35" s="57"/>
+      <c r="O35" s="60"/>
       <c r="P35" s="28" t="str">
         <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$36,2,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A35 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -4239,7 +4321,7 @@
       <c r="L36" s="26"/>
       <c r="M36" s="26"/>
       <c r="N36" s="27"/>
-      <c r="O36" s="57"/>
+      <c r="O36" s="60"/>
       <c r="P36" s="28" t="str">
         <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$36,2,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A36 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -4291,7 +4373,7 @@
       <c r="L37" s="26"/>
       <c r="M37" s="26"/>
       <c r="N37" s="27"/>
-      <c r="O37" s="57"/>
+      <c r="O37" s="60"/>
       <c r="P37" s="28" t="str">
         <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$36,2,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A37 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -4343,7 +4425,7 @@
       <c r="L38" s="26"/>
       <c r="M38" s="26"/>
       <c r="N38" s="27"/>
-      <c r="O38" s="57"/>
+      <c r="O38" s="60"/>
       <c r="P38" s="28" t="str">
         <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$36,2,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A38 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -4395,7 +4477,7 @@
       <c r="L39" s="26"/>
       <c r="M39" s="26"/>
       <c r="N39" s="27"/>
-      <c r="O39" s="57"/>
+      <c r="O39" s="60"/>
       <c r="P39" s="28" t="str">
         <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$36,2,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A39 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -4447,7 +4529,7 @@
       <c r="L40" s="26"/>
       <c r="M40" s="26"/>
       <c r="N40" s="27"/>
-      <c r="O40" s="57"/>
+      <c r="O40" s="60"/>
       <c r="P40" s="28" t="str">
         <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$36,2,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A40 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -4499,7 +4581,7 @@
       <c r="L41" s="26"/>
       <c r="M41" s="26"/>
       <c r="N41" s="27"/>
-      <c r="O41" s="57"/>
+      <c r="O41" s="60"/>
       <c r="P41" s="28" t="str">
         <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$36,2,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A41 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -4551,7 +4633,7 @@
       <c r="L42" s="26"/>
       <c r="M42" s="26"/>
       <c r="N42" s="27"/>
-      <c r="O42" s="57"/>
+      <c r="O42" s="60"/>
       <c r="P42" s="28" t="str">
         <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$36,2,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A42 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -4603,7 +4685,7 @@
       <c r="L43" s="26"/>
       <c r="M43" s="26"/>
       <c r="N43" s="27"/>
-      <c r="O43" s="57"/>
+      <c r="O43" s="60"/>
       <c r="P43" s="28" t="str">
         <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$36,2,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A43 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -4655,7 +4737,7 @@
       <c r="L44" s="26"/>
       <c r="M44" s="26"/>
       <c r="N44" s="27"/>
-      <c r="O44" s="57"/>
+      <c r="O44" s="60"/>
       <c r="P44" s="28" t="str">
         <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$36,2,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A44 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -4707,7 +4789,7 @@
       <c r="L45" s="26"/>
       <c r="M45" s="26"/>
       <c r="N45" s="27"/>
-      <c r="O45" s="57"/>
+      <c r="O45" s="60"/>
       <c r="P45" s="28" t="str">
         <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$36,2,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A45 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -4759,7 +4841,7 @@
       <c r="L46" s="26"/>
       <c r="M46" s="26"/>
       <c r="N46" s="27"/>
-      <c r="O46" s="57"/>
+      <c r="O46" s="60"/>
       <c r="P46" s="28" t="str">
         <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$36,2,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A46 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -4811,7 +4893,7 @@
       <c r="L47" s="26"/>
       <c r="M47" s="26"/>
       <c r="N47" s="27"/>
-      <c r="O47" s="57"/>
+      <c r="O47" s="60"/>
       <c r="P47" s="28" t="str">
         <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$36,2,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A47 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -4863,7 +4945,7 @@
       <c r="L48" s="26"/>
       <c r="M48" s="26"/>
       <c r="N48" s="27"/>
-      <c r="O48" s="57"/>
+      <c r="O48" s="60"/>
       <c r="P48" s="28" t="str">
         <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$36,2,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A48 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -4915,7 +4997,7 @@
       <c r="L49" s="26"/>
       <c r="M49" s="26"/>
       <c r="N49" s="27"/>
-      <c r="O49" s="57"/>
+      <c r="O49" s="60"/>
       <c r="P49" s="28" t="str">
         <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$36,2,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A49 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -4967,7 +5049,7 @@
       <c r="L50" s="26"/>
       <c r="M50" s="26"/>
       <c r="N50" s="27"/>
-      <c r="O50" s="57"/>
+      <c r="O50" s="60"/>
       <c r="P50" s="28" t="str">
         <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$36,2,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A50 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -5019,7 +5101,7 @@
       <c r="L51" s="39"/>
       <c r="M51" s="39"/>
       <c r="N51" s="40"/>
-      <c r="O51" s="60"/>
+      <c r="O51" s="64"/>
       <c r="P51" s="41" t="str">
         <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$36,2,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A51 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
@@ -5053,7 +5135,7 @@
       <c r="L52" s="46"/>
       <c r="M52" s="46"/>
       <c r="N52" s="47"/>
-      <c r="O52" s="61"/>
+      <c r="O52" s="55"/>
       <c r="P52" s="47"/>
       <c r="Q52" s="46"/>
       <c r="R52" s="46"/>
@@ -5067,27 +5149,32 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>
-  <conditionalFormatting sqref="A2:F3 A5:F5 A8:F27 A35:F51">
-    <cfRule type="expression" dxfId="4" priority="8">
+  <conditionalFormatting sqref="A2:F3 A5:F5 A35:F51 A29:F31 A8:F23">
+    <cfRule type="expression" dxfId="5" priority="9">
       <formula>OR(A2=0, A2=OFFSET(A2,-1,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:F4">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>OR(A4=0, A4=OFFSET(A4,-1,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:F7">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>OR(A7=0, A7=OFFSET(A7,-1,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:F6">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>OR(A6=0, A6=OFFSET(A6,-1,0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A28:F34">
+  <conditionalFormatting sqref="A24:F27 A32:F34">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>OR(A24=0, A24=OFFSET(A24,-1,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28:F28">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>OR(A28=0, A28=OFFSET(A28,-1,0))</formula>
     </cfRule>
@@ -5119,7 +5206,9 @@
   </sheetPr>
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5141,7 +5230,7 @@
         <v>29</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -5149,130 +5238,130 @@
         <v>16</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>100</v>
+        <v>162</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D2" s="50"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="50" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C3" s="51" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="50" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C4" s="51" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D4" s="50"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="50" t="s">
-        <v>30</v>
+        <v>167</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>101</v>
+        <v>165</v>
       </c>
       <c r="C5" s="51" t="s">
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="D5" s="50"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="50" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="C6" s="51" t="s">
-        <v>146</v>
+        <v>30</v>
       </c>
       <c r="D6" s="50"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="50" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D7" s="50"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="50" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D8" s="50"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="50" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D9" s="50"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="50" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C10" s="51" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D10" s="50"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="50" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C11" s="51" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D11" s="50"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="50" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C12" s="51" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D12" s="50"/>
     </row>
@@ -5281,10 +5370,10 @@
         <v>26</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C13" s="51" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="50"/>
     </row>
@@ -5293,115 +5382,115 @@
         <v>21</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C14" s="51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="50"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="50" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C15" s="51" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D15" s="50"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="50" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C16" s="51" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D16" s="50"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="51" t="s">
         <v>34</v>
-      </c>
-      <c r="B17" s="51" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" s="51" t="s">
-        <v>35</v>
       </c>
       <c r="D17" s="50"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="50" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C18" s="51" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D18" s="50"/>
     </row>
     <row r="19" spans="1:4" ht="135" x14ac:dyDescent="0.15">
       <c r="A19" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="51" t="s">
-        <v>111</v>
-      </c>
-      <c r="C19" s="51" t="s">
-        <v>37</v>
-      </c>
       <c r="D19" s="51" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="A20" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C20" s="51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" s="51" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="A21" s="50" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C21" s="51" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="A22" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D22" s="51" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
@@ -5409,48 +5498,48 @@
         <v>25</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="50" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B24" s="51" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C24" s="51" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D24" s="51"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="51" t="s">
         <v>39</v>
-      </c>
-      <c r="B25" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="C25" s="51" t="s">
-        <v>40</v>
       </c>
       <c r="D25" s="51"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D26" s="50"/>
     </row>
@@ -5459,125 +5548,125 @@
         <v>27</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D27" s="53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A28" s="50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C28" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D28" s="50"/>
     </row>
     <row r="29" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A29" s="50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D29" s="53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="51" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="51" t="s">
         <v>68</v>
-      </c>
-      <c r="B30" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="C30" s="51" t="s">
-        <v>69</v>
       </c>
       <c r="D30" s="53"/>
     </row>
     <row r="31" spans="1:4" ht="81" x14ac:dyDescent="0.15">
       <c r="A31" s="50" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D31" s="51" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A32" s="50" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B32" s="51" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C32" s="51" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D32" s="51" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="50" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B33" s="51" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C33" s="51" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="53" t="s">
         <v>161</v>
-      </c>
-      <c r="D33" s="53" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A34" s="50" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B34" s="51" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C34" s="51" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D34" s="53" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="52" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B35" s="52" t="s">
-        <v>141</v>
-      </c>
-      <c r="C35" s="64" t="s">
-        <v>139</v>
+        <v>137</v>
+      </c>
+      <c r="C35" s="57" t="s">
+        <v>135</v>
       </c>
       <c r="D35" s="52"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="52"/>
       <c r="B36" s="52"/>
-      <c r="C36" s="64"/>
+      <c r="C36" s="57"/>
       <c r="D36" s="52"/>
     </row>
   </sheetData>
@@ -5600,87 +5689,87 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" s="48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" s="48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" s="48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" s="48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" s="48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A10" s="48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A12" s="48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A13" s="48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A15" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A16" s="48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" s="48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" s="48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" s="48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add IE/EXE command map.
</commit_message>
<xml_diff>
--- a/PaperTester.xlsx
+++ b/PaperTester.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="178">
   <si>
     <t>No.</t>
   </si>
@@ -1197,6 +1197,22 @@
     <rPh sb="13" eb="15">
       <t>ソウサ</t>
     </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>IE</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>EXE</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>○</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>△</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -1678,7 +1694,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1873,6 +1889,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2296,7 +2324,7 @@
       <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P32" sqref="P2:P32"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2418,11 +2446,11 @@
       </c>
       <c r="O2" s="58"/>
       <c r="P2" s="16" t="str">
-        <f ca="1">IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$36,2,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A2 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$C$2:$E$36,2,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A2 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.OpenIE : onErrorExit "テストケース = 1, Excel行 = 2"</v>
       </c>
       <c r="Q2" s="16" t="str">
-        <f>IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$A$2:$C$36,3,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N2="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N2,data!$C$2:$E$36,3,0),"%0",$O2), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>InternetExplorerを開く。</v>
       </c>
       <c r="R2" s="17" t="s">
@@ -2488,11 +2516,11 @@
         <v>22</v>
       </c>
       <c r="P3" s="28" t="str">
-        <f ca="1">IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$A$2:$C$36,2,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A3 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$C$2:$E$36,2,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A3 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Navigate "http://bl.ocks.org/nezuQ/raw/9719897/" : onErrorExit "テストケース = 1, Excel行 = 3"</v>
       </c>
       <c r="Q3" s="28" t="str">
-        <f>IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$A$2:$C$36,3,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N3="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N3,data!$C$2:$E$36,3,0),"%0",$O3), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>URL「http://bl.ocks.org/nezuQ/raw/9719897/」で遷移する。</v>
       </c>
       <c r="R3" s="29"/>
@@ -2542,11 +2570,11 @@
       </c>
       <c r="O4" s="60"/>
       <c r="P4" s="28" t="str">
-        <f ca="1">IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$36,2,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A4 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$C$2:$E$36,2,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A4 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.MaximumWindow : onErrorExit "テストケース = 1, Excel行 = 4"</v>
       </c>
       <c r="Q4" s="28" t="str">
-        <f>IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$A$2:$C$36,3,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N4="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N4,data!$C$2:$E$36,3,0),"%0",$O4), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>InternetExplorerを最大化する。</v>
       </c>
       <c r="R4" s="33"/>
@@ -2599,11 +2627,11 @@
         <v>1</v>
       </c>
       <c r="P5" s="28" t="str">
-        <f ca="1">IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$A$2:$C$36,2,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A5 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$C$2:$E$36,2,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A5 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.FullScreenShot4VisibleArea "1" : onErrorExit "テストケース = 1, Excel行 = 5"</v>
       </c>
       <c r="Q5" s="28" t="str">
-        <f ca="1">IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$A$2:$C$36,3,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f ca="1">IF($N5="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N5,data!$C$2:$E$36,3,0),"%0",$O5), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>スクリーンショットを撮る。（画面全体, 表示箇所のみ, コメント："1"）</v>
       </c>
       <c r="R5" s="29"/>
@@ -2655,11 +2683,11 @@
         <v>160</v>
       </c>
       <c r="P6" s="28" t="str">
-        <f ca="1">IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$36,2,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A6 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$C$2:$E$36,2,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A6 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Record2ValidateTitle "PxCSV ～Pixiv検索結果をCSV形式で～" : onErrorExit "テストケース = 1, Excel行 = 6"</v>
       </c>
       <c r="Q6" s="28" t="str">
-        <f>IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$A$2:$C$36,3,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N6="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N6,data!$C$2:$E$36,3,0),"%0",$O6), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>画面のタイトルを検証する。検証NG時は処理を続行する。（タイトル："PxCSV ～Pixiv検索結果をCSV形式で～"）</v>
       </c>
       <c r="R6" s="33"/>
@@ -2711,11 +2739,11 @@
         <v>127</v>
       </c>
       <c r="P7" s="28" t="str">
-        <f ca="1">IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$36,2,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A7 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$C$2:$E$36,2,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A7 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Record2ValidateAttribute "id=ddlEndpoint &lt;- '0' %|% id=txtQuery &lt;- 'あああああ '" : onErrorExit "テストケース = 1, Excel行 = 7"</v>
       </c>
       <c r="Q7" s="28" t="str">
-        <f>IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$A$2:$C$36,3,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N7="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N7,data!$C$2:$E$36,3,0),"%0",$O7), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>項目の属性値を検証する。検証NG時は処理を続行する。"id=ddlEndpoint &lt;- '0' %|% id=txtQuery &lt;- 'あああああ '"</v>
       </c>
       <c r="R7" s="33"/>
@@ -2752,11 +2780,11 @@
         <v>70</v>
       </c>
       <c r="P8" s="28" t="str">
-        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$36,2,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A8 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$C$2:$E$36,2,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A8 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.ExecuteSQL "SELECT * FROM [Sheet1$] " : onErrorExit "テストケース = , Excel行 = 8"</v>
       </c>
       <c r="Q8" s="28" t="str">
-        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$A$2:$C$36,3,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N8="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N8,data!$C$2:$E$36,3,0),"%0",$O8), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>SQL文を発行する。"SELECT * FROM [Sheet1$] "</v>
       </c>
       <c r="R8" s="29"/>
@@ -2806,11 +2834,11 @@
       <c r="N9" s="27"/>
       <c r="O9" s="61"/>
       <c r="P9" s="28" t="str">
-        <f>IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$36,2,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A9 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$C$2:$E$36,2,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A9 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q9" s="28" t="str">
-        <f>IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$A$2:$C$36,3,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N9="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N9,data!$C$2:$E$36,3,0),"%0",$O9), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R9" s="29" t="s">
@@ -2880,11 +2908,11 @@
         <v>119</v>
       </c>
       <c r="P10" s="28" t="str">
-        <f ca="1">IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$36,2,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A10 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$C$2:$E$36,2,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A10 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.ValueInput "id=ddlEndpoint &lt;- '1' %|% id=ddlSearchType &lt;- '1' %|% id=txtQuery &lt;- '艦隊これくしょん' %|% id=txtPHPSessID &lt;- ''" : onErrorExit "テストケース = 2-1, Excel行 = 10"</v>
       </c>
       <c r="Q10" s="28" t="str">
-        <f>IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$A$2:$C$36,3,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N10="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N10,data!$C$2:$E$36,3,0),"%0",$O10), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>項目「引数の前部分」に値「引数の後部分」を入力する。"id=ddlEndpoint &lt;- '1' %|% id=ddlSearchType &lt;- '1' %|% id=txtQuery &lt;- '艦隊これくしょん' %|% id=txtPHPSessID &lt;- ''"</v>
       </c>
       <c r="R10" s="29" t="s">
@@ -2951,11 +2979,11 @@
         <v>2-1</v>
       </c>
       <c r="P11" s="28" t="str">
-        <f ca="1">IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$36,2,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A11 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$C$2:$E$36,2,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A11 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.FullScreenShot "2-1" : onErrorExit "テストケース = 2-1, Excel行 = 11"</v>
       </c>
       <c r="Q11" s="28" t="str">
-        <f ca="1">IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$A$2:$C$36,3,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f ca="1">IF($N11="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N11,data!$C$2:$E$36,3,0),"%0",$O11), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>スクリーンショットを撮る。（画面全体, コメント："2-1"）</v>
       </c>
       <c r="R11" s="33"/>
@@ -3007,11 +3035,11 @@
         <v>77</v>
       </c>
       <c r="P12" s="28" t="str">
-        <f ca="1">IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$36,2,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A12 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$C$2:$E$36,2,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A12 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Click "tag=input#4" : onErrorExit "テストケース = 2-1, Excel行 = 12"</v>
       </c>
       <c r="Q12" s="28" t="str">
-        <f>IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$A$2:$C$36,3,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N12="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N12,data!$C$2:$E$36,3,0),"%0",$O12), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>項目「tag=input#4」をクリックする。</v>
       </c>
       <c r="R12" s="33"/>
@@ -3061,11 +3089,11 @@
       </c>
       <c r="O13" s="60"/>
       <c r="P13" s="28" t="str">
-        <f ca="1">IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$36,2,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A13 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$C$2:$E$36,2,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A13 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.ActivateNextIE : onErrorExit "テストケース = 2-1, Excel行 = 13"</v>
       </c>
       <c r="Q13" s="28" t="str">
-        <f>IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$A$2:$C$36,3,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N13="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N13,data!$C$2:$E$36,3,0),"%0",$O13), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>次に開いたInternetExplorerをアクティブにする。</v>
       </c>
       <c r="R13" s="33"/>
@@ -3115,11 +3143,11 @@
       </c>
       <c r="O14" s="60"/>
       <c r="P14" s="28" t="str">
-        <f ca="1">IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$36,2,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A14 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$C$2:$E$36,2,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A14 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.FullScreenShot "" : onErrorExit "テストケース = 2-1, Excel行 = 14"</v>
       </c>
       <c r="Q14" s="28" t="str">
-        <f>IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$A$2:$C$36,3,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N14="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N14,data!$C$2:$E$36,3,0),"%0",$O14), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>スクリーンショットを撮る。（画面全体, コメント：""）</v>
       </c>
       <c r="R14" s="33"/>
@@ -3171,11 +3199,11 @@
         <v>116</v>
       </c>
       <c r="P15" s="28" t="str">
-        <f ca="1">IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$36,2,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A15 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$C$2:$E$36,2,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A15 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.ExecuteSQL "SELECT * FROM [Sheet1$] WHERE 列名1 = 2" : onErrorExit "テストケース = 2-1, Excel行 = 15"</v>
       </c>
       <c r="Q15" s="28" t="str">
-        <f>IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$A$2:$C$36,3,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N15="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N15,data!$C$2:$E$36,3,0),"%0",$O15), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>SQL文を発行する。"SELECT * FROM [Sheet1$] WHERE 列名1 = 2"</v>
       </c>
       <c r="R15" s="33"/>
@@ -3225,11 +3253,11 @@
       <c r="N16" s="27"/>
       <c r="O16" s="60"/>
       <c r="P16" s="28" t="str">
-        <f>IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$36,2,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A16 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$C$2:$E$36,2,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A16 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q16" s="28" t="str">
-        <f>IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$A$2:$C$36,3,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N16="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N16,data!$C$2:$E$36,3,0),"%0",$O16), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R16" s="33"/>
@@ -3283,11 +3311,11 @@
       </c>
       <c r="O17" s="60"/>
       <c r="P17" s="28" t="str">
-        <f ca="1">IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$36,2,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A17 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$C$2:$E$36,2,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A17 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Quit : onErrorExit "テストケース = 3-1, Excel行 = 17"</v>
       </c>
       <c r="Q17" s="28" t="str">
-        <f>IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$A$2:$C$36,3,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N17="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N17,data!$C$2:$E$36,3,0),"%0",$O17), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>InternetExplorerを閉じる。</v>
       </c>
       <c r="R17" s="33"/>
@@ -3339,11 +3367,11 @@
         <v>168</v>
       </c>
       <c r="P18" s="28" t="str">
-        <f ca="1">IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$36,2,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A18 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$C$2:$E$36,2,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A18 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Run "notepad.exe" : onErrorExit "テストケース = 3-1, Excel行 = 18"</v>
       </c>
       <c r="Q18" s="28" t="str">
-        <f>IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$A$2:$C$36,3,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N18,data!$C$2:$E$36,3,0),"%0",$O18), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>EXEを実行する。</v>
       </c>
       <c r="R18" s="33"/>
@@ -3393,11 +3421,11 @@
       </c>
       <c r="O19" s="60"/>
       <c r="P19" s="28" t="str">
-        <f ca="1">IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$36,2,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A19 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$C$2:$E$36,2,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A19 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.MaximumWindow : onErrorExit "テストケース = 3-1, Excel行 = 19"</v>
       </c>
       <c r="Q19" s="28" t="str">
-        <f>IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$A$2:$C$36,3,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N19,data!$C$2:$E$36,3,0),"%0",$O19), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>InternetExplorerを最大化する。</v>
       </c>
       <c r="R19" s="33"/>
@@ -3449,11 +3477,11 @@
         <v>173</v>
       </c>
       <c r="P20" s="28" t="str">
-        <f ca="1">IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$36,2,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A20 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$C$2:$E$36,2,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A20 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Paste "【開始】任意のEXEをキー操作できます。" : onErrorExit "テストケース = 3-1, Excel行 = 20"</v>
       </c>
       <c r="Q20" s="28" t="str">
-        <f>IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$A$2:$C$36,3,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N20,data!$C$2:$E$36,3,0),"%0",$O20), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>アクティブ画面へ「【開始】任意のEXEをキー操作できます。」を貼り付ける。</v>
       </c>
       <c r="R20" s="33"/>
@@ -3505,11 +3533,11 @@
         <v>171</v>
       </c>
       <c r="P21" s="28" t="str">
-        <f ca="1">IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$36,2,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A21 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$C$2:$E$36,2,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A21 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.FullScreenShot4VisibleArea "3-1" : onErrorExit "テストケース = 3-1, Excel行 = 21"</v>
       </c>
       <c r="Q21" s="28" t="str">
-        <f>IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$A$2:$C$36,3,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N21,data!$C$2:$E$36,3,0),"%0",$O21), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>スクリーンショットを撮る。（画面全体, 表示箇所のみ, コメント："3-1"）</v>
       </c>
       <c r="R21" s="33"/>
@@ -3561,11 +3589,11 @@
         <v>1</v>
       </c>
       <c r="P22" s="28" t="str">
-        <f ca="1">IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$36,2,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A22 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$C$2:$E$36,2,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A22 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Sleep 1 : onErrorExit "テストケース = 3-1, Excel行 = 22"</v>
       </c>
       <c r="Q22" s="28" t="str">
-        <f>IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$A$2:$C$36,3,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N22,data!$C$2:$E$36,3,0),"%0",$O22), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>プログラムを「1」秒停止する</v>
       </c>
       <c r="R22" s="33"/>
@@ -3617,11 +3645,11 @@
         <v>169</v>
       </c>
       <c r="P23" s="28" t="str">
-        <f ca="1">IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$36,2,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A23 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$C$2:$E$36,2,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A23 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.SendKeys "%(FNN)" : onErrorExit "テストケース = 3-1, Excel行 = 23"</v>
       </c>
       <c r="Q23" s="28" t="str">
-        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$A$2:$C$36,3,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N23,data!$C$2:$E$36,3,0),"%0",$O23), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>アクティブ画面へ「%(FNN)」をキー入力する。</v>
       </c>
       <c r="R23" s="33"/>
@@ -3673,11 +3701,11 @@
         <v>170</v>
       </c>
       <c r="P24" s="28" t="str">
-        <f ca="1">IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$36,2,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A24 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$C$2:$E$36,2,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A24 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Paste "【終了】メモ帳を開き直しました。" : onErrorExit "テストケース = 3-1, Excel行 = 24"</v>
       </c>
       <c r="Q24" s="28" t="str">
-        <f>IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$A$2:$C$36,3,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N24,data!$C$2:$E$36,3,0),"%0",$O24), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>アクティブ画面へ「【終了】メモ帳を開き直しました。」を貼り付ける。</v>
       </c>
       <c r="R24" s="33"/>
@@ -3727,11 +3755,11 @@
       </c>
       <c r="O25" s="60"/>
       <c r="P25" s="28" t="str">
-        <f ca="1">IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$36,2,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A25 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$C$2:$E$36,2,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A25 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.FullScreenShot4VisibleArea "" : onErrorExit "テストケース = 3-1, Excel行 = 25"</v>
       </c>
       <c r="Q25" s="28" t="str">
-        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$A$2:$C$36,3,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N25,data!$C$2:$E$36,3,0),"%0",$O25), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>スクリーンショットを撮る。（画面全体, 表示箇所のみ, コメント：""）</v>
       </c>
       <c r="R25" s="33"/>
@@ -3783,11 +3811,11 @@
         <v>1</v>
       </c>
       <c r="P26" s="28" t="str">
-        <f ca="1">IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$36,2,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A26 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$C$2:$E$36,2,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A26 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Sleep 1 : onErrorExit "テストケース = 3-1, Excel行 = 26"</v>
       </c>
       <c r="Q26" s="28" t="str">
-        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$A$2:$C$36,3,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N26,data!$C$2:$E$36,3,0),"%0",$O26), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>プログラムを「1」秒停止する</v>
       </c>
       <c r="R26" s="33"/>
@@ -3837,11 +3865,11 @@
       </c>
       <c r="O27" s="60"/>
       <c r="P27" s="28" t="str">
-        <f ca="1">IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$36,2,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A27 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$C$2:$E$36,2,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A27 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Quit : onErrorExit "テストケース = 3-1, Excel行 = 27"</v>
       </c>
       <c r="Q27" s="28" t="str">
-        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$A$2:$C$36,3,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N27,data!$C$2:$E$36,3,0),"%0",$O27), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>InternetExplorerを閉じる。</v>
       </c>
       <c r="R27" s="33"/>
@@ -3893,11 +3921,11 @@
         <v>1</v>
       </c>
       <c r="P28" s="28" t="str">
-        <f ca="1">IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$36,2,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A28 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$C$2:$E$36,2,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A28 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Sleep 1 : onErrorExit "テストケース = 3-1, Excel行 = 28"</v>
       </c>
       <c r="Q28" s="28" t="str">
-        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$A$2:$C$36,3,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N28="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N28,data!$C$2:$E$36,3,0),"%0",$O28), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>プログラムを「1」秒停止する</v>
       </c>
       <c r="R28" s="33"/>
@@ -3949,11 +3977,11 @@
         <v>138</v>
       </c>
       <c r="P29" s="28" t="str">
-        <f ca="1">IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$36,2,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A29 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$C$2:$E$36,2,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A29 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.ExecuteJS "alert('任意のJavascriptを実行できます。')" : onErrorExit "テストケース = 3-1, Excel行 = 29"</v>
       </c>
       <c r="Q29" s="28" t="str">
-        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$A$2:$C$36,3,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N29="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N29,data!$C$2:$E$36,3,0),"%0",$O29), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>Javascriptコード「alert('任意のJavascriptを実行できます。')」を実行する。</v>
       </c>
       <c r="R29" s="33"/>
@@ -4005,11 +4033,11 @@
         <v>1</v>
       </c>
       <c r="P30" s="28" t="str">
-        <f ca="1">IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$36,2,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A30 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$C$2:$E$36,2,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A30 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Sleep 1 : onErrorExit "テストケース = 3-1, Excel行 = 30"</v>
       </c>
       <c r="Q30" s="28" t="str">
-        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$A$2:$C$36,3,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N30="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N30,data!$C$2:$E$36,3,0),"%0",$O30), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>プログラムを「1」秒停止する</v>
       </c>
       <c r="R30" s="33"/>
@@ -4061,11 +4089,11 @@
         <v>172</v>
       </c>
       <c r="P31" s="28" t="str">
-        <f ca="1">IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$36,2,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A31 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$C$2:$E$36,2,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A31 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.SendKeys "{ENTER}" : onErrorExit "テストケース = 3-1, Excel行 = 31"</v>
       </c>
       <c r="Q31" s="28" t="str">
-        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$A$2:$C$36,3,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N31="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N31,data!$C$2:$E$36,3,0),"%0",$O31), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>アクティブ画面へ「{ENTER}」をキー入力する。</v>
       </c>
       <c r="R31" s="33"/>
@@ -4115,11 +4143,11 @@
       </c>
       <c r="O32" s="60"/>
       <c r="P32" s="28" t="str">
-        <f ca="1">IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$36,2,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A32 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f ca="1">IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$C$2:$E$36,2,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A32 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v>pt.Quit : onErrorExit "テストケース = 3-1, Excel行 = 32"</v>
       </c>
       <c r="Q32" s="28" t="str">
-        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$A$2:$C$36,3,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N32="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N32,data!$C$2:$E$36,3,0),"%0",$O32), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v>InternetExplorerを閉じる。</v>
       </c>
       <c r="R32" s="33"/>
@@ -4167,11 +4195,11 @@
       <c r="N33" s="27"/>
       <c r="O33" s="60"/>
       <c r="P33" s="28" t="str">
-        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$36,2,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A33 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$C$2:$E$36,2,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A33 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q33" s="28" t="str">
-        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$A$2:$C$36,3,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N33="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N33,data!$C$2:$E$36,3,0),"%0",$O33), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R33" s="33"/>
@@ -4219,11 +4247,11 @@
       <c r="N34" s="27"/>
       <c r="O34" s="60"/>
       <c r="P34" s="28" t="str">
-        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$36,2,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A34 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$C$2:$E$36,2,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A34 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q34" s="28" t="str">
-        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$A$2:$C$36,3,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N34="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N34,data!$C$2:$E$36,3,0),"%0",$O34), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R34" s="33"/>
@@ -4271,11 +4299,11 @@
       <c r="N35" s="27"/>
       <c r="O35" s="60"/>
       <c r="P35" s="28" t="str">
-        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$36,2,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A35 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$C$2:$E$36,2,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A35 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q35" s="28" t="str">
-        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$A$2:$C$36,3,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N35="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N35,data!$C$2:$E$36,3,0),"%0",$O35), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R35" s="33"/>
@@ -4323,11 +4351,11 @@
       <c r="N36" s="27"/>
       <c r="O36" s="60"/>
       <c r="P36" s="28" t="str">
-        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$36,2,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A36 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$C$2:$E$36,2,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A36 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q36" s="28" t="str">
-        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$A$2:$C$36,3,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N36="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N36,data!$C$2:$E$36,3,0),"%0",$O36), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R36" s="33"/>
@@ -4375,11 +4403,11 @@
       <c r="N37" s="27"/>
       <c r="O37" s="60"/>
       <c r="P37" s="28" t="str">
-        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$36,2,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A37 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$C$2:$E$36,2,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A37 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q37" s="28" t="str">
-        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$A$2:$C$36,3,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N37="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N37,data!$C$2:$E$36,3,0),"%0",$O37), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R37" s="33"/>
@@ -4427,11 +4455,11 @@
       <c r="N38" s="27"/>
       <c r="O38" s="60"/>
       <c r="P38" s="28" t="str">
-        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$36,2,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A38 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$C$2:$E$36,2,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A38 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q38" s="28" t="str">
-        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$A$2:$C$36,3,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N38="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N38,data!$C$2:$E$36,3,0),"%0",$O38), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R38" s="33"/>
@@ -4479,11 +4507,11 @@
       <c r="N39" s="27"/>
       <c r="O39" s="60"/>
       <c r="P39" s="28" t="str">
-        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$36,2,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A39 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$C$2:$E$36,2,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A39 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q39" s="28" t="str">
-        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$A$2:$C$36,3,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N39="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N39,data!$C$2:$E$36,3,0),"%0",$O39), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R39" s="33"/>
@@ -4531,11 +4559,11 @@
       <c r="N40" s="27"/>
       <c r="O40" s="60"/>
       <c r="P40" s="28" t="str">
-        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$36,2,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A40 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$C$2:$E$36,2,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A40 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q40" s="28" t="str">
-        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$A$2:$C$36,3,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N40="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N40,data!$C$2:$E$36,3,0),"%0",$O40), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R40" s="33"/>
@@ -4583,11 +4611,11 @@
       <c r="N41" s="27"/>
       <c r="O41" s="60"/>
       <c r="P41" s="28" t="str">
-        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$36,2,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A41 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$C$2:$E$36,2,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A41 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q41" s="28" t="str">
-        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$A$2:$C$36,3,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N41="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N41,data!$C$2:$E$36,3,0),"%0",$O41), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R41" s="33"/>
@@ -4635,11 +4663,11 @@
       <c r="N42" s="27"/>
       <c r="O42" s="60"/>
       <c r="P42" s="28" t="str">
-        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$36,2,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A42 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$C$2:$E$36,2,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A42 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q42" s="28" t="str">
-        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$A$2:$C$36,3,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N42="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N42,data!$C$2:$E$36,3,0),"%0",$O42), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R42" s="33"/>
@@ -4687,11 +4715,11 @@
       <c r="N43" s="27"/>
       <c r="O43" s="60"/>
       <c r="P43" s="28" t="str">
-        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$36,2,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A43 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$C$2:$E$36,2,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A43 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q43" s="28" t="str">
-        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$A$2:$C$36,3,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N43="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N43,data!$C$2:$E$36,3,0),"%0",$O43), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R43" s="33"/>
@@ -4739,11 +4767,11 @@
       <c r="N44" s="27"/>
       <c r="O44" s="60"/>
       <c r="P44" s="28" t="str">
-        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$36,2,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A44 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$C$2:$E$36,2,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A44 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q44" s="28" t="str">
-        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$A$2:$C$36,3,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N44="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N44,data!$C$2:$E$36,3,0),"%0",$O44), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R44" s="33"/>
@@ -4791,11 +4819,11 @@
       <c r="N45" s="27"/>
       <c r="O45" s="60"/>
       <c r="P45" s="28" t="str">
-        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$36,2,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A45 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$C$2:$E$36,2,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A45 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q45" s="28" t="str">
-        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$A$2:$C$36,3,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N45="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N45,data!$C$2:$E$36,3,0),"%0",$O45), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R45" s="33"/>
@@ -4843,11 +4871,11 @@
       <c r="N46" s="27"/>
       <c r="O46" s="60"/>
       <c r="P46" s="28" t="str">
-        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$36,2,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A46 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$C$2:$E$36,2,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A46 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q46" s="28" t="str">
-        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$A$2:$C$36,3,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N46="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N46,data!$C$2:$E$36,3,0),"%0",$O46), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R46" s="33"/>
@@ -4895,11 +4923,11 @@
       <c r="N47" s="27"/>
       <c r="O47" s="60"/>
       <c r="P47" s="28" t="str">
-        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$36,2,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A47 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$C$2:$E$36,2,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A47 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q47" s="28" t="str">
-        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$A$2:$C$36,3,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N47="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N47,data!$C$2:$E$36,3,0),"%0",$O47), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R47" s="33"/>
@@ -4947,11 +4975,11 @@
       <c r="N48" s="27"/>
       <c r="O48" s="60"/>
       <c r="P48" s="28" t="str">
-        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$36,2,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A48 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$C$2:$E$36,2,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A48 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q48" s="28" t="str">
-        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$A$2:$C$36,3,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N48="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N48,data!$C$2:$E$36,3,0),"%0",$O48), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R48" s="33"/>
@@ -4999,11 +5027,11 @@
       <c r="N49" s="27"/>
       <c r="O49" s="60"/>
       <c r="P49" s="28" t="str">
-        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$36,2,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A49 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$C$2:$E$36,2,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A49 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q49" s="28" t="str">
-        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$A$2:$C$36,3,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N49="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N49,data!$C$2:$E$36,3,0),"%0",$O49), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R49" s="33"/>
@@ -5051,11 +5079,11 @@
       <c r="N50" s="27"/>
       <c r="O50" s="60"/>
       <c r="P50" s="28" t="str">
-        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$36,2,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A50 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$C$2:$E$36,2,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A50 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q50" s="28" t="str">
-        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$A$2:$C$36,3,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N50="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N50,data!$C$2:$E$36,3,0),"%0",$O50), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R50" s="33"/>
@@ -5103,11 +5131,11 @@
       <c r="N51" s="40"/>
       <c r="O51" s="64"/>
       <c r="P51" s="41" t="str">
-        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$36,2,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A51 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
+        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$C$2:$E$36,2,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD) &amp; " ""テストケース = " &amp; A51 &amp; ", Excel行 = " &amp; ROW() &amp; """")</f>
         <v/>
       </c>
       <c r="Q51" s="41" t="str">
-        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$A$2:$C$36,3,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
+        <f>IF($N51="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP($N51,data!$C$2:$E$36,3,0),"%0",$O51), CHAR(10), OPTIONROW_SEPERATE_KEYWORD))</f>
         <v/>
       </c>
       <c r="R51" s="42"/>
@@ -5189,7 +5217,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>data!$A$2:$A$36</xm:f>
+            <xm:f>data!$C$2:$C$36</xm:f>
           </x14:formula1>
           <xm:sqref>N2:N51</xm:sqref>
         </x14:dataValidation>
@@ -5204,470 +5232,635 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B35"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="48.125"/>
-    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.375" customWidth="1"/>
-    <col min="4" max="4" width="91.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="1025" width="8.625"/>
+    <col min="1" max="2" width="5.625" style="68" customWidth="1"/>
+    <col min="3" max="3" width="48.125"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.375" customWidth="1"/>
+    <col min="6" max="6" width="91.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="1027" width="8.625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A1" s="65" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="D1" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="E1" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="F1" s="49" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="50" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="66"/>
+      <c r="C2" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="D2" s="51" t="s">
         <v>162</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="E2" s="51" t="s">
         <v>144</v>
       </c>
-      <c r="D2" s="50"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="50" t="s">
+      <c r="F2" s="50"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="66"/>
+      <c r="C3" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="D3" s="51" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="E3" s="51" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="50"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="50" t="s">
+      <c r="F3" s="50"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" s="66"/>
+      <c r="C4" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="D4" s="51" t="s">
         <v>140</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="E4" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="50"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="50" t="s">
+      <c r="F4" s="50"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="66"/>
+      <c r="B5" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="50" t="s">
         <v>167</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="D5" s="51" t="s">
         <v>165</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="E5" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="D5" s="50"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="50" t="s">
+      <c r="F5" s="50"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="D6" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="E6" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="50"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="50" t="s">
+      <c r="F6" s="50"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="D7" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="E7" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="50"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="50" t="s">
+      <c r="F7" s="50"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" s="66" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="D8" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="E8" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="50"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="50" t="s">
+      <c r="F8" s="50"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="66" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="D9" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="E9" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="D9" s="50"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="50" t="s">
+      <c r="F9" s="50"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="C10" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="D10" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="E10" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="D10" s="50"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="50" t="s">
+      <c r="F10" s="50"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="D11" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="E11" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="D11" s="50"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="50" t="s">
+      <c r="F11" s="50"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="D12" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="E12" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="50"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="50" t="s">
+      <c r="F12" s="50"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B13" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="D13" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="E13" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="50"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="50" t="s">
+      <c r="F13" s="50"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14" s="66"/>
+      <c r="C14" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="D14" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="C14" s="51" t="s">
+      <c r="E14" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="50"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="50" t="s">
+      <c r="F14" s="50"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B15" s="66"/>
+      <c r="C15" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="B15" s="51" t="s">
+      <c r="D15" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="C15" s="51" t="s">
+      <c r="E15" s="51" t="s">
         <v>145</v>
       </c>
-      <c r="D15" s="50"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="50" t="s">
+      <c r="F15" s="50"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B16" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="C16" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="D16" s="51" t="s">
         <v>143</v>
       </c>
-      <c r="C16" s="51" t="s">
+      <c r="E16" s="51" t="s">
         <v>146</v>
       </c>
-      <c r="D16" s="50"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="50" t="s">
+      <c r="F16" s="50"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17" s="66"/>
+      <c r="C17" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="D17" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="E17" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="50"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="50" t="s">
+      <c r="F17" s="50"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" s="66"/>
+      <c r="C18" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="D18" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="E18" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="50"/>
-    </row>
-    <row r="19" spans="1:4" ht="135" x14ac:dyDescent="0.15">
-      <c r="A19" s="50" t="s">
+      <c r="F18" s="50"/>
+    </row>
+    <row r="19" spans="1:6" ht="135" x14ac:dyDescent="0.15">
+      <c r="A19" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B19" s="66"/>
+      <c r="C19" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="D19" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="C19" s="51" t="s">
+      <c r="E19" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="51" t="s">
+      <c r="F19" s="51" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="54" x14ac:dyDescent="0.15">
-      <c r="A20" s="50" t="s">
+    <row r="20" spans="1:6" ht="54" x14ac:dyDescent="0.15">
+      <c r="A20" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B20" s="66"/>
+      <c r="C20" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="D20" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="C20" s="51" t="s">
+      <c r="E20" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="51" t="s">
+      <c r="F20" s="51" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="54" x14ac:dyDescent="0.15">
-      <c r="A21" s="50" t="s">
+    <row r="21" spans="1:6" ht="54" x14ac:dyDescent="0.15">
+      <c r="A21" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B21" s="66"/>
+      <c r="C21" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="D21" s="51" t="s">
         <v>118</v>
       </c>
-      <c r="C21" s="51" t="s">
+      <c r="E21" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="51" t="s">
+      <c r="F21" s="51" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="54" x14ac:dyDescent="0.15">
-      <c r="A22" s="50" t="s">
+    <row r="22" spans="1:6" ht="54" x14ac:dyDescent="0.15">
+      <c r="A22" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22" s="66"/>
+      <c r="C22" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="51" t="s">
+      <c r="D22" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="C22" s="51" t="s">
+      <c r="E22" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="D22" s="51" t="s">
+      <c r="F22" s="51" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="50" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B23" s="66"/>
+      <c r="C23" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="51" t="s">
+      <c r="D23" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="C23" s="51" t="s">
+      <c r="E23" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="51" t="s">
+      <c r="F23" s="51" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="50" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B24" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="C24" s="50" t="s">
         <v>128</v>
       </c>
-      <c r="B24" s="51" t="s">
+      <c r="D24" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="51" t="s">
+      <c r="E24" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="51"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="50" t="s">
+      <c r="F24" s="51"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B25" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="C25" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="51" t="s">
+      <c r="D25" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="C25" s="51" t="s">
+      <c r="E25" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="51"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="50" t="s">
+      <c r="F25" s="51"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B26" s="66"/>
+      <c r="C26" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="51" t="s">
+      <c r="D26" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="C26" s="51" t="s">
+      <c r="E26" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="50"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="50" t="s">
+      <c r="F26" s="50"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" s="66"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="51" t="s">
+      <c r="D27" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="C27" s="51" t="s">
+      <c r="E27" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="D27" s="53" t="s">
+      <c r="F27" s="53" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="27" x14ac:dyDescent="0.15">
-      <c r="A28" s="50" t="s">
+    <row r="28" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A28" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B28" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="C28" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="51" t="s">
+      <c r="D28" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="51" t="s">
+      <c r="E28" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="D28" s="50"/>
-    </row>
-    <row r="29" spans="1:4" ht="27" x14ac:dyDescent="0.15">
-      <c r="A29" s="50" t="s">
+      <c r="F28" s="50"/>
+    </row>
+    <row r="29" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A29" s="66"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="51" t="s">
+      <c r="D29" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="C29" s="51" t="s">
+      <c r="E29" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="53" t="s">
+      <c r="F29" s="53" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="50" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B30" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="C30" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="51" t="s">
+      <c r="D30" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="C30" s="51" t="s">
+      <c r="E30" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="53"/>
-    </row>
-    <row r="31" spans="1:4" ht="81" x14ac:dyDescent="0.15">
-      <c r="A31" s="50" t="s">
+      <c r="F30" s="53"/>
+    </row>
+    <row r="31" spans="1:6" ht="81" x14ac:dyDescent="0.15">
+      <c r="A31" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B31" s="66"/>
+      <c r="C31" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="B31" s="51" t="s">
+      <c r="D31" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="C31" s="51" t="s">
+      <c r="E31" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="D31" s="51" t="s">
+      <c r="F31" s="51" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="27" x14ac:dyDescent="0.15">
-      <c r="A32" s="50" t="s">
+    <row r="32" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A32" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B32" s="66"/>
+      <c r="C32" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="B32" s="51" t="s">
+      <c r="D32" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="C32" s="51" t="s">
+      <c r="E32" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="D32" s="51" t="s">
+      <c r="F32" s="51" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="50" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A33" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B33" s="66"/>
+      <c r="C33" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="B33" s="51" t="s">
+      <c r="D33" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="C33" s="51" t="s">
+      <c r="E33" s="51" t="s">
         <v>155</v>
       </c>
-      <c r="D33" s="53" t="s">
+      <c r="F33" s="53" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="27" x14ac:dyDescent="0.15">
-      <c r="A34" s="50" t="s">
+    <row r="34" spans="1:6" ht="27" x14ac:dyDescent="0.15">
+      <c r="A34" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B34" s="66"/>
+      <c r="C34" s="50" t="s">
         <v>152</v>
       </c>
-      <c r="B34" s="51" t="s">
+      <c r="D34" s="51" t="s">
         <v>154</v>
       </c>
-      <c r="C34" s="51" t="s">
+      <c r="E34" s="51" t="s">
         <v>156</v>
       </c>
-      <c r="D34" s="53" t="s">
+      <c r="F34" s="53" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="52" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A35" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="B35" s="67"/>
+      <c r="C35" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="B35" s="52" t="s">
+      <c r="D35" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="C35" s="57" t="s">
+      <c r="E35" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="D35" s="52"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="52"/>
-      <c r="B36" s="52"/>
-      <c r="C36" s="57"/>
+      <c r="F35" s="52"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A36" s="67"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="52"/>
       <c r="D36" s="52"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="52"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>

</xml_diff>